<commit_message>
thêm phép crossovver và thuật toán mới
</commit_message>
<xml_diff>
--- a/Kết quả thử nghiệm.xlsx
+++ b/Kết quả thử nghiệm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHUC\DPDP\New_DPDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74AF76D-5CEE-4D3A-844F-EFB50D74EAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7EB58-31B5-449F-8ECB-A0891899AE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -590,7 +590,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -612,6 +611,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH960"/>
   <sheetViews>
-    <sheetView topLeftCell="A396" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K420" sqref="K420"/>
+    <sheetView tabSelected="1" topLeftCell="A397" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S446" sqref="S446"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2159,22 +2159,22 @@
     <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="L44" s="51" t="s">
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="L44" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="51"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
@@ -3236,22 +3236,22 @@
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="52" t="s">
+      <c r="A63" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-      <c r="L63" s="52" t="s">
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="L63" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="M63" s="50"/>
-      <c r="N63" s="50"/>
-      <c r="O63" s="50"/>
-      <c r="P63" s="50"/>
-      <c r="Q63" s="50"/>
+      <c r="M63" s="49"/>
+      <c r="N63" s="49"/>
+      <c r="O63" s="49"/>
+      <c r="P63" s="49"/>
+      <c r="Q63" s="49"/>
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
@@ -4220,12 +4220,12 @@
     </row>
     <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="53"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50"/>
-      <c r="F82" s="50"/>
+      <c r="A82" s="52"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="49"/>
+      <c r="F82" s="49"/>
       <c r="L82" s="5"/>
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
@@ -4724,14 +4724,14 @@
     <row r="102" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R104" s="48" t="s">
+      <c r="R104" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="S104" s="48"/>
-      <c r="T104" s="48"/>
-      <c r="U104" s="48"/>
-      <c r="V104" s="48"/>
-      <c r="W104" s="48"/>
+      <c r="S104" s="47"/>
+      <c r="T104" s="47"/>
+      <c r="U104" s="47"/>
+      <c r="V104" s="47"/>
+      <c r="W104" s="47"/>
     </row>
     <row r="105" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="27" t="s">
@@ -8137,22 +8137,22 @@
     <row r="175" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="176" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="177" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="49" t="s">
+      <c r="A177" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="B177" s="50"/>
-      <c r="C177" s="50"/>
-      <c r="D177" s="50"/>
-      <c r="E177" s="50"/>
-      <c r="F177" s="50"/>
-      <c r="R177" s="50" t="s">
+      <c r="B177" s="49"/>
+      <c r="C177" s="49"/>
+      <c r="D177" s="49"/>
+      <c r="E177" s="49"/>
+      <c r="F177" s="49"/>
+      <c r="R177" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="S177" s="50"/>
-      <c r="T177" s="50"/>
-      <c r="U177" s="50"/>
-      <c r="V177" s="50"/>
-      <c r="W177" s="50"/>
+      <c r="S177" s="49"/>
+      <c r="T177" s="49"/>
+      <c r="U177" s="49"/>
+      <c r="V177" s="49"/>
+      <c r="W177" s="49"/>
     </row>
     <row r="178" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27" t="s">
@@ -13483,7 +13483,7 @@
       <c r="A317" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B317" s="28">
+      <c r="B317" s="11">
         <v>134</v>
       </c>
       <c r="C317" s="28">
@@ -13504,7 +13504,7 @@
       <c r="A318" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B318" s="28">
+      <c r="B318" s="11">
         <v>95.74</v>
       </c>
       <c r="C318" s="28">
@@ -13525,7 +13525,7 @@
       <c r="A319" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B319" s="28">
+      <c r="B319" s="11">
         <v>97.44</v>
       </c>
       <c r="C319" s="28">
@@ -13546,7 +13546,7 @@
       <c r="A320" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B320" s="28">
+      <c r="B320" s="11">
         <v>102.7342857</v>
       </c>
       <c r="C320" s="28">
@@ -13567,7 +13567,7 @@
       <c r="A321" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B321" s="17">
+      <c r="B321" s="11">
         <v>4069.6358019999998</v>
       </c>
       <c r="C321" s="28">
@@ -13588,7 +13588,7 @@
       <c r="A322" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B322" s="17">
+      <c r="B322" s="11">
         <v>105</v>
       </c>
       <c r="C322" s="28">
@@ -13609,7 +13609,7 @@
       <c r="A323" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B323" s="28">
+      <c r="B323" s="11">
         <v>10338.10578</v>
       </c>
       <c r="C323" s="28">
@@ -13630,7 +13630,7 @@
       <c r="A324" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B324" s="28">
+      <c r="B324" s="11">
         <v>68.8</v>
       </c>
       <c r="C324" s="28">
@@ -13651,7 +13651,7 @@
       <c r="A325" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B325" s="28">
+      <c r="B325" s="11">
         <v>3307.1417280000001</v>
       </c>
       <c r="C325" s="28">
@@ -13672,7 +13672,7 @@
       <c r="A326" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B326" s="28">
+      <c r="B326" s="11">
         <v>194000</v>
       </c>
       <c r="C326" s="28">
@@ -13714,7 +13714,7 @@
       <c r="A327" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B327" s="28">
+      <c r="B327" s="11">
         <v>910.73827159999996</v>
       </c>
       <c r="C327" s="28">
@@ -13765,7 +13765,7 @@
       <c r="A328" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B328" s="28">
+      <c r="B328" s="11">
         <v>14974.64444</v>
       </c>
       <c r="C328" s="28">
@@ -13795,7 +13795,7 @@
       <c r="A329" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B329" s="28">
+      <c r="B329" s="11">
         <v>3359.6609880000001</v>
       </c>
       <c r="C329" s="28">
@@ -13837,7 +13837,7 @@
       <c r="A330" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B330" s="28">
+      <c r="B330" s="11">
         <v>18163.26296</v>
       </c>
       <c r="C330" s="28">
@@ -13876,7 +13876,7 @@
       <c r="A331" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B331" s="28">
+      <c r="B331" s="11">
         <v>32301.335800000001</v>
       </c>
       <c r="C331" s="28">
@@ -13918,7 +13918,7 @@
       <c r="A332" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B332" s="28">
+      <c r="B332" s="11">
         <v>51313.376790000002</v>
       </c>
       <c r="C332" s="28">
@@ -13963,7 +13963,7 @@
       <c r="A333" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B333" s="38">
+      <c r="B333" s="11">
         <v>84.667500000000004</v>
       </c>
       <c r="C333" s="39">
@@ -14014,7 +14014,7 @@
       <c r="A334" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B334" s="38">
+      <c r="B334" s="11">
         <v>1627.9475</v>
       </c>
       <c r="C334" s="39">
@@ -14065,7 +14065,7 @@
       <c r="A335" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B335" s="38">
+      <c r="B335" s="11">
         <v>1260.0333889999999</v>
       </c>
       <c r="C335" s="39">
@@ -14116,7 +14116,7 @@
       <c r="A336" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B336" s="38">
+      <c r="B336" s="11">
         <v>7055.9061670000001</v>
       </c>
       <c r="C336" s="39">
@@ -14167,7 +14167,7 @@
       <c r="A337" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B337" s="38">
+      <c r="B337" s="11">
         <v>2396.498556</v>
       </c>
       <c r="C337" s="39">
@@ -14188,7 +14188,7 @@
       <c r="A338" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B338" s="38">
+      <c r="B338" s="11">
         <v>3322.8712220000002</v>
       </c>
       <c r="C338" s="39">
@@ -14209,7 +14209,7 @@
       <c r="A339" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B339" s="38">
+      <c r="B339" s="11">
         <v>106.435</v>
       </c>
       <c r="C339" s="39">
@@ -14230,7 +14230,7 @@
       <c r="A340" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B340" s="38">
+      <c r="B340" s="11">
         <v>92.355999999999995</v>
       </c>
       <c r="C340" s="39">
@@ -14251,7 +14251,7 @@
       <c r="A341" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B341" s="38">
+      <c r="B341" s="11">
         <v>10300</v>
       </c>
       <c r="C341" s="39">
@@ -14272,8 +14272,8 @@
       <c r="A342" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B342" s="40">
-        <v>34883</v>
+      <c r="B342" s="11">
+        <v>10659.381670000001</v>
       </c>
       <c r="C342" s="39">
         <v>275000</v>
@@ -14293,7 +14293,7 @@
       <c r="A343" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B343" s="40">
+      <c r="B343" s="11">
         <v>134</v>
       </c>
       <c r="C343" s="39">
@@ -14314,8 +14314,8 @@
       <c r="A344" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B344" s="40">
-        <v>7100</v>
+      <c r="B344" s="11">
+        <v>7137.7017219999998</v>
       </c>
       <c r="C344" s="39">
         <v>9440</v>
@@ -14335,8 +14335,8 @@
       <c r="A345" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B345" s="40">
-        <v>6400</v>
+      <c r="B345" s="11">
+        <v>9044.8115560000006</v>
       </c>
       <c r="C345" s="39">
         <v>163000</v>
@@ -14356,7 +14356,7 @@
       <c r="A346" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B346" s="40">
+      <c r="B346" s="11">
         <v>119</v>
       </c>
       <c r="C346" s="39">
@@ -14377,7 +14377,7 @@
       <c r="A347" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B347" s="40">
+      <c r="B347" s="11">
         <v>22600</v>
       </c>
       <c r="C347" s="39">
@@ -14398,7 +14398,7 @@
       <c r="A348" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B348" s="40">
+      <c r="B348" s="11">
         <v>7670</v>
       </c>
       <c r="C348" s="39">
@@ -14419,8 +14419,8 @@
       <c r="A349" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B349" s="40">
-        <v>1590</v>
+      <c r="B349" s="11">
+        <v>3667.1041329999998</v>
       </c>
       <c r="C349" s="39">
         <v>7030</v>
@@ -14465,7 +14465,7 @@
         <v>40</v>
       </c>
       <c r="B350" s="11">
-        <v>10500</v>
+        <v>11149.197980000001</v>
       </c>
       <c r="C350" s="11">
         <v>10500</v>
@@ -14507,7 +14507,7 @@
         <v>41</v>
       </c>
       <c r="B351" s="11">
-        <v>3440</v>
+        <v>3475.4503169999998</v>
       </c>
       <c r="C351" s="11">
         <v>15800</v>
@@ -14646,7 +14646,7 @@
         <v>44</v>
       </c>
       <c r="B354" s="11">
-        <v>15000</v>
+        <v>16497.968720000001</v>
       </c>
       <c r="C354" s="11">
         <v>30100</v>
@@ -14692,7 +14692,7 @@
         <v>45</v>
       </c>
       <c r="B355" s="11">
-        <v>14900</v>
+        <v>20275.580959999999</v>
       </c>
       <c r="C355" s="11">
         <v>22300</v>
@@ -14738,7 +14738,7 @@
         <v>46</v>
       </c>
       <c r="B356" s="11">
-        <v>10200</v>
+        <v>13444.76433</v>
       </c>
       <c r="C356" s="11">
         <v>24300</v>
@@ -14787,7 +14787,7 @@
         <v>47</v>
       </c>
       <c r="B357" s="11">
-        <v>29300</v>
+        <v>36129.024490000003</v>
       </c>
       <c r="C357" s="11">
         <v>124000</v>
@@ -14863,7 +14863,7 @@
         <v>51</v>
       </c>
       <c r="B361" s="11">
-        <v>36300</v>
+        <v>47357.535309999999</v>
       </c>
       <c r="C361" s="11">
         <v>181000</v>
@@ -14920,7 +14920,7 @@
         <v>54</v>
       </c>
       <c r="B364" s="11">
-        <v>15200</v>
+        <v>18153.645619999999</v>
       </c>
       <c r="C364" s="11">
         <v>124000</v>
@@ -14977,7 +14977,7 @@
         <v>57</v>
       </c>
       <c r="B367" s="11">
-        <v>74400</v>
+        <v>192540.7703</v>
       </c>
       <c r="C367" s="11">
         <v>515000</v>
@@ -15044,7 +15044,7 @@
         <v>61</v>
       </c>
       <c r="B371" s="11">
-        <v>323000</v>
+        <v>519003.67749999999</v>
       </c>
       <c r="C371" s="11">
         <v>730000</v>
@@ -15076,7 +15076,7 @@
         <v>63</v>
       </c>
       <c r="B373" s="11">
-        <v>10400000</v>
+        <v>10686649.529999999</v>
       </c>
       <c r="C373" s="11">
         <v>22400000</v>
@@ -15092,7 +15092,7 @@
         <v>64</v>
       </c>
       <c r="B374" s="11">
-        <v>10000000</v>
+        <v>10283491.050000001</v>
       </c>
       <c r="C374" s="11">
         <v>13200000</v>
@@ -15108,7 +15108,7 @@
         <v>65</v>
       </c>
       <c r="B375" s="11">
-        <v>7770000</v>
+        <v>9319943.2860000003</v>
       </c>
       <c r="C375" s="11">
         <v>12400000</v>
@@ -15140,7 +15140,7 @@
         <v>67</v>
       </c>
       <c r="B377" s="11">
-        <v>6030000</v>
+        <v>6331051.2470000004</v>
       </c>
       <c r="C377" s="11">
         <v>9100000</v>
@@ -15203,7 +15203,7 @@
     <row r="382" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="383" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="384" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="27" t="s">
         <v>71</v>
       </c>
@@ -15223,11 +15223,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B386" s="28">
+      <c r="B386" s="11">
         <v>134</v>
       </c>
       <c r="C386" s="28">
@@ -15273,12 +15273,20 @@
       <c r="P386">
         <v>117.41999999999901</v>
       </c>
-    </row>
-    <row r="387" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R386" s="11">
+        <f xml:space="preserve"> (F386 - B386)/B386</f>
+        <v>-2.7074626865673232E-2</v>
+      </c>
+      <c r="S386" s="19">
+        <f xml:space="preserve"> R386 * 100  * -1</f>
+        <v>2.707462686567323</v>
+      </c>
+    </row>
+    <row r="387" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B387" s="28">
+      <c r="B387" s="11">
         <v>95.74</v>
       </c>
       <c r="C387" s="28">
@@ -15324,12 +15332,20 @@
       <c r="P387">
         <v>89.2</v>
       </c>
-    </row>
-    <row r="388" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R387" s="11">
+        <f t="shared" ref="R387:R442" si="19" xml:space="preserve"> (F387 - B387)/B387</f>
+        <v>-5.8679757677042088E-2</v>
+      </c>
+      <c r="S387" s="19">
+        <f t="shared" ref="S387:S437" si="20" xml:space="preserve"> R387 * 100  * -1</f>
+        <v>5.867975767704209</v>
+      </c>
+    </row>
+    <row r="388" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B388" s="28">
+      <c r="B388" s="11">
         <v>97.44</v>
       </c>
       <c r="C388" s="28">
@@ -15375,12 +15391,20 @@
       <c r="P388">
         <v>102.42</v>
       </c>
-    </row>
-    <row r="389" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R388" s="11">
+        <f t="shared" si="19"/>
+        <v>4.8296387520524314E-2</v>
+      </c>
+      <c r="S388" s="19">
+        <f t="shared" si="20"/>
+        <v>-4.8296387520524311</v>
+      </c>
+    </row>
+    <row r="389" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B389" s="28">
+      <c r="B389" s="11">
         <v>102.7342857</v>
       </c>
       <c r="C389" s="28">
@@ -15426,12 +15450,20 @@
       <c r="P389">
         <v>92.14</v>
       </c>
-    </row>
-    <row r="390" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R389" s="11">
+        <f t="shared" si="19"/>
+        <v>-9.6348416038094048E-2</v>
+      </c>
+      <c r="S389" s="19">
+        <f t="shared" si="20"/>
+        <v>9.634841603809404</v>
+      </c>
+    </row>
+    <row r="390" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B390" s="28">
+      <c r="B390" s="11">
         <v>4069.6358019999998</v>
       </c>
       <c r="C390" s="28">
@@ -15477,12 +15509,20 @@
       <c r="P390">
         <v>5445.26</v>
       </c>
-    </row>
-    <row r="391" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R390" s="11">
+        <f t="shared" si="19"/>
+        <v>0.3380848471314884</v>
+      </c>
+      <c r="S390" s="19">
+        <f t="shared" si="20"/>
+        <v>-33.808484713148843</v>
+      </c>
+    </row>
+    <row r="391" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B391" s="28">
+      <c r="B391" s="11">
         <v>105</v>
       </c>
       <c r="C391" s="28">
@@ -15528,12 +15568,20 @@
       <c r="P391">
         <v>115.46</v>
       </c>
-    </row>
-    <row r="392" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R391" s="11">
+        <f t="shared" si="19"/>
+        <v>9.8723809523809658E-2</v>
+      </c>
+      <c r="S391" s="19">
+        <f t="shared" si="20"/>
+        <v>-9.8723809523809649</v>
+      </c>
+    </row>
+    <row r="392" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B392" s="28">
+      <c r="B392" s="11">
         <v>10338.10578</v>
       </c>
       <c r="C392" s="28">
@@ -15579,12 +15627,20 @@
       <c r="P392">
         <v>3750.5266666666598</v>
       </c>
-    </row>
-    <row r="393" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R392" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.61874982220711361</v>
+      </c>
+      <c r="S392" s="19">
+        <f t="shared" si="20"/>
+        <v>61.87498222071136</v>
+      </c>
+    </row>
+    <row r="393" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B393" s="28">
+      <c r="B393" s="11">
         <v>68.8</v>
       </c>
       <c r="C393" s="28">
@@ -15597,7 +15653,7 @@
         <v>95</v>
       </c>
       <c r="F393" s="19">
-        <f t="shared" ref="F393:F397" si="19" xml:space="preserve"> AVERAGE(G393:P393)</f>
+        <f t="shared" ref="F393:F397" si="21" xml:space="preserve"> AVERAGE(G393:P393)</f>
         <v>65.895999999999958</v>
       </c>
       <c r="G393">
@@ -15630,12 +15686,20 @@
       <c r="P393">
         <v>68.739999999999995</v>
       </c>
-    </row>
-    <row r="394" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R393" s="11">
+        <f t="shared" si="19"/>
+        <v>-4.2209302325581961E-2</v>
+      </c>
+      <c r="S393" s="19">
+        <f t="shared" si="20"/>
+        <v>4.2209302325581959</v>
+      </c>
+    </row>
+    <row r="394" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B394" s="28">
+      <c r="B394" s="11">
         <v>3307.1417280000001</v>
       </c>
       <c r="C394" s="28">
@@ -15648,7 +15712,7 @@
         <v>5000</v>
       </c>
       <c r="F394" s="19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>161.41399999999993</v>
       </c>
       <c r="G394">
@@ -15681,12 +15745,20 @@
       <c r="P394">
         <v>160.47999999999999</v>
       </c>
-    </row>
-    <row r="395" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R394" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.95119229435092423</v>
+      </c>
+      <c r="S394" s="19">
+        <f t="shared" si="20"/>
+        <v>95.119229435092421</v>
+      </c>
+    </row>
+    <row r="395" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B395" s="28">
+      <c r="B395" s="11">
         <v>194000</v>
       </c>
       <c r="C395" s="28">
@@ -15699,7 +15771,7 @@
         <v>183000</v>
       </c>
       <c r="F395" s="19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>142430.18866666619</v>
       </c>
       <c r="G395">
@@ -15732,12 +15804,20 @@
       <c r="P395">
         <v>133916.80444444399</v>
       </c>
-    </row>
-    <row r="396" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R395" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.26582376975945265</v>
+      </c>
+      <c r="S395" s="19">
+        <f t="shared" si="20"/>
+        <v>26.582376975945266</v>
+      </c>
+    </row>
+    <row r="396" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B396" s="28">
+      <c r="B396" s="11">
         <v>910.73827159999996</v>
       </c>
       <c r="C396" s="28">
@@ -15750,7 +15830,7 @@
         <v>500</v>
       </c>
       <c r="F396" s="19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>166.702</v>
       </c>
       <c r="G396">
@@ -15783,12 +15863,20 @@
       <c r="P396">
         <v>164.14</v>
       </c>
-    </row>
-    <row r="397" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R396" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.81695948748575686</v>
+      </c>
+      <c r="S396" s="19">
+        <f t="shared" si="20"/>
+        <v>81.695948748575688</v>
+      </c>
+    </row>
+    <row r="397" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B397" s="28">
+      <c r="B397" s="11">
         <v>14974.64444</v>
       </c>
       <c r="C397" s="28">
@@ -15801,7 +15889,7 @@
         <v>79000</v>
       </c>
       <c r="F397" s="19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>23826.100444444404</v>
       </c>
       <c r="G397">
@@ -15834,12 +15922,20 @@
       <c r="P397">
         <v>6693.4022222222202</v>
       </c>
-    </row>
-    <row r="398" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R397" s="11">
+        <f t="shared" si="19"/>
+        <v>0.591096238706046</v>
+      </c>
+      <c r="S397" s="19">
+        <f t="shared" si="20"/>
+        <v>-59.109623870604601</v>
+      </c>
+    </row>
+    <row r="398" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B398" s="28">
+      <c r="B398" s="11">
         <v>3359.6609880000001</v>
       </c>
       <c r="C398" s="28">
@@ -15885,12 +15981,20 @@
       <c r="P398">
         <v>174.18</v>
       </c>
-    </row>
-    <row r="399" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R398" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.7805387036998408</v>
+      </c>
+      <c r="S398" s="19">
+        <f t="shared" si="20"/>
+        <v>78.053870369984082</v>
+      </c>
+    </row>
+    <row r="399" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B399" s="28">
+      <c r="B399" s="11">
         <v>18163.26296</v>
       </c>
       <c r="C399" s="28">
@@ -15903,7 +16007,7 @@
         <v>6500</v>
       </c>
       <c r="F399" s="19">
-        <f t="shared" ref="F399:F414" si="20" xml:space="preserve"> AVERAGE(G399:P399)</f>
+        <f t="shared" ref="F399:F414" si="22" xml:space="preserve"> AVERAGE(G399:P399)</f>
         <v>655.91456790123334</v>
       </c>
       <c r="G399">
@@ -15933,12 +16037,20 @@
       <c r="O399">
         <v>164.88</v>
       </c>
-    </row>
-    <row r="400" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R399" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.96388784496784974</v>
+      </c>
+      <c r="S399" s="19">
+        <f t="shared" si="20"/>
+        <v>96.388784496784979</v>
+      </c>
+    </row>
+    <row r="400" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B400" s="28">
+      <c r="B400" s="11">
         <v>32301.335800000001</v>
       </c>
       <c r="C400" s="28">
@@ -15951,7 +16063,7 @@
         <v>47000</v>
       </c>
       <c r="F400" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>28053.94599999996</v>
       </c>
       <c r="G400">
@@ -15984,12 +16096,20 @@
       <c r="P400">
         <v>22814.426666666601</v>
       </c>
-    </row>
-    <row r="401" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R400" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.13149269820599929</v>
+      </c>
+      <c r="S400" s="19">
+        <f t="shared" si="20"/>
+        <v>13.14926982059993</v>
+      </c>
+    </row>
+    <row r="401" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B401" s="28">
+      <c r="B401" s="11">
         <v>51313.376790000002</v>
       </c>
       <c r="C401" s="28">
@@ -16002,7 +16122,7 @@
         <v>49000</v>
       </c>
       <c r="F401" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>19360.027111111056</v>
       </c>
       <c r="G401">
@@ -16035,25 +16155,33 @@
       <c r="P401">
         <v>17476.3644444444</v>
       </c>
-    </row>
-    <row r="402" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R401" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.62270993798864638</v>
+      </c>
+      <c r="S401" s="19">
+        <f t="shared" si="20"/>
+        <v>62.270993798864637</v>
+      </c>
+    </row>
+    <row r="402" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B402" s="44">
+      <c r="B402" s="11">
         <v>84.667500000000004</v>
       </c>
-      <c r="C402" s="45">
+      <c r="C402" s="44">
         <v>96</v>
       </c>
-      <c r="D402" s="46">
+      <c r="D402" s="45">
         <v>411</v>
       </c>
-      <c r="E402" s="46">
+      <c r="E402" s="45">
         <v>92</v>
       </c>
       <c r="F402" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>80.656499999999994</v>
       </c>
       <c r="G402">
@@ -16086,25 +16214,33 @@
       <c r="P402">
         <v>81.995000000000005</v>
       </c>
-    </row>
-    <row r="403" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R402" s="11">
+        <f t="shared" si="19"/>
+        <v>-4.737354947293837E-2</v>
+      </c>
+      <c r="S402" s="19">
+        <f t="shared" si="20"/>
+        <v>4.737354947293837</v>
+      </c>
+    </row>
+    <row r="403" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B403" s="44">
+      <c r="B403" s="11">
         <v>1627.9475</v>
       </c>
-      <c r="C403" s="45">
+      <c r="C403" s="44">
         <v>112</v>
       </c>
-      <c r="D403" s="46">
+      <c r="D403" s="45">
         <v>8560</v>
       </c>
-      <c r="E403" s="46">
+      <c r="E403" s="45">
         <v>96.42</v>
       </c>
       <c r="F403" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>85.755999999999986</v>
       </c>
       <c r="G403">
@@ -16137,25 +16273,33 @@
       <c r="P403">
         <v>86.49</v>
       </c>
-    </row>
-    <row r="404" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R403" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.94732262557607039</v>
+      </c>
+      <c r="S403" s="19">
+        <f t="shared" si="20"/>
+        <v>94.732262557607044</v>
+      </c>
+    </row>
+    <row r="404" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="B404" s="44">
+      <c r="B404" s="11">
         <v>1260.0333889999999</v>
       </c>
-      <c r="C404" s="45">
+      <c r="C404" s="44">
         <v>478</v>
       </c>
-      <c r="D404" s="46">
+      <c r="D404" s="45">
         <v>4150</v>
       </c>
-      <c r="E404" s="46">
+      <c r="E404" s="45">
         <v>120</v>
       </c>
       <c r="F404" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>108.50283333333309</v>
       </c>
       <c r="G404">
@@ -16188,25 +16332,33 @@
       <c r="P404">
         <v>109.675</v>
       </c>
-    </row>
-    <row r="405" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R404" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.91388892208686301</v>
+      </c>
+      <c r="S404" s="19">
+        <f t="shared" si="20"/>
+        <v>91.3888922086863</v>
+      </c>
+    </row>
+    <row r="405" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B405" s="44">
+      <c r="B405" s="11">
         <v>7055.9061670000001</v>
       </c>
-      <c r="C405" s="45">
+      <c r="C405" s="44">
         <v>3980</v>
       </c>
-      <c r="D405" s="46">
+      <c r="D405" s="45">
         <v>16200</v>
       </c>
-      <c r="E405" s="46">
+      <c r="E405" s="45">
         <v>100</v>
       </c>
       <c r="F405" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3385.2657777777722</v>
       </c>
       <c r="G405">
@@ -16239,25 +16391,33 @@
       <c r="P405">
         <v>3297.2877777777699</v>
       </c>
-    </row>
-    <row r="406" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R405" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.52022239275085136</v>
+      </c>
+      <c r="S405" s="19">
+        <f t="shared" si="20"/>
+        <v>52.022239275085134</v>
+      </c>
+    </row>
+    <row r="406" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A406" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B406" s="44">
+      <c r="B406" s="11">
         <v>2396.498556</v>
       </c>
-      <c r="C406" s="45">
+      <c r="C406" s="44">
         <v>2340</v>
       </c>
-      <c r="D406" s="46">
+      <c r="D406" s="45">
         <v>18500</v>
       </c>
-      <c r="E406" s="46">
+      <c r="E406" s="45">
         <v>110</v>
       </c>
       <c r="F406" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>104.54357142857144</v>
       </c>
       <c r="G406">
@@ -16281,25 +16441,33 @@
       <c r="M406">
         <v>103.47</v>
       </c>
-    </row>
-    <row r="407" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R406" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.95637653477118501</v>
+      </c>
+      <c r="S406" s="19">
+        <f t="shared" si="20"/>
+        <v>95.637653477118505</v>
+      </c>
+    </row>
+    <row r="407" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A407" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B407" s="44">
+      <c r="B407" s="11">
         <v>3322.8712220000002</v>
       </c>
-      <c r="C407" s="45">
+      <c r="C407" s="44">
         <v>3320</v>
       </c>
-      <c r="D407" s="46">
+      <c r="D407" s="45">
         <v>21100</v>
       </c>
-      <c r="E407" s="46">
+      <c r="E407" s="45">
         <v>96</v>
       </c>
       <c r="F407" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1641.851111111109</v>
       </c>
       <c r="G407">
@@ -16329,25 +16497,33 @@
       <c r="O407">
         <v>1640.6172222222201</v>
       </c>
-    </row>
-    <row r="408" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R407" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.50589384859672759</v>
+      </c>
+      <c r="S407" s="19">
+        <f t="shared" si="20"/>
+        <v>50.589384859672762</v>
+      </c>
+    </row>
+    <row r="408" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A408" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B408" s="44">
+      <c r="B408" s="11">
         <v>106.435</v>
       </c>
-      <c r="C408" s="45">
+      <c r="C408" s="44">
         <v>6870</v>
       </c>
-      <c r="D408" s="46">
+      <c r="D408" s="45">
         <v>809</v>
       </c>
-      <c r="E408" s="46">
+      <c r="E408" s="45">
         <v>105</v>
       </c>
       <c r="F408" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>104.70777777777744</v>
       </c>
       <c r="G408">
@@ -16377,25 +16553,33 @@
       <c r="O408">
         <v>104.509999999999</v>
       </c>
-    </row>
-    <row r="409" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R408" s="11">
+        <f t="shared" si="19"/>
+        <v>-1.6227953419669892E-2</v>
+      </c>
+      <c r="S408" s="19">
+        <f t="shared" si="20"/>
+        <v>1.6227953419669892</v>
+      </c>
+    </row>
+    <row r="409" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A409" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B409" s="44">
+      <c r="B409" s="11">
         <v>92.355999999999995</v>
       </c>
-      <c r="C409" s="45">
+      <c r="C409" s="44">
         <v>1290</v>
       </c>
-      <c r="D409" s="46">
+      <c r="D409" s="45">
         <v>2000</v>
       </c>
-      <c r="E409" s="46">
+      <c r="E409" s="45">
         <v>94.4</v>
       </c>
       <c r="F409" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>89.923999999999978</v>
       </c>
       <c r="G409">
@@ -16428,25 +16612,33 @@
       <c r="P409">
         <v>88.864999999999995</v>
       </c>
-    </row>
-    <row r="410" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R409" s="11">
+        <f t="shared" si="19"/>
+        <v>-2.6332885789770197E-2</v>
+      </c>
+      <c r="S409" s="19">
+        <f t="shared" si="20"/>
+        <v>2.63328857897702</v>
+      </c>
+    </row>
+    <row r="410" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B410" s="44">
+      <c r="B410" s="11">
         <v>10300</v>
       </c>
-      <c r="C410" s="45">
+      <c r="C410" s="44">
         <v>92400</v>
       </c>
-      <c r="D410" s="46">
+      <c r="D410" s="45">
         <v>21500</v>
       </c>
-      <c r="E410" s="46">
+      <c r="E410" s="45">
         <v>6428</v>
       </c>
       <c r="F410" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8691.0338333333257</v>
       </c>
       <c r="G410">
@@ -16479,25 +16671,33 @@
       <c r="P410">
         <v>7451.8594444444398</v>
       </c>
-    </row>
-    <row r="411" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R410" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.15621030744336645</v>
+      </c>
+      <c r="S410" s="19">
+        <f t="shared" si="20"/>
+        <v>15.621030744336645</v>
+      </c>
+    </row>
+    <row r="411" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A411" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B411" s="46">
-        <v>34883</v>
-      </c>
-      <c r="C411" s="45">
+      <c r="B411" s="11">
+        <v>10659.381670000001</v>
+      </c>
+      <c r="C411" s="44">
         <v>275000</v>
       </c>
-      <c r="D411" s="46">
+      <c r="D411" s="45">
         <v>54000</v>
       </c>
-      <c r="E411" s="46">
+      <c r="E411" s="45">
         <v>9285</v>
       </c>
       <c r="F411" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>7385.2874074074025</v>
       </c>
       <c r="G411">
@@ -16527,25 +16727,33 @@
       <c r="O411">
         <v>3980.29</v>
       </c>
-    </row>
-    <row r="412" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R411" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.30715611505002033</v>
+      </c>
+      <c r="S411" s="19">
+        <f t="shared" si="20"/>
+        <v>30.715611505002034</v>
+      </c>
+    </row>
+    <row r="412" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B412" s="46">
+      <c r="B412" s="11">
         <v>134</v>
       </c>
-      <c r="C412" s="45">
+      <c r="C412" s="44">
         <v>18400</v>
       </c>
-      <c r="D412" s="46">
+      <c r="D412" s="45">
         <v>18800</v>
       </c>
-      <c r="E412" s="46">
+      <c r="E412" s="45">
         <v>130</v>
       </c>
       <c r="F412" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>127.37444444444444</v>
       </c>
       <c r="G412">
@@ -16575,25 +16783,33 @@
       <c r="O412">
         <v>126.82</v>
       </c>
-    </row>
-    <row r="413" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R412" s="11">
+        <f t="shared" si="19"/>
+        <v>-4.9444444444444513E-2</v>
+      </c>
+      <c r="S412" s="19">
+        <f t="shared" si="20"/>
+        <v>4.9444444444444517</v>
+      </c>
+    </row>
+    <row r="413" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A413" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B413" s="46">
-        <v>7100</v>
-      </c>
-      <c r="C413" s="45">
+      <c r="B413" s="11">
+        <v>7137.7017219999998</v>
+      </c>
+      <c r="C413" s="44">
         <v>9440</v>
       </c>
-      <c r="D413" s="46">
+      <c r="D413" s="45">
         <v>14900</v>
       </c>
-      <c r="E413" s="46">
+      <c r="E413" s="45">
         <v>302</v>
       </c>
       <c r="F413" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>7119.334388888883</v>
       </c>
       <c r="G413">
@@ -16626,25 +16842,33 @@
       <c r="P413">
         <v>7138.5372222222204</v>
       </c>
-    </row>
-    <row r="414" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R413" s="11">
+        <f t="shared" si="19"/>
+        <v>-2.5732839261837608E-3</v>
+      </c>
+      <c r="S413" s="19">
+        <f t="shared" si="20"/>
+        <v>0.25732839261837609</v>
+      </c>
+    </row>
+    <row r="414" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A414" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B414" s="46">
-        <v>6400</v>
-      </c>
-      <c r="C414" s="45">
+      <c r="B414" s="11">
+        <v>9044.8115560000006</v>
+      </c>
+      <c r="C414" s="44">
         <v>163000</v>
       </c>
-      <c r="D414" s="46">
+      <c r="D414" s="45">
         <v>42400</v>
       </c>
-      <c r="E414" s="46">
+      <c r="E414" s="45">
         <v>925</v>
       </c>
       <c r="F414" s="19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>6311.7867901234513</v>
       </c>
       <c r="G414">
@@ -16674,21 +16898,29 @@
       <c r="O414">
         <v>6098.7288888888797</v>
       </c>
-    </row>
-    <row r="415" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R414" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.30216492062386413</v>
+      </c>
+      <c r="S414" s="19">
+        <f t="shared" si="20"/>
+        <v>30.216492062386415</v>
+      </c>
+    </row>
+    <row r="415" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A415" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B415" s="46">
+      <c r="B415" s="11">
         <v>119</v>
       </c>
-      <c r="C415" s="45">
+      <c r="C415" s="44">
         <v>74000</v>
       </c>
-      <c r="D415" s="46">
+      <c r="D415" s="45">
         <v>21100</v>
       </c>
-      <c r="E415" s="46">
+      <c r="E415" s="45">
         <v>450</v>
       </c>
       <c r="F415" s="19">
@@ -16725,25 +16957,33 @@
       <c r="P415">
         <v>124.36499999999999</v>
       </c>
-    </row>
-    <row r="416" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R415" s="11">
+        <f t="shared" si="19"/>
+        <v>2.9794584500463957E-2</v>
+      </c>
+      <c r="S415" s="19">
+        <f t="shared" si="20"/>
+        <v>-2.9794584500463959</v>
+      </c>
+    </row>
+    <row r="416" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B416" s="46">
+      <c r="B416" s="11">
         <v>22600</v>
       </c>
-      <c r="C416" s="45">
+      <c r="C416" s="44">
         <v>147000</v>
       </c>
-      <c r="D416" s="46">
+      <c r="D416" s="45">
         <v>23300</v>
       </c>
-      <c r="E416" s="46">
+      <c r="E416" s="45">
         <v>22000</v>
       </c>
       <c r="F416" s="19">
-        <f t="shared" ref="F416:F436" si="21" xml:space="preserve"> AVERAGE(G416:P416)</f>
+        <f t="shared" ref="F416:F436" si="23" xml:space="preserve"> AVERAGE(G416:P416)</f>
         <v>16303.368541666627</v>
       </c>
       <c r="G416">
@@ -16770,25 +17010,33 @@
       <c r="N416">
         <v>15879.9783333333</v>
       </c>
-    </row>
-    <row r="417" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R416" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.27861201143068026</v>
+      </c>
+      <c r="S416" s="19">
+        <f t="shared" si="20"/>
+        <v>27.861201143068026</v>
+      </c>
+    </row>
+    <row r="417" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A417" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B417" s="46">
+      <c r="B417" s="11">
         <v>7670</v>
       </c>
-      <c r="C417" s="45">
+      <c r="C417" s="44">
         <v>60400</v>
       </c>
-      <c r="D417" s="46">
+      <c r="D417" s="45">
         <v>19600</v>
       </c>
-      <c r="E417" s="46">
+      <c r="E417" s="45">
         <v>200</v>
       </c>
       <c r="F417" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>7489.0393888888839</v>
       </c>
       <c r="G417">
@@ -16821,25 +17069,33 @@
       <c r="P417">
         <v>7531.5038888888803</v>
       </c>
-    </row>
-    <row r="418" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R417" s="11">
+        <f t="shared" si="19"/>
+        <v>-2.3593300014487107E-2</v>
+      </c>
+      <c r="S417" s="19">
+        <f t="shared" si="20"/>
+        <v>2.3593300014487109</v>
+      </c>
+    </row>
+    <row r="418" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A418" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B418" s="46">
-        <v>1590</v>
-      </c>
-      <c r="C418" s="45">
+      <c r="B418" s="11">
+        <v>3667.1041329999998</v>
+      </c>
+      <c r="C418" s="44">
         <v>7030</v>
       </c>
-      <c r="D418" s="46">
+      <c r="D418" s="45">
         <v>95000</v>
       </c>
-      <c r="E418" s="47">
+      <c r="E418" s="46">
         <v>1300</v>
       </c>
       <c r="F418" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>77.451499999999967</v>
       </c>
       <c r="H418">
@@ -16866,25 +17122,33 @@
       <c r="P418">
         <v>77.305999999999997</v>
       </c>
-    </row>
-    <row r="419" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R418" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.97887938351599568</v>
+      </c>
+      <c r="S418" s="19">
+        <f t="shared" si="20"/>
+        <v>97.887938351599573</v>
+      </c>
+    </row>
+    <row r="419" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A419" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B419" s="46">
+      <c r="B419" s="11">
+        <v>11149.197980000001</v>
+      </c>
+      <c r="C419" s="45">
         <v>10500</v>
       </c>
-      <c r="C419" s="46">
-        <v>10500</v>
-      </c>
-      <c r="D419" s="46">
+      <c r="D419" s="45">
         <v>54400</v>
       </c>
-      <c r="E419" s="46">
+      <c r="E419" s="45">
         <v>100</v>
       </c>
       <c r="F419" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>9384.5324444444268</v>
       </c>
       <c r="G419">
@@ -16902,25 +17166,33 @@
       <c r="K419">
         <v>6893.8571111111096</v>
       </c>
-    </row>
-    <row r="420" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R419" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.15827735221144346</v>
+      </c>
+      <c r="S419" s="19">
+        <f t="shared" si="20"/>
+        <v>15.827735221144346</v>
+      </c>
+    </row>
+    <row r="420" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A420" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B420" s="46">
-        <v>3440</v>
-      </c>
-      <c r="C420" s="46">
+      <c r="B420" s="11">
+        <v>3475.4503169999998</v>
+      </c>
+      <c r="C420" s="45">
         <v>15800</v>
       </c>
-      <c r="D420" s="46">
+      <c r="D420" s="45">
         <v>104000</v>
       </c>
-      <c r="E420" s="46">
+      <c r="E420" s="45">
         <v>100</v>
       </c>
       <c r="F420" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2661.466499999995</v>
       </c>
       <c r="G420">
@@ -16935,25 +17207,33 @@
       <c r="J420">
         <v>3442.4795555555502</v>
       </c>
-    </row>
-    <row r="421" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R420" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.23420959667253527</v>
+      </c>
+      <c r="S420" s="19">
+        <f t="shared" si="20"/>
+        <v>23.420959667253527</v>
+      </c>
+    </row>
+    <row r="421" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A421" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B421" s="46">
+      <c r="B421" s="11">
         <v>17500</v>
       </c>
-      <c r="C421" s="46">
+      <c r="C421" s="45">
         <v>23200</v>
       </c>
-      <c r="D421" s="46">
+      <c r="D421" s="45">
         <v>113000</v>
       </c>
-      <c r="E421" s="46">
+      <c r="E421" s="45">
         <v>900</v>
       </c>
       <c r="F421" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>16790.943283950553</v>
       </c>
       <c r="G421">
@@ -16983,23 +17263,31 @@
       <c r="O421">
         <v>13459.8686666666</v>
       </c>
-    </row>
-    <row r="422" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R421" s="11">
+        <f t="shared" si="19"/>
+        <v>-4.0517526631396947E-2</v>
+      </c>
+      <c r="S421" s="19">
+        <f t="shared" si="20"/>
+        <v>4.0517526631396947</v>
+      </c>
+    </row>
+    <row r="422" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A422" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B422" s="46">
+      <c r="B422" s="11">
         <v>11200</v>
       </c>
-      <c r="C422" s="46">
+      <c r="C422" s="45">
         <v>5140</v>
       </c>
-      <c r="D422" s="46">
+      <c r="D422" s="45">
         <v>95700</v>
       </c>
-      <c r="E422" s="46"/>
+      <c r="E422" s="45"/>
       <c r="F422" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>11610.224172839464</v>
       </c>
       <c r="G422">
@@ -17029,23 +17317,31 @@
       <c r="O422">
         <v>12367.747555555499</v>
       </c>
-    </row>
-    <row r="423" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R422" s="11">
+        <f t="shared" si="19"/>
+        <v>3.6627158289237835E-2</v>
+      </c>
+      <c r="S422" s="19">
+        <f t="shared" si="20"/>
+        <v>-3.6627158289237833</v>
+      </c>
+    </row>
+    <row r="423" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A423" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B423" s="46">
-        <v>15000</v>
-      </c>
-      <c r="C423" s="46">
+      <c r="B423" s="11">
+        <v>16497.968720000001</v>
+      </c>
+      <c r="C423" s="45">
         <v>30100</v>
       </c>
-      <c r="D423" s="46">
+      <c r="D423" s="45">
         <v>94200</v>
       </c>
-      <c r="E423" s="46"/>
+      <c r="E423" s="45"/>
       <c r="F423" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>14929.591925925888</v>
       </c>
       <c r="G423">
@@ -17075,23 +17371,31 @@
       <c r="P423">
         <v>14489.042666666601</v>
       </c>
-    </row>
-    <row r="424" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R423" s="11">
+        <f t="shared" si="19"/>
+        <v>-9.5064842265873362E-2</v>
+      </c>
+      <c r="S423" s="19">
+        <f t="shared" si="20"/>
+        <v>9.5064842265873359</v>
+      </c>
+    </row>
+    <row r="424" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A424" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="B424" s="46">
-        <v>14900</v>
-      </c>
-      <c r="C424" s="46">
+      <c r="B424" s="11">
+        <v>20275.580959999999</v>
+      </c>
+      <c r="C424" s="45">
         <v>22300</v>
       </c>
-      <c r="D424" s="46">
+      <c r="D424" s="45">
         <v>85200</v>
       </c>
-      <c r="E424" s="46"/>
+      <c r="E424" s="45"/>
       <c r="F424" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>20397.098155555508</v>
       </c>
       <c r="G424">
@@ -17124,23 +17428,31 @@
       <c r="P424">
         <v>20112.312222222201</v>
       </c>
-    </row>
-    <row r="425" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R424" s="11">
+        <f t="shared" si="19"/>
+        <v>5.9932781110065324E-3</v>
+      </c>
+      <c r="S424" s="19">
+        <f t="shared" si="20"/>
+        <v>-0.59932781110065325</v>
+      </c>
+    </row>
+    <row r="425" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A425" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B425" s="46">
-        <v>10200</v>
-      </c>
-      <c r="C425" s="46">
+      <c r="B425" s="11">
+        <v>13444.76433</v>
+      </c>
+      <c r="C425" s="45">
         <v>24300</v>
       </c>
-      <c r="D425" s="46">
+      <c r="D425" s="45">
         <v>117000</v>
       </c>
-      <c r="E425" s="46"/>
+      <c r="E425" s="45"/>
       <c r="F425" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>11284.419377777747</v>
       </c>
       <c r="G425">
@@ -17173,249 +17485,577 @@
       <c r="P425">
         <v>12744.6397777777</v>
       </c>
-    </row>
-    <row r="426" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R425" s="11">
+        <f t="shared" si="19"/>
+        <v>-0.16068299147510998</v>
+      </c>
+      <c r="S425" s="19">
+        <f t="shared" si="20"/>
+        <v>16.068299147510999</v>
+      </c>
+    </row>
+    <row r="426" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A426" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B426" s="46">
-        <v>29300</v>
-      </c>
-      <c r="C426" s="46">
+      <c r="B426" s="11">
+        <v>36129.024490000003</v>
+      </c>
+      <c r="C426" s="45">
         <v>124000</v>
       </c>
-      <c r="D426" s="46">
+      <c r="D426" s="45">
         <v>549000</v>
       </c>
-      <c r="E426" s="46"/>
-      <c r="F426" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="427" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E426" s="45"/>
+      <c r="F426" s="19">
+        <f t="shared" si="23"/>
+        <v>207022.75875555529</v>
+      </c>
+      <c r="G426">
+        <v>164021.74299999999</v>
+      </c>
+      <c r="H426">
+        <v>122205.894</v>
+      </c>
+      <c r="I426">
+        <v>172769.11900000001</v>
+      </c>
+      <c r="J426">
+        <v>435877.087</v>
+      </c>
+      <c r="K426">
+        <v>136222.36900000001</v>
+      </c>
+      <c r="L426">
+        <v>218342.11133333301</v>
+      </c>
+      <c r="M426">
+        <v>278337.30377777701</v>
+      </c>
+      <c r="N426">
+        <v>243400.15688888801</v>
+      </c>
+      <c r="O426">
+        <v>140814.03200000001</v>
+      </c>
+      <c r="P426">
+        <v>158237.77155555499</v>
+      </c>
+      <c r="R426" s="11">
+        <f t="shared" si="19"/>
+        <v>4.7300954475772299</v>
+      </c>
+      <c r="S426" s="19">
+        <f t="shared" si="20"/>
+        <v>-473.00954475772301</v>
+      </c>
+    </row>
+    <row r="427" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A427" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B427" s="46">
+      <c r="B427" s="11">
         <v>52900</v>
       </c>
-      <c r="C427" s="46">
+      <c r="C427" s="45">
         <v>164000</v>
       </c>
-      <c r="D427" s="46">
+      <c r="D427" s="45">
         <v>601000</v>
       </c>
-      <c r="E427" s="46"/>
-      <c r="F427" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="428" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E427" s="45"/>
+      <c r="F427" s="19">
+        <f t="shared" si="23"/>
+        <v>143218.90014444414</v>
+      </c>
+      <c r="G427">
+        <v>95210.844888888896</v>
+      </c>
+      <c r="H427">
+        <v>136200.40177777701</v>
+      </c>
+      <c r="I427">
+        <v>189898.52622222199</v>
+      </c>
+      <c r="J427">
+        <v>171337.83911111101</v>
+      </c>
+      <c r="K427">
+        <v>173983.24733333301</v>
+      </c>
+      <c r="L427">
+        <v>117334.333</v>
+      </c>
+      <c r="M427">
+        <v>96815.714000000007</v>
+      </c>
+      <c r="N427">
+        <v>186761.78955555501</v>
+      </c>
+      <c r="O427">
+        <v>83367.455777777694</v>
+      </c>
+      <c r="P427">
+        <v>181278.84977777701</v>
+      </c>
+      <c r="R427" s="11">
+        <f t="shared" si="19"/>
+        <v>1.7073516095358061</v>
+      </c>
+      <c r="S427" s="19">
+        <f t="shared" si="20"/>
+        <v>-170.73516095358062</v>
+      </c>
+    </row>
+    <row r="428" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A428" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="B428" s="46">
+      <c r="B428" s="11">
         <v>69800</v>
       </c>
-      <c r="C428" s="46">
+      <c r="C428" s="45">
         <v>167000</v>
       </c>
-      <c r="D428" s="46">
+      <c r="D428" s="45">
         <v>551000</v>
       </c>
-      <c r="E428" s="46"/>
-      <c r="F428" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="429" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E428" s="45"/>
+      <c r="F428" s="19">
+        <f t="shared" si="23"/>
+        <v>267055.65427777747</v>
+      </c>
+      <c r="G428">
+        <v>352650.73866666597</v>
+      </c>
+      <c r="H428">
+        <v>292547.13099999999</v>
+      </c>
+      <c r="I428">
+        <v>210357.89244444401</v>
+      </c>
+      <c r="J428">
+        <v>239467.83377777701</v>
+      </c>
+      <c r="K428">
+        <v>79989.063555555505</v>
+      </c>
+      <c r="L428">
+        <v>343567.06777777697</v>
+      </c>
+      <c r="M428">
+        <v>261552.549</v>
+      </c>
+      <c r="N428">
+        <v>356312.95799999998</v>
+      </c>
+      <c r="R428" s="11">
+        <f t="shared" si="19"/>
+        <v>2.8260122389366402</v>
+      </c>
+      <c r="S428" s="19">
+        <f t="shared" si="20"/>
+        <v>-282.60122389366404</v>
+      </c>
+    </row>
+    <row r="429" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A429" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B429" s="46">
+      <c r="B429" s="11">
         <v>77800</v>
       </c>
-      <c r="C429" s="46">
+      <c r="C429" s="45">
         <v>191000</v>
       </c>
-      <c r="D429" s="46">
+      <c r="D429" s="45">
         <v>715000</v>
       </c>
-      <c r="E429" s="46"/>
-      <c r="F429" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="430" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E429" s="45"/>
+      <c r="F429" s="19">
+        <f t="shared" si="23"/>
+        <v>276897.77470000007</v>
+      </c>
+      <c r="G429">
+        <v>361988.228</v>
+      </c>
+      <c r="H429">
+        <v>732255.07</v>
+      </c>
+      <c r="I429">
+        <v>202407.78400000001</v>
+      </c>
+      <c r="J429">
+        <v>220081.008</v>
+      </c>
+      <c r="K429">
+        <v>188214.77900000001</v>
+      </c>
+      <c r="L429">
+        <v>327527.93599999999</v>
+      </c>
+      <c r="M429">
+        <v>204213.72399999999</v>
+      </c>
+      <c r="N429">
+        <v>174205.416</v>
+      </c>
+      <c r="O429">
+        <v>262261.37800000003</v>
+      </c>
+      <c r="P429">
+        <v>95822.423999999999</v>
+      </c>
+      <c r="R429" s="11">
+        <f t="shared" si="19"/>
+        <v>2.5590973611825203</v>
+      </c>
+      <c r="S429" s="19">
+        <f t="shared" si="20"/>
+        <v>-255.90973611825203</v>
+      </c>
+    </row>
+    <row r="430" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A430" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B430" s="46">
-        <v>36300</v>
-      </c>
-      <c r="C430" s="46">
+      <c r="B430" s="11">
+        <v>47357.535309999999</v>
+      </c>
+      <c r="C430" s="45">
         <v>181000</v>
       </c>
-      <c r="D430" s="46">
+      <c r="D430" s="45">
         <v>616000</v>
       </c>
-      <c r="E430" s="46"/>
-      <c r="F430" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="431" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E430" s="45"/>
+      <c r="F430" s="19">
+        <f t="shared" si="23"/>
+        <v>339636.52133333334</v>
+      </c>
+      <c r="G430">
+        <v>88323.585999999996</v>
+      </c>
+      <c r="H430">
+        <v>201047.31099999999</v>
+      </c>
+      <c r="I430">
+        <v>474327.098</v>
+      </c>
+      <c r="J430">
+        <v>183434.12299999999</v>
+      </c>
+      <c r="K430">
+        <v>277786.462</v>
+      </c>
+      <c r="L430">
+        <v>812900.54799999995</v>
+      </c>
+      <c r="R430" s="11">
+        <f t="shared" si="19"/>
+        <v>6.1717524805733674</v>
+      </c>
+      <c r="S430" s="19">
+        <f t="shared" si="20"/>
+        <v>-617.17524805733672</v>
+      </c>
+    </row>
+    <row r="431" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A431" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B431" s="46">
+      <c r="B431" s="11">
         <v>30900</v>
       </c>
-      <c r="C431" s="46">
+      <c r="C431" s="45">
         <v>176000</v>
       </c>
-      <c r="D431" s="46">
+      <c r="D431" s="45">
         <v>798000</v>
       </c>
-      <c r="E431" s="46"/>
-      <c r="F431" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="432" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E431" s="45"/>
+      <c r="F431" s="19">
+        <f t="shared" si="23"/>
+        <v>127134.93691358007</v>
+      </c>
+      <c r="G431">
+        <v>189867.79</v>
+      </c>
+      <c r="H431">
+        <v>47604.072</v>
+      </c>
+      <c r="I431">
+        <v>177147.40533333301</v>
+      </c>
+      <c r="J431">
+        <v>74595.248888888804</v>
+      </c>
+      <c r="K431">
+        <v>101578.350888888</v>
+      </c>
+      <c r="L431">
+        <v>151848.77911111101</v>
+      </c>
+      <c r="M431">
+        <v>82757.094444444403</v>
+      </c>
+      <c r="N431">
+        <v>222721.14933333301</v>
+      </c>
+      <c r="O431">
+        <v>96094.542222222197</v>
+      </c>
+      <c r="R431" s="11">
+        <f t="shared" si="19"/>
+        <v>3.1143992528666686</v>
+      </c>
+      <c r="S431" s="19">
+        <f t="shared" si="20"/>
+        <v>-311.43992528666683</v>
+      </c>
+    </row>
+    <row r="432" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A432" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B432" s="46">
+      <c r="B432" s="11">
         <v>26800</v>
       </c>
-      <c r="C432" s="46">
+      <c r="C432" s="45">
         <v>104000</v>
       </c>
-      <c r="D432" s="46">
+      <c r="D432" s="45">
         <v>603000</v>
       </c>
-      <c r="E432" s="46"/>
-      <c r="F432" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="433" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E432" s="45"/>
+      <c r="F432" s="19">
+        <f t="shared" si="23"/>
+        <v>83958.0199333333</v>
+      </c>
+      <c r="G432">
+        <v>116096.109111111</v>
+      </c>
+      <c r="H432">
+        <v>29262.415000000001</v>
+      </c>
+      <c r="I432">
+        <v>139410.85200000001</v>
+      </c>
+      <c r="J432">
+        <v>227857.71</v>
+      </c>
+      <c r="K432">
+        <v>118276.814</v>
+      </c>
+      <c r="L432">
+        <v>19390.263999999999</v>
+      </c>
+      <c r="M432">
+        <v>81489.434999999998</v>
+      </c>
+      <c r="N432">
+        <v>30315.036444444399</v>
+      </c>
+      <c r="O432">
+        <v>29783.2113333333</v>
+      </c>
+      <c r="P432">
+        <v>47698.352444444397</v>
+      </c>
+      <c r="R432" s="11">
+        <f t="shared" si="19"/>
+        <v>2.1327619378109439</v>
+      </c>
+      <c r="S432" s="19">
+        <f t="shared" si="20"/>
+        <v>-213.27619378109438</v>
+      </c>
+    </row>
+    <row r="433" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A433" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B433" s="46">
-        <v>15200</v>
-      </c>
-      <c r="C433" s="46">
+      <c r="B433" s="11">
+        <v>18153.645619999999</v>
+      </c>
+      <c r="C433" s="45">
         <v>124000</v>
       </c>
-      <c r="D433" s="46">
+      <c r="D433" s="45">
         <v>549000</v>
       </c>
-      <c r="E433" s="46"/>
-      <c r="F433" s="19" t="e">
-        <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="434" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E433" s="45"/>
+      <c r="F433" s="19">
+        <f t="shared" si="23"/>
+        <v>24510.86032222219</v>
+      </c>
+      <c r="G433">
+        <v>17346.763555555499</v>
+      </c>
+      <c r="H433">
+        <v>28511.510999999999</v>
+      </c>
+      <c r="I433">
+        <v>42622.4162222222</v>
+      </c>
+      <c r="J433">
+        <v>12842.07</v>
+      </c>
+      <c r="K433">
+        <v>18294</v>
+      </c>
+      <c r="L433">
+        <v>32022.610444444399</v>
+      </c>
+      <c r="M433">
+        <v>15969.1328888888</v>
+      </c>
+      <c r="N433">
+        <v>13005.1271111111</v>
+      </c>
+      <c r="O433">
+        <v>39516.830888888799</v>
+      </c>
+      <c r="P433">
+        <v>24978.141111111101</v>
+      </c>
+      <c r="R433" s="11">
+        <f t="shared" si="19"/>
+        <v>0.35018942394790403</v>
+      </c>
+      <c r="S433" s="19">
+        <f t="shared" si="20"/>
+        <v>-35.0189423947904</v>
+      </c>
+    </row>
+    <row r="434" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A434" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B434" s="46">
+      <c r="B434" s="11">
         <v>1580000</v>
       </c>
-      <c r="C434" s="46">
+      <c r="C434" s="45">
         <v>1180000</v>
       </c>
-      <c r="D434" s="46">
+      <c r="D434" s="45">
         <v>1590000</v>
       </c>
-      <c r="E434" s="46"/>
+      <c r="E434" s="45"/>
       <c r="F434" s="19" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="435" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R434" s="11" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S434" s="19" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="435" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A435" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B435" s="46">
+      <c r="B435" s="11">
         <v>931000</v>
       </c>
-      <c r="C435" s="46">
+      <c r="C435" s="45">
         <v>572000</v>
       </c>
-      <c r="D435" s="46">
+      <c r="D435" s="45">
         <v>2510000</v>
       </c>
-      <c r="E435" s="46"/>
+      <c r="E435" s="45"/>
       <c r="F435" s="19" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="436" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R435" s="11" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S435" s="19" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="436" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A436" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B436" s="46">
-        <v>74400</v>
-      </c>
-      <c r="C436" s="46">
+      <c r="B436" s="11">
+        <v>192540.7703</v>
+      </c>
+      <c r="C436" s="45">
         <v>515000</v>
       </c>
-      <c r="D436" s="46">
+      <c r="D436" s="45">
         <v>1340000</v>
       </c>
-      <c r="E436" s="46"/>
+      <c r="E436" s="45"/>
       <c r="F436" s="19" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="437" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R436" s="11" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S436" s="19" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="437" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A437" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B437" s="46">
+      <c r="B437" s="11">
         <v>761000</v>
       </c>
-      <c r="C437" s="46">
+      <c r="C437" s="45">
         <v>448000</v>
       </c>
-      <c r="D437" s="46">
+      <c r="D437" s="45">
         <v>2030000</v>
       </c>
-      <c r="E437" s="46"/>
-      <c r="F437" s="46"/>
-    </row>
-    <row r="438" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E437" s="45"/>
+      <c r="F437" s="45"/>
+      <c r="R437" s="11">
+        <f t="shared" si="19"/>
+        <v>-1</v>
+      </c>
+      <c r="S437" s="19">
+        <f t="shared" si="20"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="438" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A438" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B438" s="46">
+      <c r="B438" s="11">
         <v>84700</v>
       </c>
-      <c r="C438" s="46">
+      <c r="C438" s="45">
         <v>317000</v>
       </c>
-      <c r="D438" s="46">
+      <c r="D438" s="45">
         <v>1930000</v>
       </c>
-      <c r="E438" s="46"/>
-      <c r="F438" s="46"/>
-    </row>
-    <row r="439" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E438" s="45"/>
+      <c r="F438" s="45"/>
+      <c r="R438" s="11">
+        <f t="shared" si="19"/>
+        <v>-1</v>
+      </c>
+      <c r="S438" s="45"/>
+    </row>
+    <row r="439" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A439" s="32" t="s">
         <v>60</v>
       </c>
@@ -17430,13 +18070,18 @@
       </c>
       <c r="E439" s="11"/>
       <c r="F439" s="11"/>
-    </row>
-    <row r="440" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R439" s="11">
+        <f t="shared" si="19"/>
+        <v>-1</v>
+      </c>
+      <c r="S439" s="11"/>
+    </row>
+    <row r="440" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="32" t="s">
         <v>61</v>
       </c>
       <c r="B440" s="11">
-        <v>323000</v>
+        <v>519003.67749999999</v>
       </c>
       <c r="C440" s="11">
         <v>730000</v>
@@ -17446,8 +18091,13 @@
       </c>
       <c r="E440" s="11"/>
       <c r="F440" s="11"/>
-    </row>
-    <row r="441" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R440" s="11">
+        <f t="shared" si="19"/>
+        <v>-1</v>
+      </c>
+      <c r="S440" s="11"/>
+    </row>
+    <row r="441" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A441" s="32" t="s">
         <v>62</v>
       </c>
@@ -17462,13 +18112,18 @@
       </c>
       <c r="E441" s="11"/>
       <c r="F441" s="11"/>
-    </row>
-    <row r="442" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R441" s="11">
+        <f t="shared" si="19"/>
+        <v>-1</v>
+      </c>
+      <c r="S441" s="11"/>
+    </row>
+    <row r="442" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A442" s="32" t="s">
         <v>63</v>
       </c>
       <c r="B442" s="11">
-        <v>10400000</v>
+        <v>10686649.529999999</v>
       </c>
       <c r="C442" s="11">
         <v>22400000</v>
@@ -17478,13 +18133,17 @@
       </c>
       <c r="E442" s="11"/>
       <c r="F442" s="11"/>
-    </row>
-    <row r="443" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R442" s="11">
+        <f t="shared" si="19"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A443" s="32" t="s">
         <v>64</v>
       </c>
       <c r="B443" s="11">
-        <v>10000000</v>
+        <v>10283491.050000001</v>
       </c>
       <c r="C443" s="11">
         <v>13200000</v>
@@ -17494,13 +18153,14 @@
       </c>
       <c r="E443" s="11"/>
       <c r="F443" s="11"/>
-    </row>
-    <row r="444" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R443" s="11"/>
+    </row>
+    <row r="444" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A444" s="32" t="s">
         <v>65</v>
       </c>
       <c r="B444" s="11">
-        <v>7770000</v>
+        <v>9319943.2860000003</v>
       </c>
       <c r="C444" s="11">
         <v>12400000</v>
@@ -17510,8 +18170,9 @@
       </c>
       <c r="E444" s="11"/>
       <c r="F444" s="11"/>
-    </row>
-    <row r="445" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R444" s="11"/>
+    </row>
+    <row r="445" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445" s="32" t="s">
         <v>66</v>
       </c>
@@ -17527,12 +18188,12 @@
       <c r="E445" s="11"/>
       <c r="F445" s="11"/>
     </row>
-    <row r="446" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="32" t="s">
         <v>67</v>
       </c>
       <c r="B446" s="11">
-        <v>6030000</v>
+        <v>6331051.2470000004</v>
       </c>
       <c r="C446" s="11">
         <v>9100000</v>
@@ -17542,8 +18203,12 @@
       </c>
       <c r="E446" s="11"/>
       <c r="F446" s="11"/>
-    </row>
-    <row r="447" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S446" s="53">
+        <f xml:space="preserve"> AVERAGE(S386:S425)</f>
+        <v>27.37018786489719</v>
+      </c>
+    </row>
+    <row r="447" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A447" s="32" t="s">
         <v>68</v>
       </c>
@@ -17559,7 +18224,7 @@
       <c r="E447" s="11"/>
       <c r="F447" s="11"/>
     </row>
-    <row r="448" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A448" s="32" t="s">
         <v>69</v>
       </c>
@@ -18123,8 +18788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911A5E9-8C1D-4937-B2E8-4FEF8E2ACD16}">
   <dimension ref="A1:AA148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
sửa thuật toán chính GAVND5
</commit_message>
<xml_diff>
--- a/Kết quả thử nghiệm.xlsx
+++ b/Kết quả thử nghiệm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHUC\DPDP\New_DPDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7EB58-31B5-449F-8ECB-A0891899AE13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6917AC-B0F9-41C5-B931-B5E5E9C88FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,6 +593,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,7 +612,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A397" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S446" sqref="S446"/>
+    <sheetView tabSelected="1" topLeftCell="A316" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P332" sqref="P332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2159,22 +2159,22 @@
     <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
+      <c r="A44" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="L44" s="50" t="s">
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="L44" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="51"/>
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
@@ -3236,22 +3236,22 @@
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="51" t="s">
+      <c r="A63" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="49"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="L63" s="51" t="s">
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
+      <c r="L63" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="M63" s="49"/>
-      <c r="N63" s="49"/>
-      <c r="O63" s="49"/>
-      <c r="P63" s="49"/>
-      <c r="Q63" s="49"/>
+      <c r="M63" s="50"/>
+      <c r="N63" s="50"/>
+      <c r="O63" s="50"/>
+      <c r="P63" s="50"/>
+      <c r="Q63" s="50"/>
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
@@ -4220,12 +4220,12 @@
     </row>
     <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="49"/>
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="49"/>
+      <c r="A82" s="53"/>
+      <c r="B82" s="50"/>
+      <c r="C82" s="50"/>
+      <c r="D82" s="50"/>
+      <c r="E82" s="50"/>
+      <c r="F82" s="50"/>
       <c r="L82" s="5"/>
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
@@ -4724,14 +4724,14 @@
     <row r="102" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R104" s="47" t="s">
+      <c r="R104" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="S104" s="47"/>
-      <c r="T104" s="47"/>
-      <c r="U104" s="47"/>
-      <c r="V104" s="47"/>
-      <c r="W104" s="47"/>
+      <c r="S104" s="48"/>
+      <c r="T104" s="48"/>
+      <c r="U104" s="48"/>
+      <c r="V104" s="48"/>
+      <c r="W104" s="48"/>
     </row>
     <row r="105" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="27" t="s">
@@ -8137,22 +8137,22 @@
     <row r="175" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="176" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="177" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="48" t="s">
+      <c r="A177" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B177" s="49"/>
-      <c r="C177" s="49"/>
-      <c r="D177" s="49"/>
-      <c r="E177" s="49"/>
-      <c r="F177" s="49"/>
-      <c r="R177" s="49" t="s">
+      <c r="B177" s="50"/>
+      <c r="C177" s="50"/>
+      <c r="D177" s="50"/>
+      <c r="E177" s="50"/>
+      <c r="F177" s="50"/>
+      <c r="R177" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="S177" s="49"/>
-      <c r="T177" s="49"/>
-      <c r="U177" s="49"/>
-      <c r="V177" s="49"/>
-      <c r="W177" s="49"/>
+      <c r="S177" s="50"/>
+      <c r="T177" s="50"/>
+      <c r="U177" s="50"/>
+      <c r="V177" s="50"/>
+      <c r="W177" s="50"/>
     </row>
     <row r="178" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27" t="s">
@@ -13685,29 +13685,38 @@
         <v>183000</v>
       </c>
       <c r="F326" s="16">
-        <f t="shared" si="15"/>
-        <v>142707.54507936476</v>
+        <f xml:space="preserve"> AVERAGE(G326:P326)</f>
+        <v>183746.80266666616</v>
       </c>
       <c r="G326">
-        <v>153947.42000000001</v>
+        <v>161528.50222222201</v>
       </c>
       <c r="H326">
-        <v>184605.83555555501</v>
+        <v>211673.46444444399</v>
       </c>
       <c r="I326">
-        <v>89018.644444444406</v>
+        <v>197705.96444444399</v>
       </c>
       <c r="J326">
-        <v>167394.724444444</v>
+        <v>154222.44</v>
+      </c>
+      <c r="K326">
+        <v>216599.58444444399</v>
       </c>
       <c r="L326">
-        <v>128688.431111111</v>
+        <v>120552.377777777</v>
       </c>
       <c r="M326">
-        <v>133723.377777777</v>
+        <v>222127.108888888</v>
       </c>
       <c r="N326">
-        <v>141574.38222222199</v>
+        <v>213021.34666666601</v>
+      </c>
+      <c r="O326">
+        <v>175628.21555555501</v>
+      </c>
+      <c r="P326">
+        <v>164409.022222222</v>
       </c>
     </row>
     <row r="327" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13728,37 +13737,37 @@
       </c>
       <c r="F327" s="16">
         <f t="shared" si="15"/>
-        <v>174.05400000000003</v>
+        <v>178.80399999999992</v>
       </c>
       <c r="G327">
-        <v>171.14</v>
+        <v>170.51999999999899</v>
       </c>
       <c r="H327">
-        <v>173.72</v>
+        <v>177.92</v>
       </c>
       <c r="I327">
-        <v>182.94</v>
+        <v>169.08</v>
       </c>
       <c r="J327">
-        <v>171.1</v>
+        <v>176.56</v>
       </c>
       <c r="K327">
-        <v>163.84</v>
+        <v>188.58</v>
       </c>
       <c r="L327">
-        <v>179.22</v>
+        <v>190.94</v>
       </c>
       <c r="M327">
-        <v>166.88</v>
+        <v>184.86</v>
       </c>
       <c r="N327">
-        <v>185.52</v>
+        <v>178.74</v>
       </c>
       <c r="O327">
-        <v>159.19999999999999</v>
+        <v>166.16</v>
       </c>
       <c r="P327">
-        <v>186.98</v>
+        <v>184.68</v>
       </c>
     </row>
     <row r="328" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13779,16 +13788,37 @@
       </c>
       <c r="F328" s="16">
         <f t="shared" si="15"/>
-        <v>20781.988888888867</v>
+        <v>51789.177999999942</v>
+      </c>
+      <c r="G328">
+        <v>12471.3866666666</v>
+      </c>
+      <c r="H328">
+        <v>13442.5933333333</v>
+      </c>
+      <c r="I328">
+        <v>21760.651111111099</v>
+      </c>
+      <c r="J328">
+        <v>73244.317777777702</v>
+      </c>
+      <c r="K328">
+        <v>16490.006666666599</v>
       </c>
       <c r="L328">
-        <v>21422.253333333301</v>
+        <v>40722.5666666666</v>
       </c>
       <c r="M328">
-        <v>21831.48</v>
+        <v>57745.471111111103</v>
+      </c>
+      <c r="N328">
+        <v>45654.106666666601</v>
+      </c>
+      <c r="O328">
+        <v>55791.148888888798</v>
       </c>
       <c r="P328">
-        <v>19092.233333333301</v>
+        <v>180569.53111111099</v>
       </c>
     </row>
     <row r="329" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13809,28 +13839,37 @@
       </c>
       <c r="F329" s="16">
         <f xml:space="preserve"> AVERAGE(G329:P329)</f>
-        <v>178.93142857142828</v>
+        <v>1348.7262222222209</v>
       </c>
       <c r="G329">
-        <v>187.88</v>
+        <v>174.16</v>
+      </c>
+      <c r="H329">
+        <v>489.56</v>
       </c>
       <c r="I329">
-        <v>189.11999999999901</v>
+        <v>174.18</v>
+      </c>
+      <c r="J329">
+        <v>1568.24444444444</v>
       </c>
       <c r="K329">
-        <v>173.7</v>
+        <v>174.18</v>
+      </c>
+      <c r="L329">
+        <v>174.16</v>
       </c>
       <c r="M329">
-        <v>172.57999999999899</v>
+        <v>188.01999999999899</v>
       </c>
       <c r="N329">
-        <v>180.44</v>
+        <v>4193.08</v>
       </c>
       <c r="O329">
-        <v>174.62</v>
+        <v>6160.5777777777703</v>
       </c>
       <c r="P329">
-        <v>174.18</v>
+        <v>191.099999999999</v>
       </c>
     </row>
     <row r="330" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13851,25 +13890,37 @@
       </c>
       <c r="F330" s="16">
         <f t="shared" ref="F330:F345" si="16" xml:space="preserve"> AVERAGE(G330:P330)</f>
-        <v>878.42851851851674</v>
+        <v>1938.3351111111101</v>
       </c>
       <c r="G330">
-        <v>166.62</v>
+        <v>168.8</v>
+      </c>
+      <c r="H330">
+        <v>9325.4155555555499</v>
       </c>
       <c r="I330">
-        <v>158.56</v>
+        <v>169.11999999999901</v>
+      </c>
+      <c r="J330">
+        <v>8720.3555555555504</v>
       </c>
       <c r="K330">
-        <v>164.88</v>
+        <v>160.80000000000001</v>
+      </c>
+      <c r="L330">
+        <v>170.4</v>
       </c>
       <c r="M330">
-        <v>155.13999999999999</v>
+        <v>170.58</v>
       </c>
       <c r="N330">
-        <v>1082.1444444444401</v>
+        <v>165.8</v>
+      </c>
+      <c r="O330">
+        <v>169.18</v>
       </c>
       <c r="P330">
-        <v>3543.2266666666601</v>
+        <v>162.9</v>
       </c>
     </row>
     <row r="331" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13890,28 +13941,37 @@
       </c>
       <c r="F331" s="16">
         <f t="shared" si="16"/>
-        <v>20544.331746031705</v>
+        <v>44386.338444444409</v>
       </c>
       <c r="G331">
-        <v>16249.6111111111</v>
+        <v>74215.506666666595</v>
+      </c>
+      <c r="H331">
+        <v>19824.071111111101</v>
       </c>
       <c r="I331">
-        <v>6603.7155555555501</v>
+        <v>49814.391111111101</v>
+      </c>
+      <c r="J331">
+        <v>36897.235555555497</v>
       </c>
       <c r="K331">
-        <v>18213.026666666599</v>
+        <v>18456.326666666599</v>
       </c>
       <c r="L331">
-        <v>30445.855555555499</v>
+        <v>19347.593333333301</v>
+      </c>
+      <c r="M331">
+        <v>57513.131111111099</v>
       </c>
       <c r="N331">
-        <v>24268.9088888888</v>
+        <v>48280.771111111098</v>
       </c>
       <c r="O331">
-        <v>16756.6711111111</v>
+        <v>78344.78</v>
       </c>
       <c r="P331">
-        <v>31272.5333333333</v>
+        <v>41169.577777777697</v>
       </c>
     </row>
     <row r="332" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13932,31 +13992,34 @@
       </c>
       <c r="F332" s="16">
         <f t="shared" si="16"/>
-        <v>20344.828333333273</v>
+        <v>19445.814567901201</v>
+      </c>
+      <c r="G332">
+        <v>17598.926666666601</v>
       </c>
       <c r="H332">
-        <v>15425.608888888801</v>
+        <v>20866.6733333333</v>
       </c>
       <c r="I332">
-        <v>17565.313333333299</v>
+        <v>22341.3511111111</v>
       </c>
       <c r="J332">
-        <v>16691.9288888888</v>
+        <v>24497.971111111099</v>
+      </c>
+      <c r="K332">
+        <v>13998.8266666666</v>
       </c>
       <c r="L332">
-        <v>14201.904444444401</v>
+        <v>18360.444444444402</v>
       </c>
       <c r="M332">
-        <v>24808.137777777702</v>
+        <v>16238.311111111099</v>
       </c>
       <c r="N332">
-        <v>29805.126666666602</v>
+        <v>27113.8</v>
       </c>
       <c r="O332">
-        <v>24202.880000000001</v>
-      </c>
-      <c r="P332">
-        <v>20057.7266666666</v>
+        <v>13996.026666666599</v>
       </c>
     </row>
     <row r="333" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13977,37 +14040,34 @@
       </c>
       <c r="F333" s="16">
         <f t="shared" si="16"/>
-        <v>81.438999999999979</v>
+        <v>83.656666666666666</v>
       </c>
       <c r="G333">
-        <v>82.004999999999995</v>
+        <v>83.334999999999994</v>
       </c>
       <c r="H333">
-        <v>80.784999999999997</v>
+        <v>88.344999999999999</v>
       </c>
       <c r="I333">
-        <v>79.119999999999905</v>
+        <v>84.75</v>
       </c>
       <c r="J333">
-        <v>83.47</v>
+        <v>83.665000000000006</v>
       </c>
       <c r="K333">
-        <v>83.33</v>
+        <v>83.73</v>
       </c>
       <c r="L333">
-        <v>85.09</v>
+        <v>82.729999999999905</v>
       </c>
       <c r="M333">
-        <v>78.364999999999995</v>
+        <v>79.995000000000005</v>
       </c>
       <c r="N333">
-        <v>82.549999999999898</v>
+        <v>82.78</v>
       </c>
       <c r="O333">
-        <v>78.349999999999994</v>
-      </c>
-      <c r="P333">
-        <v>81.325000000000003</v>
+        <v>83.58</v>
       </c>
     </row>
     <row r="334" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14028,37 +14088,34 @@
       </c>
       <c r="F334" s="16">
         <f t="shared" si="16"/>
-        <v>87.762999999999977</v>
+        <v>87.089444444444439</v>
       </c>
       <c r="G334">
-        <v>88.584999999999994</v>
+        <v>85.68</v>
       </c>
       <c r="H334">
-        <v>92.47</v>
+        <v>83.74</v>
       </c>
       <c r="I334">
-        <v>84.439999999999898</v>
+        <v>86.699999999999903</v>
       </c>
       <c r="J334">
-        <v>89.825000000000003</v>
+        <v>85.74</v>
       </c>
       <c r="K334">
-        <v>86.8</v>
+        <v>87.46</v>
       </c>
       <c r="L334">
-        <v>91.87</v>
+        <v>87.094999999999999</v>
       </c>
       <c r="M334">
-        <v>84.694999999999993</v>
+        <v>89.06</v>
       </c>
       <c r="N334">
-        <v>86.924999999999997</v>
+        <v>91.22</v>
       </c>
       <c r="O334">
-        <v>87.534999999999997</v>
-      </c>
-      <c r="P334">
-        <v>84.4849999999999</v>
+        <v>87.11</v>
       </c>
     </row>
     <row r="335" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14077,39 +14134,9 @@
       <c r="E335" s="40">
         <v>120</v>
       </c>
-      <c r="F335" s="16">
+      <c r="F335" s="16" t="e">
         <f t="shared" si="16"/>
-        <v>116.8216111111107</v>
-      </c>
-      <c r="G335">
-        <v>110.375</v>
-      </c>
-      <c r="H335">
-        <v>110.729999999999</v>
-      </c>
-      <c r="I335">
-        <v>113.814999999999</v>
-      </c>
-      <c r="J335">
-        <v>141.81888888888801</v>
-      </c>
-      <c r="K335">
-        <v>145.56888888888801</v>
-      </c>
-      <c r="L335">
-        <v>113.34333333333301</v>
-      </c>
-      <c r="M335">
-        <v>113.25</v>
-      </c>
-      <c r="N335">
-        <v>105.785</v>
-      </c>
-      <c r="O335">
-        <v>105.995</v>
-      </c>
-      <c r="P335">
-        <v>107.535</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="336" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14128,39 +14155,9 @@
       <c r="E336" s="18">
         <v>100</v>
       </c>
-      <c r="F336" s="19">
+      <c r="F336" s="19" t="e">
         <f t="shared" si="16"/>
-        <v>3387.148777777772</v>
-      </c>
-      <c r="G336">
-        <v>3295.3027777777702</v>
-      </c>
-      <c r="H336">
-        <v>3526.6661111111098</v>
-      </c>
-      <c r="I336">
-        <v>3528.1861111111102</v>
-      </c>
-      <c r="J336">
-        <v>3302.4727777777698</v>
-      </c>
-      <c r="K336">
-        <v>3296.10777777777</v>
-      </c>
-      <c r="L336">
-        <v>3498.10777777777</v>
-      </c>
-      <c r="M336">
-        <v>3298.85777777777</v>
-      </c>
-      <c r="N336">
-        <v>3299.3427777777702</v>
-      </c>
-      <c r="O336">
-        <v>3529.13611111111</v>
-      </c>
-      <c r="P336">
-        <v>3297.3077777777698</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="337" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18203,7 +18200,7 @@
       </c>
       <c r="E446" s="11"/>
       <c r="F446" s="11"/>
-      <c r="S446" s="53">
+      <c r="S446" s="47">
         <f xml:space="preserve"> AVERAGE(S386:S425)</f>
         <v>27.37018786489719</v>
       </c>

</xml_diff>

<commit_message>
Thêm các ràng buộc cho cost và chống lặp vô hạn
</commit_message>
<xml_diff>
--- a/Kết quả thử nghiệm.xlsx
+++ b/Kết quả thử nghiệm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHUC\DPDP\New_DPDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6917AC-B0F9-41C5-B931-B5E5E9C88FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB2E3A7-0130-429A-977E-F418570615C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P332" sqref="P332"/>
+    <sheetView tabSelected="1" topLeftCell="A330" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O351" sqref="O351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13686,37 +13686,37 @@
       </c>
       <c r="F326" s="16">
         <f xml:space="preserve"> AVERAGE(G326:P326)</f>
-        <v>183746.80266666616</v>
+        <v>130400.34022222183</v>
       </c>
       <c r="G326">
-        <v>161528.50222222201</v>
+        <v>168786.22666666601</v>
       </c>
       <c r="H326">
-        <v>211673.46444444399</v>
+        <v>110920.96222222201</v>
       </c>
       <c r="I326">
-        <v>197705.96444444399</v>
+        <v>156206.90888888799</v>
       </c>
       <c r="J326">
-        <v>154222.44</v>
+        <v>98414.882222222193</v>
       </c>
       <c r="K326">
-        <v>216599.58444444399</v>
+        <v>146500.63777777701</v>
       </c>
       <c r="L326">
-        <v>120552.377777777</v>
+        <v>137100.82222222199</v>
       </c>
       <c r="M326">
-        <v>222127.108888888</v>
+        <v>132591.30444444399</v>
       </c>
       <c r="N326">
-        <v>213021.34666666601</v>
+        <v>113643.40222222199</v>
       </c>
       <c r="O326">
-        <v>175628.21555555501</v>
+        <v>118955.82</v>
       </c>
       <c r="P326">
-        <v>164409.022222222</v>
+        <v>120882.435555555</v>
       </c>
     </row>
     <row r="327" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13788,37 +13788,28 @@
       </c>
       <c r="F328" s="16">
         <f t="shared" si="15"/>
-        <v>51789.177999999942</v>
+        <v>29970.866984126915</v>
       </c>
       <c r="G328">
-        <v>12471.3866666666</v>
+        <v>38938.075555555501</v>
       </c>
       <c r="H328">
-        <v>13442.5933333333</v>
+        <v>22255.637777777702</v>
       </c>
       <c r="I328">
-        <v>21760.651111111099</v>
+        <v>29598.828888888798</v>
       </c>
       <c r="J328">
-        <v>73244.317777777702</v>
+        <v>29534.968888888801</v>
       </c>
       <c r="K328">
-        <v>16490.006666666599</v>
-      </c>
-      <c r="L328">
-        <v>40722.5666666666</v>
-      </c>
-      <c r="M328">
-        <v>57745.471111111103</v>
+        <v>40626.871111111097</v>
       </c>
       <c r="N328">
-        <v>45654.106666666601</v>
-      </c>
-      <c r="O328">
-        <v>55791.148888888798</v>
+        <v>35924.608888888797</v>
       </c>
       <c r="P328">
-        <v>180569.53111111099</v>
+        <v>12917.0777777777</v>
       </c>
     </row>
     <row r="329" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13839,20 +13830,14 @@
       </c>
       <c r="F329" s="16">
         <f xml:space="preserve"> AVERAGE(G329:P329)</f>
-        <v>1348.7262222222209</v>
+        <v>179.29999999999964</v>
       </c>
       <c r="G329">
         <v>174.16</v>
       </c>
-      <c r="H329">
-        <v>489.56</v>
-      </c>
       <c r="I329">
         <v>174.18</v>
       </c>
-      <c r="J329">
-        <v>1568.24444444444</v>
-      </c>
       <c r="K329">
         <v>174.18</v>
       </c>
@@ -13861,12 +13846,6 @@
       </c>
       <c r="M329">
         <v>188.01999999999899</v>
-      </c>
-      <c r="N329">
-        <v>4193.08</v>
-      </c>
-      <c r="O329">
-        <v>6160.5777777777703</v>
       </c>
       <c r="P329">
         <v>191.099999999999</v>
@@ -13890,19 +13869,13 @@
       </c>
       <c r="F330" s="16">
         <f t="shared" ref="F330:F345" si="16" xml:space="preserve"> AVERAGE(G330:P330)</f>
-        <v>1938.3351111111101</v>
+        <v>167.19749999999991</v>
       </c>
       <c r="G330">
         <v>168.8</v>
       </c>
-      <c r="H330">
-        <v>9325.4155555555499</v>
-      </c>
       <c r="I330">
         <v>169.11999999999901</v>
-      </c>
-      <c r="J330">
-        <v>8720.3555555555504</v>
       </c>
       <c r="K330">
         <v>160.80000000000001</v>
@@ -13941,37 +13914,31 @@
       </c>
       <c r="F331" s="16">
         <f t="shared" si="16"/>
-        <v>44386.338444444409</v>
-      </c>
-      <c r="G331">
-        <v>74215.506666666595</v>
+        <v>20242.6011111111</v>
       </c>
       <c r="H331">
-        <v>19824.071111111101</v>
+        <v>34599.722222222197</v>
       </c>
       <c r="I331">
-        <v>49814.391111111101</v>
+        <v>24214.942222222198</v>
       </c>
       <c r="J331">
-        <v>36897.235555555497</v>
+        <v>26221.98</v>
       </c>
       <c r="K331">
-        <v>18456.326666666599</v>
+        <v>7447.5711111111104</v>
       </c>
       <c r="L331">
-        <v>19347.593333333301</v>
+        <v>10834.36</v>
       </c>
       <c r="M331">
-        <v>57513.131111111099</v>
-      </c>
-      <c r="N331">
-        <v>48280.771111111098</v>
+        <v>10829.82</v>
       </c>
       <c r="O331">
-        <v>78344.78</v>
+        <v>33452.92</v>
       </c>
       <c r="P331">
-        <v>41169.577777777697</v>
+        <v>14339.493333333299</v>
       </c>
     </row>
     <row r="332" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13992,34 +13959,34 @@
       </c>
       <c r="F332" s="16">
         <f t="shared" si="16"/>
-        <v>19445.814567901201</v>
+        <v>14527.631358024648</v>
       </c>
       <c r="G332">
-        <v>17598.926666666601</v>
+        <v>16038.677777777701</v>
       </c>
       <c r="H332">
-        <v>20866.6733333333</v>
+        <v>18878.2</v>
       </c>
       <c r="I332">
-        <v>22341.3511111111</v>
+        <v>14747.1933333333</v>
       </c>
       <c r="J332">
-        <v>24497.971111111099</v>
+        <v>11022.026666666599</v>
       </c>
       <c r="K332">
-        <v>13998.8266666666</v>
+        <v>14413.971111111099</v>
       </c>
       <c r="L332">
-        <v>18360.444444444402</v>
-      </c>
-      <c r="M332">
-        <v>16238.311111111099</v>
+        <v>16833.6933333333</v>
       </c>
       <c r="N332">
-        <v>27113.8</v>
+        <v>9785.7333333333299</v>
       </c>
       <c r="O332">
-        <v>13996.026666666599</v>
+        <v>14260.9777777777</v>
+      </c>
+      <c r="P332">
+        <v>14768.208888888799</v>
       </c>
     </row>
     <row r="333" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14134,9 +14101,39 @@
       <c r="E335" s="40">
         <v>120</v>
       </c>
-      <c r="F335" s="16" t="e">
+      <c r="F335" s="16">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
+        <v>112.2491666666665</v>
+      </c>
+      <c r="G335">
+        <v>108.785</v>
+      </c>
+      <c r="H335">
+        <v>106.06</v>
+      </c>
+      <c r="I335">
+        <v>109.47499999999999</v>
+      </c>
+      <c r="J335">
+        <v>117.598333333333</v>
+      </c>
+      <c r="K335">
+        <v>105.81</v>
+      </c>
+      <c r="L335">
+        <v>114.948333333333</v>
+      </c>
+      <c r="M335">
+        <v>109.24</v>
+      </c>
+      <c r="N335">
+        <v>116.558333333333</v>
+      </c>
+      <c r="O335">
+        <v>115.23333333333299</v>
+      </c>
+      <c r="P335">
+        <v>118.783333333333</v>
       </c>
     </row>
     <row r="336" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -14155,12 +14152,42 @@
       <c r="E336" s="18">
         <v>100</v>
       </c>
-      <c r="F336" s="19" t="e">
+      <c r="F336" s="19">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="337" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3406.6567777777723</v>
+      </c>
+      <c r="G336">
+        <v>3299.73277777777</v>
+      </c>
+      <c r="H336">
+        <v>3530.92611111111</v>
+      </c>
+      <c r="I336">
+        <v>3297.73277777777</v>
+      </c>
+      <c r="J336">
+        <v>3297.4477777777702</v>
+      </c>
+      <c r="K336">
+        <v>3296.3627777777701</v>
+      </c>
+      <c r="L336">
+        <v>3492.9027777777701</v>
+      </c>
+      <c r="M336">
+        <v>3528.5811111111102</v>
+      </c>
+      <c r="N336">
+        <v>3496.6977777777702</v>
+      </c>
+      <c r="O336">
+        <v>3296.1627777777699</v>
+      </c>
+      <c r="P336">
+        <v>3530.0211111111098</v>
+      </c>
+    </row>
+    <row r="337" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="32" t="s">
         <v>27</v>
       </c>
@@ -14176,12 +14203,36 @@
       <c r="E337" s="40">
         <v>110</v>
       </c>
-      <c r="F337" s="16" t="e">
+      <c r="F337" s="16">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="338" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>104.08999999999988</v>
+      </c>
+      <c r="G337">
+        <v>104.304999999999</v>
+      </c>
+      <c r="H337">
+        <v>104.69</v>
+      </c>
+      <c r="I337">
+        <v>102.54</v>
+      </c>
+      <c r="J337">
+        <v>102.31</v>
+      </c>
+      <c r="K337">
+        <v>105.155</v>
+      </c>
+      <c r="L337">
+        <v>102.155</v>
+      </c>
+      <c r="M337">
+        <v>105.2</v>
+      </c>
+      <c r="N337">
+        <v>106.36499999999999</v>
+      </c>
+    </row>
+    <row r="338" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="8" t="s">
         <v>28</v>
       </c>
@@ -14197,12 +14248,30 @@
       <c r="E338" s="18">
         <v>96</v>
       </c>
-      <c r="F338" s="19" t="e">
+      <c r="F338" s="19">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="339" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1641.5255555555534</v>
+      </c>
+      <c r="G338">
+        <v>1642.4422222222199</v>
+      </c>
+      <c r="H338">
+        <v>1639.02722222222</v>
+      </c>
+      <c r="I338">
+        <v>1643.0022222222201</v>
+      </c>
+      <c r="J338">
+        <v>1642.64222222222</v>
+      </c>
+      <c r="L338">
+        <v>1642.0772222222199</v>
+      </c>
+      <c r="M338">
+        <v>1639.9622222222199</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="32" t="s">
         <v>29</v>
       </c>
@@ -14218,12 +14287,30 @@
       <c r="E339" s="40">
         <v>105</v>
       </c>
-      <c r="F339" s="16" t="e">
+      <c r="F339" s="16">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="340" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>104.4325</v>
+      </c>
+      <c r="G339">
+        <v>103.14</v>
+      </c>
+      <c r="H339">
+        <v>107.795</v>
+      </c>
+      <c r="I339">
+        <v>102.21</v>
+      </c>
+      <c r="J339">
+        <v>104.745</v>
+      </c>
+      <c r="L339">
+        <v>105.12</v>
+      </c>
+      <c r="M339">
+        <v>103.58499999999999</v>
+      </c>
+    </row>
+    <row r="340" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="8" t="s">
         <v>30</v>
       </c>
@@ -14239,12 +14326,27 @@
       <c r="E340" s="40">
         <v>94.4</v>
       </c>
-      <c r="F340" s="16" t="e">
+      <c r="F340" s="16">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="341" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89.744</v>
+      </c>
+      <c r="G340">
+        <v>88.54</v>
+      </c>
+      <c r="H340">
+        <v>90.77</v>
+      </c>
+      <c r="J340">
+        <v>88.305000000000007</v>
+      </c>
+      <c r="L340">
+        <v>91.11</v>
+      </c>
+      <c r="M340">
+        <v>89.995000000000005</v>
+      </c>
+    </row>
+    <row r="341" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="32" t="s">
         <v>31</v>
       </c>
@@ -14260,12 +14362,42 @@
       <c r="E341" s="18">
         <v>6428</v>
       </c>
-      <c r="F341" s="19" t="e">
+      <c r="F341" s="19">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="342" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9801.2519444444224</v>
+      </c>
+      <c r="G341">
+        <v>9851.0961111111101</v>
+      </c>
+      <c r="H341">
+        <v>9551.2511111111107</v>
+      </c>
+      <c r="I341">
+        <v>10485.8994444444</v>
+      </c>
+      <c r="J341">
+        <v>9697.9494444444408</v>
+      </c>
+      <c r="K341">
+        <v>9755.4611111111099</v>
+      </c>
+      <c r="L341">
+        <v>12830.9233333333</v>
+      </c>
+      <c r="M341">
+        <v>5926.65888888888</v>
+      </c>
+      <c r="N341">
+        <v>10202.472777777701</v>
+      </c>
+      <c r="O341">
+        <v>10089.394444444401</v>
+      </c>
+      <c r="P341">
+        <v>9621.4127777777703</v>
+      </c>
+    </row>
+    <row r="342" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="8" t="s">
         <v>32</v>
       </c>
@@ -14281,12 +14413,42 @@
       <c r="E342" s="40">
         <v>9285</v>
       </c>
-      <c r="F342" s="16" t="e">
+      <c r="F342" s="16">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="343" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8534.9488333333156</v>
+      </c>
+      <c r="G342">
+        <v>8321.8922222222209</v>
+      </c>
+      <c r="H342">
+        <v>6025.5372222222204</v>
+      </c>
+      <c r="I342">
+        <v>9662.6505555555505</v>
+      </c>
+      <c r="J342">
+        <v>10065.4783333333</v>
+      </c>
+      <c r="K342">
+        <v>5562.7155555555501</v>
+      </c>
+      <c r="L342">
+        <v>8562.2105555555499</v>
+      </c>
+      <c r="M342">
+        <v>12160.7583333333</v>
+      </c>
+      <c r="N342">
+        <v>5858.6255555555499</v>
+      </c>
+      <c r="O342">
+        <v>9040.4511111111096</v>
+      </c>
+      <c r="P342">
+        <v>10089.1688888888</v>
+      </c>
+    </row>
+    <row r="343" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="32" t="s">
         <v>33</v>
       </c>
@@ -14302,12 +14464,42 @@
       <c r="E343" s="40">
         <v>130</v>
       </c>
-      <c r="F343" s="16" t="e">
+      <c r="F343" s="16">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="344" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>128.17699999999962</v>
+      </c>
+      <c r="G343">
+        <v>127.485</v>
+      </c>
+      <c r="H343">
+        <v>130.87</v>
+      </c>
+      <c r="I343">
+        <v>128.73499999999899</v>
+      </c>
+      <c r="J343">
+        <v>127.61</v>
+      </c>
+      <c r="K343">
+        <v>130.495</v>
+      </c>
+      <c r="L343">
+        <v>130.625</v>
+      </c>
+      <c r="M343">
+        <v>127.92</v>
+      </c>
+      <c r="N343">
+        <v>126.009999999999</v>
+      </c>
+      <c r="O343">
+        <v>126.009999999999</v>
+      </c>
+      <c r="P343">
+        <v>126.009999999999</v>
+      </c>
+    </row>
+    <row r="344" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="8" t="s">
         <v>34</v>
       </c>
@@ -14323,12 +14515,42 @@
       <c r="E344" s="18">
         <v>302</v>
       </c>
-      <c r="F344" s="19" t="e">
+      <c r="F344" s="19">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="345" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7153.3489444444422</v>
+      </c>
+      <c r="G344">
+        <v>7128.89222222222</v>
+      </c>
+      <c r="H344">
+        <v>7135.7222222222199</v>
+      </c>
+      <c r="I344">
+        <v>7133.5922222222198</v>
+      </c>
+      <c r="J344">
+        <v>7138.0372222222204</v>
+      </c>
+      <c r="K344">
+        <v>7136.7522222222196</v>
+      </c>
+      <c r="L344">
+        <v>7129.9272222222198</v>
+      </c>
+      <c r="M344">
+        <v>7333.2644444444404</v>
+      </c>
+      <c r="N344">
+        <v>7133.6172222222203</v>
+      </c>
+      <c r="O344">
+        <v>7133.6172222222203</v>
+      </c>
+      <c r="P344">
+        <v>7130.0672222222202</v>
+      </c>
+    </row>
+    <row r="345" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="32" t="s">
         <v>35</v>
       </c>
@@ -14344,12 +14566,39 @@
       <c r="E345" s="18">
         <v>925</v>
       </c>
-      <c r="F345" s="19" t="e">
+      <c r="F345" s="19">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="346" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5492.8387037036982</v>
+      </c>
+      <c r="G345">
+        <v>3025.2166666666599</v>
+      </c>
+      <c r="H345">
+        <v>6091.6738888888804</v>
+      </c>
+      <c r="J345">
+        <v>5668.4505555555497</v>
+      </c>
+      <c r="K345">
+        <v>5669.13055555555</v>
+      </c>
+      <c r="L345">
+        <v>6071.0855555555499</v>
+      </c>
+      <c r="M345">
+        <v>5699.8044444444404</v>
+      </c>
+      <c r="N345">
+        <v>5669.13055555555</v>
+      </c>
+      <c r="O345">
+        <v>5871.9255555555501</v>
+      </c>
+      <c r="P345">
+        <v>5669.13055555555</v>
+      </c>
+    </row>
+    <row r="346" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="8" t="s">
         <v>36</v>
       </c>
@@ -14370,7 +14619,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="347" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="32" t="s">
         <v>37</v>
       </c>
@@ -14386,12 +14635,42 @@
       <c r="E347" s="40">
         <v>22000</v>
       </c>
-      <c r="F347" s="16" t="e">
-        <f t="shared" ref="F347:F367" si="17" xml:space="preserve"> AVERAGE(G347:P347)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="348" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F347" s="16">
+        <f xml:space="preserve"> AVERAGE(G347:P347)</f>
+        <v>15396.787866666651</v>
+      </c>
+      <c r="G347">
+        <v>14681.418</v>
+      </c>
+      <c r="H347">
+        <v>15915.227000000001</v>
+      </c>
+      <c r="I347">
+        <v>15918.182000000001</v>
+      </c>
+      <c r="J347">
+        <v>16120.347</v>
+      </c>
+      <c r="K347">
+        <v>16808.321666666601</v>
+      </c>
+      <c r="L347">
+        <v>19749.764999999999</v>
+      </c>
+      <c r="M347">
+        <v>16183.993</v>
+      </c>
+      <c r="N347">
+        <v>10261.3416666666</v>
+      </c>
+      <c r="O347">
+        <v>13749.674999999999</v>
+      </c>
+      <c r="P347">
+        <v>14579.608333333301</v>
+      </c>
+    </row>
+    <row r="348" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="8" t="s">
         <v>38</v>
       </c>
@@ -14407,57 +14686,63 @@
       <c r="E348" s="18">
         <v>200</v>
       </c>
-      <c r="F348" s="19" t="e">
+      <c r="F348" s="19">
+        <f t="shared" ref="F348:F367" si="17" xml:space="preserve"> AVERAGE(G348:P348)</f>
+        <v>6638.2183666666651</v>
+      </c>
+      <c r="G348">
+        <v>5827.8689999999997</v>
+      </c>
+      <c r="H348">
+        <v>7729.5389999999998</v>
+      </c>
+      <c r="I348">
+        <v>6191.1459999999997</v>
+      </c>
+      <c r="J348">
+        <v>7528.9440000000004</v>
+      </c>
+      <c r="K348">
+        <v>5993.0955555555502</v>
+      </c>
+      <c r="L348">
+        <v>6257.8469999999998</v>
+      </c>
+      <c r="M348">
+        <v>5687.7110000000002</v>
+      </c>
+      <c r="N348">
+        <v>5688.4359999999997</v>
+      </c>
+      <c r="O348">
+        <v>7621.0788888888801</v>
+      </c>
+      <c r="P348">
+        <v>7856.51722222222</v>
+      </c>
+    </row>
+    <row r="349" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B349" s="11">
+        <v>3667.1041329999998</v>
+      </c>
+      <c r="C349" s="39">
+        <v>7030</v>
+      </c>
+      <c r="D349" s="40">
+        <v>95000</v>
+      </c>
+      <c r="E349" s="41">
+        <v>1300</v>
+      </c>
+      <c r="F349" s="16" t="e">
         <f t="shared" si="17"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="349" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B349" s="11">
-        <v>3667.1041329999998</v>
-      </c>
-      <c r="C349" s="39">
-        <v>7030</v>
-      </c>
-      <c r="D349" s="40">
-        <v>95000</v>
-      </c>
-      <c r="E349" s="41">
-        <v>1300</v>
-      </c>
-      <c r="F349" s="16">
-        <f t="shared" si="17"/>
-        <v>75.40674999999996</v>
-      </c>
-      <c r="G349">
-        <v>76.616</v>
-      </c>
-      <c r="H349">
-        <v>76.073999999999899</v>
-      </c>
-      <c r="I349">
-        <v>72.337999999999994</v>
-      </c>
-      <c r="J349">
-        <v>72.363999999999905</v>
-      </c>
-      <c r="K349">
-        <v>75.569999999999993</v>
-      </c>
-      <c r="L349">
-        <v>77.518000000000001</v>
-      </c>
-      <c r="M349">
-        <v>76.367999999999995</v>
-      </c>
-      <c r="N349">
-        <v>76.406000000000006</v>
-      </c>
-    </row>
-    <row r="350" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="32" t="s">
         <v>40</v>
       </c>
@@ -14473,33 +14758,12 @@
       <c r="E350" s="18">
         <v>100</v>
       </c>
-      <c r="F350" s="19">
+      <c r="F350" s="19" t="e">
         <f t="shared" si="17"/>
-        <v>6721.8893968253897</v>
-      </c>
-      <c r="G350">
-        <v>7151.0086666666602</v>
-      </c>
-      <c r="H350">
-        <v>10492.193111111101</v>
-      </c>
-      <c r="I350">
-        <v>9087.2817777777691</v>
-      </c>
-      <c r="J350">
-        <v>3517.18711111111</v>
-      </c>
-      <c r="K350">
-        <v>5161.6337777777699</v>
-      </c>
-      <c r="L350">
-        <v>6292.1208888888796</v>
-      </c>
-      <c r="M350">
-        <v>5351.8004444444396</v>
-      </c>
-    </row>
-    <row r="351" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="351" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="32" t="s">
         <v>41</v>
       </c>
@@ -14515,36 +14779,12 @@
       <c r="E351" s="18">
         <v>100</v>
       </c>
-      <c r="F351" s="19">
-        <f t="shared" si="17"/>
-        <v>3439.5528055555501</v>
-      </c>
-      <c r="G351">
-        <v>3439.7535555555501</v>
-      </c>
-      <c r="H351">
-        <v>3440.2415555555499</v>
-      </c>
-      <c r="I351">
-        <v>3439.8295555555501</v>
-      </c>
-      <c r="J351">
-        <v>3441.00755555555</v>
-      </c>
-      <c r="K351">
-        <v>3438.7235555555499</v>
-      </c>
-      <c r="L351">
-        <v>3435.6955555555501</v>
-      </c>
-      <c r="M351">
-        <v>3439.1135555555502</v>
-      </c>
-      <c r="N351">
-        <v>3442.0575555555502</v>
-      </c>
-    </row>
-    <row r="352" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F351" s="19" t="e">
+        <f xml:space="preserve"> AVERAGE(G351:P351)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="352" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="32" t="s">
         <v>42</v>
       </c>
@@ -14560,36 +14800,12 @@
       <c r="E352" s="18">
         <v>900</v>
       </c>
-      <c r="F352" s="19">
+      <c r="F352" s="19" t="e">
         <f t="shared" si="17"/>
-        <v>16175.446305555502</v>
-      </c>
-      <c r="G352">
-        <v>16870.1455555555</v>
-      </c>
-      <c r="H352">
-        <v>15306.350888888799</v>
-      </c>
-      <c r="I352">
-        <v>13071.2473333333</v>
-      </c>
-      <c r="J352">
-        <v>17786.636444444401</v>
-      </c>
-      <c r="K352">
-        <v>14320.6397777777</v>
-      </c>
-      <c r="L352">
-        <v>16874.241555555502</v>
-      </c>
-      <c r="M352">
-        <v>17254.641111111101</v>
-      </c>
-      <c r="N352">
-        <v>17919.6677777777</v>
-      </c>
-    </row>
-    <row r="353" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="32" t="s">
         <v>43</v>
       </c>
@@ -14603,42 +14819,12 @@
         <v>95700</v>
       </c>
       <c r="E353" s="11"/>
-      <c r="F353" s="19">
+      <c r="F353" s="19" t="e">
         <f t="shared" si="17"/>
-        <v>10559.417244444416</v>
-      </c>
-      <c r="G353">
-        <v>7403.4340000000002</v>
-      </c>
-      <c r="H353">
-        <v>9994.3808888888798</v>
-      </c>
-      <c r="I353">
-        <v>11661.5895555555</v>
-      </c>
-      <c r="J353">
-        <v>9526.2962222222195</v>
-      </c>
-      <c r="K353">
-        <v>11826.0482222222</v>
-      </c>
-      <c r="L353">
-        <v>11726.098222222199</v>
-      </c>
-      <c r="M353">
-        <v>12058.531555555501</v>
-      </c>
-      <c r="N353">
-        <v>11960.6875555555</v>
-      </c>
-      <c r="O353">
-        <v>11865.995555555501</v>
-      </c>
-      <c r="P353">
-        <v>7571.1106666666601</v>
-      </c>
-    </row>
-    <row r="354" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="32" t="s">
         <v>44</v>
       </c>
@@ -14652,39 +14838,13 @@
         <v>94200</v>
       </c>
       <c r="E354" s="11"/>
-      <c r="F354" s="19">
+      <c r="F354" s="19" t="e">
         <f t="shared" si="17"/>
-        <v>15479.12938271601</v>
-      </c>
-      <c r="G354">
-        <v>18008.4931111111</v>
-      </c>
-      <c r="H354">
-        <v>17641.586444444401</v>
-      </c>
-      <c r="I354" s="42">
-        <v>17203.9391111111</v>
-      </c>
-      <c r="J354">
-        <v>18176.341777777699</v>
-      </c>
-      <c r="K354">
-        <v>13573.589777777701</v>
-      </c>
-      <c r="L354">
-        <v>11105.961111111101</v>
-      </c>
-      <c r="M354">
-        <v>15309.105111111099</v>
-      </c>
-      <c r="N354">
-        <v>12685.8728888888</v>
-      </c>
-      <c r="O354">
-        <v>15607.275111111099</v>
-      </c>
-    </row>
-    <row r="355" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I354" s="42"/>
+    </row>
+    <row r="355" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="32" t="s">
         <v>45</v>
       </c>
@@ -14698,39 +14858,12 @@
         <v>85200</v>
       </c>
       <c r="E355" s="11"/>
-      <c r="F355" s="19">
+      <c r="F355" s="19" t="e">
         <f t="shared" si="17"/>
-        <v>20701.367777777723</v>
-      </c>
-      <c r="G355">
-        <v>19248.343555555501</v>
-      </c>
-      <c r="H355">
-        <v>20945.167555555501</v>
-      </c>
-      <c r="I355">
-        <v>21414.2522222222</v>
-      </c>
-      <c r="J355">
-        <v>21478.886888888799</v>
-      </c>
-      <c r="K355">
-        <v>19143.811555555501</v>
-      </c>
-      <c r="L355">
-        <v>21245.933555555501</v>
-      </c>
-      <c r="M355">
-        <v>21414.5582222222</v>
-      </c>
-      <c r="N355">
-        <v>19876.650888888798</v>
-      </c>
-      <c r="O355">
-        <v>21544.705555555502</v>
-      </c>
-    </row>
-    <row r="356" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="356" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="32" t="s">
         <v>46</v>
       </c>
@@ -14744,42 +14877,12 @@
         <v>117000</v>
       </c>
       <c r="E356" s="11"/>
-      <c r="F356" s="19">
+      <c r="F356" s="19" t="e">
         <f t="shared" si="17"/>
-        <v>10650.547577777757</v>
-      </c>
-      <c r="G356">
-        <v>11778.4911111111</v>
-      </c>
-      <c r="H356">
-        <v>13510.790444444399</v>
-      </c>
-      <c r="I356">
-        <v>10497.4551111111</v>
-      </c>
-      <c r="J356">
-        <v>8495.9677777777706</v>
-      </c>
-      <c r="K356">
-        <v>9799.2811111111096</v>
-      </c>
-      <c r="L356">
-        <v>10399.7951111111</v>
-      </c>
-      <c r="M356">
-        <v>12376.543111111099</v>
-      </c>
-      <c r="N356">
-        <v>9835.5444444444402</v>
-      </c>
-      <c r="O356">
-        <v>9070.58977777777</v>
-      </c>
-      <c r="P356">
-        <v>10741.017777777701</v>
-      </c>
-    </row>
-    <row r="357" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="357" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="32" t="s">
         <v>47</v>
       </c>
@@ -14798,7 +14901,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="358" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="32" t="s">
         <v>48</v>
       </c>
@@ -14817,7 +14920,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="359" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="32" t="s">
         <v>49</v>
       </c>
@@ -14836,7 +14939,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="360" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="32" t="s">
         <v>50</v>
       </c>
@@ -14855,7 +14958,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="361" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="32" t="s">
         <v>51</v>
       </c>
@@ -14874,7 +14977,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="362" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="32" t="s">
         <v>52</v>
       </c>
@@ -14893,7 +14996,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="363" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="32" t="s">
         <v>53</v>
       </c>
@@ -14912,7 +15015,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="364" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="32" t="s">
         <v>54</v>
       </c>
@@ -14931,7 +15034,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="365" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="32" t="s">
         <v>55</v>
       </c>
@@ -14950,7 +15053,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="366" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="32" t="s">
         <v>56</v>
       </c>
@@ -14969,7 +15072,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="367" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="32" t="s">
         <v>57</v>
       </c>
@@ -14988,7 +15091,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="368" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="32" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Cập nhật thuật toán GAVND6
</commit_message>
<xml_diff>
--- a/Kết quả thử nghiệm.xlsx
+++ b/Kết quả thử nghiệm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHUC\DPDP\New_DPDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB2E3A7-0130-429A-977E-F418570615C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0A0ABA-18AF-472C-9C50-D102C7F9BA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -830,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O351" sqref="O351"/>
+    <sheetView tabSelected="1" topLeftCell="A406" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F328" sqref="F328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13686,37 +13686,37 @@
       </c>
       <c r="F326" s="16">
         <f xml:space="preserve"> AVERAGE(G326:P326)</f>
-        <v>130400.34022222183</v>
+        <v>126363.84222222201</v>
       </c>
       <c r="G326">
-        <v>168786.22666666601</v>
+        <v>115298.86</v>
       </c>
       <c r="H326">
-        <v>110920.96222222201</v>
+        <v>117446.32</v>
       </c>
       <c r="I326">
-        <v>156206.90888888799</v>
+        <v>121328.177777777</v>
       </c>
       <c r="J326">
-        <v>98414.882222222193</v>
+        <v>138760.62444444399</v>
       </c>
       <c r="K326">
-        <v>146500.63777777701</v>
+        <v>145471.67999999999</v>
       </c>
       <c r="L326">
-        <v>137100.82222222199</v>
+        <v>146481.731111111</v>
       </c>
       <c r="M326">
-        <v>132591.30444444399</v>
+        <v>123929.11111111099</v>
       </c>
       <c r="N326">
-        <v>113643.40222222199</v>
+        <v>116147.74</v>
       </c>
       <c r="O326">
-        <v>118955.82</v>
+        <v>121327.857777777</v>
       </c>
       <c r="P326">
-        <v>120882.435555555</v>
+        <v>117446.32</v>
       </c>
     </row>
     <row r="327" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cap nhat thuat toan GAVND7
</commit_message>
<xml_diff>
--- a/Kết quả thử nghiệm.xlsx
+++ b/Kết quả thử nghiệm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PHUC\DPDP\New_DPDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0A0ABA-18AF-472C-9C50-D102C7F9BA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10548B1-684A-44C5-A316-CD21E15DA373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -350,17 +350,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -521,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,6 +597,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="13" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -830,28 +838,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A406" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F328" sqref="F328"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B369" sqref="B369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="9" width="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="11" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
-    <col min="16" max="17" width="11.42578125" customWidth="1"/>
+    <col min="15" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" customWidth="1"/>
     <col min="19" max="20" width="12.42578125" customWidth="1"/>
     <col min="21" max="21" width="12.5703125" customWidth="1"/>
@@ -2159,22 +2162,22 @@
     <row r="42" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="L44" s="51" t="s">
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="L44" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="51"/>
+      <c r="M44" s="54"/>
+      <c r="N44" s="54"/>
+      <c r="O44" s="54"/>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="54"/>
     </row>
     <row r="45" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
@@ -3236,22 +3239,22 @@
     </row>
     <row r="62" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="52" t="s">
+      <c r="A63" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="50"/>
-      <c r="F63" s="50"/>
-      <c r="L63" s="52" t="s">
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="L63" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="M63" s="50"/>
-      <c r="N63" s="50"/>
-      <c r="O63" s="50"/>
-      <c r="P63" s="50"/>
-      <c r="Q63" s="50"/>
+      <c r="M63" s="53"/>
+      <c r="N63" s="53"/>
+      <c r="O63" s="53"/>
+      <c r="P63" s="53"/>
+      <c r="Q63" s="53"/>
     </row>
     <row r="64" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
@@ -4220,12 +4223,12 @@
     </row>
     <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="53"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="50"/>
-      <c r="F82" s="50"/>
+      <c r="A82" s="56"/>
+      <c r="B82" s="53"/>
+      <c r="C82" s="53"/>
+      <c r="D82" s="53"/>
+      <c r="E82" s="53"/>
+      <c r="F82" s="53"/>
       <c r="L82" s="5"/>
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
@@ -4724,14 +4727,14 @@
     <row r="102" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="103" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R104" s="48" t="s">
+      <c r="R104" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="S104" s="48"/>
-      <c r="T104" s="48"/>
-      <c r="U104" s="48"/>
-      <c r="V104" s="48"/>
-      <c r="W104" s="48"/>
+      <c r="S104" s="51"/>
+      <c r="T104" s="51"/>
+      <c r="U104" s="51"/>
+      <c r="V104" s="51"/>
+      <c r="W104" s="51"/>
     </row>
     <row r="105" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="27" t="s">
@@ -8137,22 +8140,22 @@
     <row r="175" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="176" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="177" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="49" t="s">
+      <c r="A177" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B177" s="50"/>
-      <c r="C177" s="50"/>
-      <c r="D177" s="50"/>
-      <c r="E177" s="50"/>
-      <c r="F177" s="50"/>
-      <c r="R177" s="50" t="s">
+      <c r="B177" s="53"/>
+      <c r="C177" s="53"/>
+      <c r="D177" s="53"/>
+      <c r="E177" s="53"/>
+      <c r="F177" s="53"/>
+      <c r="R177" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="S177" s="50"/>
-      <c r="T177" s="50"/>
-      <c r="U177" s="50"/>
-      <c r="V177" s="50"/>
-      <c r="W177" s="50"/>
+      <c r="S177" s="53"/>
+      <c r="T177" s="53"/>
+      <c r="U177" s="53"/>
+      <c r="V177" s="53"/>
+      <c r="W177" s="53"/>
     </row>
     <row r="178" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="27" t="s">
@@ -11370,7 +11373,7 @@
         <v>95</v>
       </c>
       <c r="F255" s="16">
-        <f t="shared" ref="F255:F298" si="13" xml:space="preserve"> AVERAGE(G255:P255)</f>
+        <f t="shared" ref="F255:F311" si="13" xml:space="preserve"> AVERAGE(G255:P255)</f>
         <v>65.543999999999954</v>
       </c>
       <c r="G255">
@@ -13261,7 +13264,10 @@
         <v>2030000</v>
       </c>
       <c r="E299" s="11"/>
-      <c r="F299" s="11"/>
+      <c r="F299" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="300" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="32" t="s">
@@ -13277,7 +13283,10 @@
         <v>1930000</v>
       </c>
       <c r="E300" s="11"/>
-      <c r="F300" s="11"/>
+      <c r="F300" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="301" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="32" t="s">
@@ -13293,7 +13302,10 @@
         <v>2000000</v>
       </c>
       <c r="E301" s="11"/>
-      <c r="F301" s="11"/>
+      <c r="F301" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="302" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="32" t="s">
@@ -13309,7 +13321,10 @@
         <v>1980000</v>
       </c>
       <c r="E302" s="11"/>
-      <c r="F302" s="11"/>
+      <c r="F302" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="303" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="32" t="s">
@@ -13325,7 +13340,10 @@
         <v>2160000</v>
       </c>
       <c r="E303" s="11"/>
-      <c r="F303" s="11"/>
+      <c r="F303" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="304" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="32" t="s">
@@ -13341,9 +13359,12 @@
         <v>16500000</v>
       </c>
       <c r="E304" s="11"/>
-      <c r="F304" s="11"/>
-    </row>
-    <row r="305" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F304" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="305" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="32" t="s">
         <v>64</v>
       </c>
@@ -13357,9 +13378,12 @@
         <v>11200000</v>
       </c>
       <c r="E305" s="11"/>
-      <c r="F305" s="11"/>
-    </row>
-    <row r="306" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F305" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="306" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="32" t="s">
         <v>65</v>
       </c>
@@ -13373,9 +13397,12 @@
         <v>9540000</v>
       </c>
       <c r="E306" s="11"/>
-      <c r="F306" s="11"/>
-    </row>
-    <row r="307" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F306" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="307" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="32" t="s">
         <v>66</v>
       </c>
@@ -13389,9 +13416,12 @@
         <v>13200000</v>
       </c>
       <c r="E307" s="11"/>
-      <c r="F307" s="11"/>
-    </row>
-    <row r="308" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F307" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="308" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="32" t="s">
         <v>67</v>
       </c>
@@ -13405,9 +13435,12 @@
         <v>7210000</v>
       </c>
       <c r="E308" s="11"/>
-      <c r="F308" s="11"/>
-    </row>
-    <row r="309" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F308" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="309" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="32" t="s">
         <v>68</v>
       </c>
@@ -13421,9 +13454,12 @@
         <v>10900000</v>
       </c>
       <c r="E309" s="11"/>
-      <c r="F309" s="11"/>
-    </row>
-    <row r="310" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F309" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="310" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="32" t="s">
         <v>69</v>
       </c>
@@ -13437,9 +13473,12 @@
         <v>25000000</v>
       </c>
       <c r="E310" s="11"/>
-      <c r="F310" s="11"/>
-    </row>
-    <row r="311" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F310" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="311" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="32" t="s">
         <v>70</v>
       </c>
@@ -13453,13 +13492,16 @@
         <v>27400000</v>
       </c>
       <c r="E311" s="11"/>
-      <c r="F311" s="11"/>
-    </row>
-    <row r="312" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F311" s="19" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="312" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="27" t="s">
         <v>71</v>
       </c>
@@ -13479,7 +13521,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="317" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="8" t="s">
         <v>0</v>
       </c>
@@ -13495,12 +13537,50 @@
       <c r="E317" s="19">
         <v>135</v>
       </c>
-      <c r="F317" s="16" t="e">
+      <c r="F317" s="19">
         <f xml:space="preserve"> AVERAGE(G317:P317)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>130.37199999999979</v>
+      </c>
+      <c r="G317">
+        <v>116.979999999999</v>
+      </c>
+      <c r="H317">
+        <v>131.69999999999999</v>
+      </c>
+      <c r="I317">
+        <v>128.38</v>
+      </c>
+      <c r="J317">
+        <v>137.06</v>
+      </c>
+      <c r="K317">
+        <v>136.1</v>
+      </c>
+      <c r="L317">
+        <v>131.69999999999999</v>
+      </c>
+      <c r="M317">
+        <v>135.72</v>
+      </c>
+      <c r="N317">
+        <v>135.91999999999999</v>
+      </c>
+      <c r="O317">
+        <v>132.74</v>
+      </c>
+      <c r="P317">
+        <v>117.41999999999901</v>
+      </c>
+      <c r="S317">
+        <f>COUNTIF(T317:T372, "&gt;=0")</f>
+        <v>41</v>
+      </c>
+      <c r="T317">
+        <f>(B317-F317)/B317 * 100</f>
+        <v>2.707462686567323</v>
+      </c>
+    </row>
+    <row r="318" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="8" t="s">
         <v>1</v>
       </c>
@@ -13516,12 +13596,46 @@
       <c r="E318" s="28">
         <v>95.6</v>
       </c>
-      <c r="F318" s="16" t="e">
+      <c r="F318" s="19">
         <f t="shared" ref="F318:F322" si="14" xml:space="preserve"> AVERAGE(G318:P318)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="319" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>90.121999999999986</v>
+      </c>
+      <c r="G318">
+        <v>92.4</v>
+      </c>
+      <c r="H318">
+        <v>92.1</v>
+      </c>
+      <c r="I318">
+        <v>89.52</v>
+      </c>
+      <c r="J318">
+        <v>92.12</v>
+      </c>
+      <c r="K318">
+        <v>92.9</v>
+      </c>
+      <c r="L318">
+        <v>86.92</v>
+      </c>
+      <c r="M318">
+        <v>87</v>
+      </c>
+      <c r="N318">
+        <v>92.14</v>
+      </c>
+      <c r="O318">
+        <v>86.92</v>
+      </c>
+      <c r="P318">
+        <v>89.2</v>
+      </c>
+      <c r="T318">
+        <f t="shared" ref="T318:T372" si="15">(B318-F318)/B318 * 100</f>
+        <v>5.867975767704209</v>
+      </c>
+    </row>
+    <row r="319" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="8" t="s">
         <v>2</v>
       </c>
@@ -13531,18 +13645,56 @@
       <c r="C319" s="28">
         <v>35800</v>
       </c>
-      <c r="D319" s="17">
+      <c r="D319" s="48">
         <v>96.5</v>
       </c>
       <c r="E319" s="28">
         <v>96.8</v>
       </c>
-      <c r="F319" s="19" t="e">
+      <c r="F319" s="19">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="320" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102.14599999999989</v>
+      </c>
+      <c r="G319">
+        <v>102.55999999999899</v>
+      </c>
+      <c r="H319">
+        <v>101.7</v>
+      </c>
+      <c r="I319">
+        <v>102.42</v>
+      </c>
+      <c r="J319">
+        <v>101.7</v>
+      </c>
+      <c r="K319">
+        <v>101.7</v>
+      </c>
+      <c r="L319">
+        <v>102.42</v>
+      </c>
+      <c r="M319">
+        <v>102.42</v>
+      </c>
+      <c r="N319">
+        <v>101.7</v>
+      </c>
+      <c r="O319">
+        <v>102.42</v>
+      </c>
+      <c r="P319">
+        <v>102.42</v>
+      </c>
+      <c r="S319">
+        <f xml:space="preserve"> AVERAGEIF(T317:T372, "&lt;0")</f>
+        <v>-37.019977684935014</v>
+      </c>
+      <c r="T319">
+        <f t="shared" si="15"/>
+        <v>-4.8296387520524311</v>
+      </c>
+    </row>
+    <row r="320" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="8" t="s">
         <v>3</v>
       </c>
@@ -13558,12 +13710,46 @@
       <c r="E320" s="28">
         <v>94.6</v>
       </c>
-      <c r="F320" s="16" t="e">
+      <c r="F320" s="19">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="321" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92.835999999999984</v>
+      </c>
+      <c r="G320">
+        <v>91.86</v>
+      </c>
+      <c r="H320">
+        <v>92.82</v>
+      </c>
+      <c r="I320">
+        <v>91.66</v>
+      </c>
+      <c r="J320">
+        <v>90.56</v>
+      </c>
+      <c r="K320">
+        <v>96.32</v>
+      </c>
+      <c r="L320">
+        <v>91.66</v>
+      </c>
+      <c r="M320">
+        <v>93.78</v>
+      </c>
+      <c r="N320">
+        <v>93.78</v>
+      </c>
+      <c r="O320">
+        <v>93.78</v>
+      </c>
+      <c r="P320">
+        <v>92.14</v>
+      </c>
+      <c r="T320">
+        <f t="shared" si="15"/>
+        <v>9.634841603809404</v>
+      </c>
+    </row>
+    <row r="321" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="8" t="s">
         <v>4</v>
       </c>
@@ -13579,12 +13765,46 @@
       <c r="E321" s="28">
         <v>8000</v>
       </c>
-      <c r="F321" s="19" t="e">
+      <c r="F321" s="19">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="322" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5445.5180000000018</v>
+      </c>
+      <c r="G321">
+        <v>5448.62</v>
+      </c>
+      <c r="H321">
+        <v>5445.26</v>
+      </c>
+      <c r="I321">
+        <v>5445.26</v>
+      </c>
+      <c r="J321">
+        <v>5445.48</v>
+      </c>
+      <c r="K321">
+        <v>5445.26</v>
+      </c>
+      <c r="L321">
+        <v>5444.76</v>
+      </c>
+      <c r="M321">
+        <v>5445.26</v>
+      </c>
+      <c r="N321">
+        <v>5445.26</v>
+      </c>
+      <c r="O321">
+        <v>5444.76</v>
+      </c>
+      <c r="P321">
+        <v>5445.26</v>
+      </c>
+      <c r="T321">
+        <f t="shared" si="15"/>
+        <v>-33.808484713148843</v>
+      </c>
+    </row>
+    <row r="322" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="8" t="s">
         <v>5</v>
       </c>
@@ -13600,12 +13820,46 @@
       <c r="E322" s="19">
         <v>120</v>
       </c>
-      <c r="F322" s="19" t="e">
+      <c r="F322" s="19">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="323" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>115.36600000000001</v>
+      </c>
+      <c r="G322">
+        <v>108.96</v>
+      </c>
+      <c r="H322">
+        <v>117.72</v>
+      </c>
+      <c r="I322">
+        <v>118.58</v>
+      </c>
+      <c r="J322">
+        <v>116.72</v>
+      </c>
+      <c r="K322">
+        <v>114.98</v>
+      </c>
+      <c r="L322">
+        <v>118.24</v>
+      </c>
+      <c r="M322">
+        <v>118.58</v>
+      </c>
+      <c r="N322">
+        <v>108.96</v>
+      </c>
+      <c r="O322">
+        <v>115.46</v>
+      </c>
+      <c r="P322">
+        <v>115.46</v>
+      </c>
+      <c r="T322">
+        <f t="shared" si="15"/>
+        <v>-9.8723809523809649</v>
+      </c>
+    </row>
+    <row r="323" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="8" t="s">
         <v>6</v>
       </c>
@@ -13621,12 +13875,46 @@
       <c r="E323" s="19">
         <v>7200</v>
       </c>
-      <c r="F323" s="16" t="e">
+      <c r="F323" s="19">
         <f xml:space="preserve"> AVERAGE(G323:P323)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="324" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3941.4046666666663</v>
+      </c>
+      <c r="G323">
+        <v>3785.04</v>
+      </c>
+      <c r="H323">
+        <v>3984.62</v>
+      </c>
+      <c r="I323">
+        <v>3783.7</v>
+      </c>
+      <c r="J323">
+        <v>3984.96</v>
+      </c>
+      <c r="K323">
+        <v>3985.02</v>
+      </c>
+      <c r="L323">
+        <v>4385.72</v>
+      </c>
+      <c r="M323">
+        <v>3985.48</v>
+      </c>
+      <c r="N323">
+        <v>3783.9</v>
+      </c>
+      <c r="O323">
+        <v>3985.08</v>
+      </c>
+      <c r="P323">
+        <v>3750.5266666666598</v>
+      </c>
+      <c r="T323">
+        <f t="shared" si="15"/>
+        <v>61.87498222071136</v>
+      </c>
+    </row>
+    <row r="324" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="8" t="s">
         <v>7</v>
       </c>
@@ -13642,12 +13930,46 @@
       <c r="E324" s="19">
         <v>95</v>
       </c>
-      <c r="F324" s="16" t="e">
-        <f t="shared" ref="F324:F328" si="15" xml:space="preserve"> AVERAGE(G324:P324)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="325" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F324" s="19">
+        <f t="shared" ref="F324:F328" si="16" xml:space="preserve"> AVERAGE(G324:P324)</f>
+        <v>65.895999999999958</v>
+      </c>
+      <c r="G324">
+        <v>65.64</v>
+      </c>
+      <c r="H324">
+        <v>65.759999999999906</v>
+      </c>
+      <c r="I324">
+        <v>65.38</v>
+      </c>
+      <c r="J324">
+        <v>65.64</v>
+      </c>
+      <c r="K324">
+        <v>65.64</v>
+      </c>
+      <c r="L324">
+        <v>65.539999999999907</v>
+      </c>
+      <c r="M324">
+        <v>65.539999999999907</v>
+      </c>
+      <c r="N324">
+        <v>65.539999999999907</v>
+      </c>
+      <c r="O324">
+        <v>65.539999999999907</v>
+      </c>
+      <c r="P324">
+        <v>68.739999999999995</v>
+      </c>
+      <c r="T324">
+        <f t="shared" si="15"/>
+        <v>4.2209302325581959</v>
+      </c>
+    </row>
+    <row r="325" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="8" t="s">
         <v>8</v>
       </c>
@@ -13663,12 +13985,46 @@
       <c r="E325" s="19">
         <v>5000</v>
       </c>
-      <c r="F325" s="16" t="e">
+      <c r="F325" s="19">
+        <f t="shared" si="16"/>
+        <v>161.41399999999993</v>
+      </c>
+      <c r="G325">
+        <v>159.96</v>
+      </c>
+      <c r="H325">
+        <v>163.19999999999999</v>
+      </c>
+      <c r="I325">
+        <v>164.82</v>
+      </c>
+      <c r="J325">
+        <v>161.08000000000001</v>
+      </c>
+      <c r="K325">
+        <v>158.74</v>
+      </c>
+      <c r="L325">
+        <v>167.08</v>
+      </c>
+      <c r="M325">
+        <v>161</v>
+      </c>
+      <c r="N325">
+        <v>163.01999999999899</v>
+      </c>
+      <c r="O325">
+        <v>154.76</v>
+      </c>
+      <c r="P325">
+        <v>160.47999999999999</v>
+      </c>
+      <c r="T325">
         <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="326" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95.119229435092421</v>
+      </c>
+    </row>
+    <row r="326" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="8" t="s">
         <v>9</v>
       </c>
@@ -13684,7 +14040,7 @@
       <c r="E326" s="28">
         <v>183000</v>
       </c>
-      <c r="F326" s="16">
+      <c r="F326" s="19">
         <f xml:space="preserve"> AVERAGE(G326:P326)</f>
         <v>126363.84222222201</v>
       </c>
@@ -13718,8 +14074,13 @@
       <c r="P326">
         <v>117446.32</v>
       </c>
-    </row>
-    <row r="327" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S326" s="47"/>
+      <c r="T326">
+        <f t="shared" si="15"/>
+        <v>34.863998854524738</v>
+      </c>
+    </row>
+    <row r="327" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="8" t="s">
         <v>10</v>
       </c>
@@ -13735,8 +14096,8 @@
       <c r="E327" s="19">
         <v>500</v>
       </c>
-      <c r="F327" s="16">
-        <f t="shared" si="15"/>
+      <c r="F327" s="19">
+        <f t="shared" si="16"/>
         <v>178.80399999999992</v>
       </c>
       <c r="G327">
@@ -13769,8 +14130,13 @@
       <c r="P327">
         <v>184.68</v>
       </c>
-    </row>
-    <row r="328" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S327" s="47"/>
+      <c r="T327">
+        <f t="shared" si="15"/>
+        <v>80.367136687264278</v>
+      </c>
+    </row>
+    <row r="328" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="8" t="s">
         <v>11</v>
       </c>
@@ -13786,8 +14152,8 @@
       <c r="E328" s="19">
         <v>79000</v>
       </c>
-      <c r="F328" s="16">
-        <f t="shared" si="15"/>
+      <c r="F328" s="19">
+        <f t="shared" si="16"/>
         <v>29970.866984126915</v>
       </c>
       <c r="G328">
@@ -13811,8 +14177,13 @@
       <c r="P328">
         <v>12917.0777777777</v>
       </c>
-    </row>
-    <row r="329" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S328" s="47"/>
+      <c r="T328">
+        <f t="shared" si="15"/>
+        <v>-100.14409760587888</v>
+      </c>
+    </row>
+    <row r="329" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="8" t="s">
         <v>12</v>
       </c>
@@ -13828,7 +14199,7 @@
       <c r="E329" s="19">
         <v>1100</v>
       </c>
-      <c r="F329" s="16">
+      <c r="F329" s="19">
         <f xml:space="preserve"> AVERAGE(G329:P329)</f>
         <v>179.29999999999964</v>
       </c>
@@ -13850,8 +14221,13 @@
       <c r="P329">
         <v>191.099999999999</v>
       </c>
-    </row>
-    <row r="330" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S329" s="47"/>
+      <c r="T329">
+        <f t="shared" si="15"/>
+        <v>94.66315200728819</v>
+      </c>
+    </row>
+    <row r="330" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="8" t="s">
         <v>13</v>
       </c>
@@ -13867,8 +14243,8 @@
       <c r="E330" s="19">
         <v>6500</v>
       </c>
-      <c r="F330" s="16">
-        <f t="shared" ref="F330:F345" si="16" xml:space="preserve"> AVERAGE(G330:P330)</f>
+      <c r="F330" s="19">
+        <f t="shared" ref="F330:F345" si="17" xml:space="preserve"> AVERAGE(G330:P330)</f>
         <v>167.19749999999991</v>
       </c>
       <c r="G330">
@@ -13895,8 +14271,13 @@
       <c r="P330">
         <v>162.9</v>
       </c>
-    </row>
-    <row r="331" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S330" s="47"/>
+      <c r="T330">
+        <f t="shared" si="15"/>
+        <v>99.079474319299294</v>
+      </c>
+    </row>
+    <row r="331" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="32" t="s">
         <v>14</v>
       </c>
@@ -13912,8 +14293,8 @@
       <c r="E331" s="19">
         <v>47000</v>
       </c>
-      <c r="F331" s="16">
-        <f t="shared" si="16"/>
+      <c r="F331" s="19">
+        <f t="shared" si="17"/>
         <v>20242.6011111111</v>
       </c>
       <c r="H331">
@@ -13940,8 +14321,13 @@
       <c r="P331">
         <v>14339.493333333299</v>
       </c>
-    </row>
-    <row r="332" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S331" s="47"/>
+      <c r="T331">
+        <f t="shared" si="15"/>
+        <v>37.332000024868634</v>
+      </c>
+    </row>
+    <row r="332" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="8" t="s">
         <v>15</v>
       </c>
@@ -13957,8 +14343,8 @@
       <c r="E332" s="19">
         <v>49000</v>
       </c>
-      <c r="F332" s="16">
-        <f t="shared" si="16"/>
+      <c r="F332" s="19">
+        <f t="shared" si="17"/>
         <v>14527.631358024648</v>
       </c>
       <c r="G332">
@@ -13988,8 +14374,13 @@
       <c r="P332">
         <v>14768.208888888799</v>
       </c>
-    </row>
-    <row r="333" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S332" s="47"/>
+      <c r="T332">
+        <f t="shared" si="15"/>
+        <v>71.688412911356465</v>
+      </c>
+    </row>
+    <row r="333" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="32" t="s">
         <v>23</v>
       </c>
@@ -14005,8 +14396,8 @@
       <c r="E333" s="40">
         <v>92</v>
       </c>
-      <c r="F333" s="16">
-        <f t="shared" si="16"/>
+      <c r="F333" s="19">
+        <f t="shared" si="17"/>
         <v>83.656666666666666</v>
       </c>
       <c r="G333">
@@ -14036,8 +14427,13 @@
       <c r="O333">
         <v>83.58</v>
       </c>
-    </row>
-    <row r="334" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S333" s="47"/>
+      <c r="T333">
+        <f t="shared" si="15"/>
+        <v>1.1938858869499367</v>
+      </c>
+    </row>
+    <row r="334" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="8" t="s">
         <v>24</v>
       </c>
@@ -14053,8 +14449,8 @@
       <c r="E334" s="40">
         <v>96.42</v>
       </c>
-      <c r="F334" s="16">
-        <f t="shared" si="16"/>
+      <c r="F334" s="19">
+        <f t="shared" si="17"/>
         <v>87.089444444444439</v>
       </c>
       <c r="G334">
@@ -14084,8 +14480,13 @@
       <c r="O334">
         <v>87.11</v>
       </c>
-    </row>
-    <row r="335" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S334" s="47"/>
+      <c r="T334">
+        <f t="shared" si="15"/>
+        <v>94.650353009268144</v>
+      </c>
+    </row>
+    <row r="335" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="32" t="s">
         <v>25</v>
       </c>
@@ -14101,8 +14502,8 @@
       <c r="E335" s="40">
         <v>120</v>
       </c>
-      <c r="F335" s="16">
-        <f t="shared" si="16"/>
+      <c r="F335" s="19">
+        <f t="shared" si="17"/>
         <v>112.2491666666665</v>
       </c>
       <c r="G335">
@@ -14135,8 +14536,13 @@
       <c r="P335">
         <v>118.783333333333</v>
       </c>
-    </row>
-    <row r="336" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S335" s="47"/>
+      <c r="T335">
+        <f t="shared" si="15"/>
+        <v>91.091572045106616</v>
+      </c>
+    </row>
+    <row r="336" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="8" t="s">
         <v>26</v>
       </c>
@@ -14149,11 +14555,11 @@
       <c r="D336" s="40">
         <v>16200</v>
       </c>
-      <c r="E336" s="18">
+      <c r="E336" s="49">
         <v>100</v>
       </c>
       <c r="F336" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3406.6567777777723</v>
       </c>
       <c r="G336">
@@ -14186,8 +14592,13 @@
       <c r="P336">
         <v>3530.0211111111098</v>
       </c>
-    </row>
-    <row r="337" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S336" s="47"/>
+      <c r="T336">
+        <f t="shared" si="15"/>
+        <v>51.719074812665767</v>
+      </c>
+    </row>
+    <row r="337" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="32" t="s">
         <v>27</v>
       </c>
@@ -14203,8 +14614,8 @@
       <c r="E337" s="40">
         <v>110</v>
       </c>
-      <c r="F337" s="16">
-        <f t="shared" si="16"/>
+      <c r="F337" s="19">
+        <f t="shared" si="17"/>
         <v>104.08999999999988</v>
       </c>
       <c r="G337">
@@ -14231,8 +14642,13 @@
       <c r="N337">
         <v>106.36499999999999</v>
       </c>
-    </row>
-    <row r="338" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S337" s="47"/>
+      <c r="T337">
+        <f t="shared" si="15"/>
+        <v>95.656579899061725</v>
+      </c>
+    </row>
+    <row r="338" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="8" t="s">
         <v>28</v>
       </c>
@@ -14245,11 +14661,11 @@
       <c r="D338" s="40">
         <v>21100</v>
       </c>
-      <c r="E338" s="18">
+      <c r="E338" s="49">
         <v>96</v>
       </c>
       <c r="F338" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1641.5255555555534</v>
       </c>
       <c r="G338">
@@ -14270,8 +14686,13 @@
       <c r="M338">
         <v>1639.9622222222199</v>
       </c>
-    </row>
-    <row r="339" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S338" s="47"/>
+      <c r="T338">
+        <f t="shared" si="15"/>
+        <v>50.599182276840182</v>
+      </c>
+    </row>
+    <row r="339" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="32" t="s">
         <v>29</v>
       </c>
@@ -14287,8 +14708,8 @@
       <c r="E339" s="40">
         <v>105</v>
       </c>
-      <c r="F339" s="16">
-        <f t="shared" si="16"/>
+      <c r="F339" s="19">
+        <f t="shared" si="17"/>
         <v>104.4325</v>
       </c>
       <c r="G339">
@@ -14309,8 +14730,13 @@
       <c r="M339">
         <v>103.58499999999999</v>
       </c>
-    </row>
-    <row r="340" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S339" s="47"/>
+      <c r="T339">
+        <f t="shared" si="15"/>
+        <v>1.8814299807394161</v>
+      </c>
+    </row>
+    <row r="340" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="8" t="s">
         <v>30</v>
       </c>
@@ -14326,8 +14752,8 @@
       <c r="E340" s="40">
         <v>94.4</v>
       </c>
-      <c r="F340" s="16">
-        <f t="shared" si="16"/>
+      <c r="F340" s="19">
+        <f t="shared" si="17"/>
         <v>89.744</v>
       </c>
       <c r="G340">
@@ -14345,8 +14771,13 @@
       <c r="M340">
         <v>89.995000000000005</v>
       </c>
-    </row>
-    <row r="341" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S340" s="47"/>
+      <c r="T340">
+        <f t="shared" si="15"/>
+        <v>2.8281865823552286</v>
+      </c>
+    </row>
+    <row r="341" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="32" t="s">
         <v>31</v>
       </c>
@@ -14359,11 +14790,11 @@
       <c r="D341" s="40">
         <v>21500</v>
       </c>
-      <c r="E341" s="18">
+      <c r="E341" s="49">
         <v>6428</v>
       </c>
       <c r="F341" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9801.2519444444224</v>
       </c>
       <c r="G341">
@@ -14396,8 +14827,13 @@
       <c r="P341">
         <v>9621.4127777777703</v>
       </c>
-    </row>
-    <row r="342" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S341" s="47"/>
+      <c r="T341">
+        <f t="shared" si="15"/>
+        <v>4.8422141316075491</v>
+      </c>
+    </row>
+    <row r="342" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="8" t="s">
         <v>32</v>
       </c>
@@ -14413,8 +14849,8 @@
       <c r="E342" s="40">
         <v>9285</v>
       </c>
-      <c r="F342" s="16">
-        <f t="shared" si="16"/>
+      <c r="F342" s="19">
+        <f t="shared" si="17"/>
         <v>8534.9488333333156</v>
       </c>
       <c r="G342">
@@ -14447,8 +14883,13 @@
       <c r="P342">
         <v>10089.1688888888</v>
       </c>
-    </row>
-    <row r="343" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S342" s="47"/>
+      <c r="T342">
+        <f t="shared" si="15"/>
+        <v>19.930169520486686</v>
+      </c>
+    </row>
+    <row r="343" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="32" t="s">
         <v>33</v>
       </c>
@@ -14464,8 +14905,8 @@
       <c r="E343" s="40">
         <v>130</v>
       </c>
-      <c r="F343" s="16">
-        <f t="shared" si="16"/>
+      <c r="F343" s="19">
+        <f t="shared" si="17"/>
         <v>128.17699999999962</v>
       </c>
       <c r="G343">
@@ -14498,8 +14939,13 @@
       <c r="P343">
         <v>126.009999999999</v>
       </c>
-    </row>
-    <row r="344" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S343" s="47"/>
+      <c r="T343">
+        <f t="shared" si="15"/>
+        <v>4.3455223880599831</v>
+      </c>
+    </row>
+    <row r="344" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="8" t="s">
         <v>34</v>
       </c>
@@ -14512,11 +14958,11 @@
       <c r="D344" s="40">
         <v>14900</v>
       </c>
-      <c r="E344" s="18">
+      <c r="E344" s="49">
         <v>302</v>
       </c>
       <c r="F344" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7153.3489444444422</v>
       </c>
       <c r="G344">
@@ -14549,8 +14995,13 @@
       <c r="P344">
         <v>7130.0672222222202</v>
       </c>
-    </row>
-    <row r="345" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S344" s="47"/>
+      <c r="T344">
+        <f t="shared" si="15"/>
+        <v>-0.21921933773463975</v>
+      </c>
+    </row>
+    <row r="345" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="32" t="s">
         <v>35</v>
       </c>
@@ -14563,11 +15014,11 @@
       <c r="D345" s="40">
         <v>42400</v>
       </c>
-      <c r="E345" s="18">
+      <c r="E345" s="49">
         <v>925</v>
       </c>
       <c r="F345" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5492.8387037036982</v>
       </c>
       <c r="G345">
@@ -14597,8 +15048,13 @@
       <c r="P345">
         <v>5669.13055555555</v>
       </c>
-    </row>
-    <row r="346" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S345" s="47"/>
+      <c r="T345">
+        <f t="shared" si="15"/>
+        <v>39.270833121338519</v>
+      </c>
+    </row>
+    <row r="346" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="8" t="s">
         <v>36</v>
       </c>
@@ -14614,12 +15070,47 @@
       <c r="E346" s="40">
         <v>450</v>
       </c>
-      <c r="F346" s="16" t="e">
+      <c r="F346" s="19">
         <f xml:space="preserve"> AVERAGE(G346:O346)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="347" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>122.54555555555521</v>
+      </c>
+      <c r="G346">
+        <v>123.53</v>
+      </c>
+      <c r="H346">
+        <v>124.064999999999</v>
+      </c>
+      <c r="I346">
+        <v>114.235</v>
+      </c>
+      <c r="J346">
+        <v>125.83499999999999</v>
+      </c>
+      <c r="K346">
+        <v>121.354999999999</v>
+      </c>
+      <c r="L346">
+        <v>125.435</v>
+      </c>
+      <c r="M346">
+        <v>125.905</v>
+      </c>
+      <c r="N346">
+        <v>121.854999999999</v>
+      </c>
+      <c r="O346">
+        <v>120.69499999999999</v>
+      </c>
+      <c r="P346">
+        <v>124.36499999999999</v>
+      </c>
+      <c r="S346" s="47"/>
+      <c r="T346">
+        <f t="shared" si="15"/>
+        <v>-2.9794584500463959</v>
+      </c>
+    </row>
+    <row r="347" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="32" t="s">
         <v>37</v>
       </c>
@@ -14635,7 +15126,7 @@
       <c r="E347" s="40">
         <v>22000</v>
       </c>
-      <c r="F347" s="16">
+      <c r="F347" s="19">
         <f xml:space="preserve"> AVERAGE(G347:P347)</f>
         <v>15396.787866666651</v>
       </c>
@@ -14669,8 +15160,13 @@
       <c r="P347">
         <v>14579.608333333301</v>
       </c>
-    </row>
-    <row r="348" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S347" s="47"/>
+      <c r="T347">
+        <f t="shared" si="15"/>
+        <v>31.872620058997121</v>
+      </c>
+    </row>
+    <row r="348" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="8" t="s">
         <v>38</v>
       </c>
@@ -14683,11 +15179,11 @@
       <c r="D348" s="40">
         <v>19600</v>
       </c>
-      <c r="E348" s="18">
+      <c r="E348" s="49">
         <v>200</v>
       </c>
       <c r="F348" s="19">
-        <f t="shared" ref="F348:F367" si="17" xml:space="preserve"> AVERAGE(G348:P348)</f>
+        <f t="shared" ref="F348:F380" si="18" xml:space="preserve"> AVERAGE(G348:P348)</f>
         <v>6638.2183666666651</v>
       </c>
       <c r="G348">
@@ -14720,8 +15216,13 @@
       <c r="P348">
         <v>7856.51722222222</v>
       </c>
-    </row>
-    <row r="349" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S348" s="47"/>
+      <c r="T348">
+        <f t="shared" si="15"/>
+        <v>13.452172533681029</v>
+      </c>
+    </row>
+    <row r="349" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="32" t="s">
         <v>39</v>
       </c>
@@ -14737,12 +15238,40 @@
       <c r="E349" s="41">
         <v>1300</v>
       </c>
-      <c r="F349" s="16" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="350" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F349" s="19">
+        <f t="shared" si="18"/>
+        <v>77.451499999999967</v>
+      </c>
+      <c r="H349">
+        <v>78.085999999999999</v>
+      </c>
+      <c r="I349">
+        <v>77.305999999999898</v>
+      </c>
+      <c r="K349">
+        <v>76.557999999999893</v>
+      </c>
+      <c r="L349">
+        <v>78.149999999999906</v>
+      </c>
+      <c r="M349">
+        <v>74.786000000000001</v>
+      </c>
+      <c r="N349">
+        <v>77.683999999999997</v>
+      </c>
+      <c r="O349">
+        <v>79.736000000000004</v>
+      </c>
+      <c r="P349">
+        <v>77.305999999999997</v>
+      </c>
+      <c r="T349">
+        <f t="shared" si="15"/>
+        <v>97.887938351599573</v>
+      </c>
+    </row>
+    <row r="350" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="32" t="s">
         <v>40</v>
       </c>
@@ -14752,18 +15281,38 @@
       <c r="C350" s="11">
         <v>10500</v>
       </c>
-      <c r="D350" s="11">
+      <c r="D350" s="50">
         <v>54400</v>
       </c>
-      <c r="E350" s="18">
+      <c r="E350" s="49">
         <v>100</v>
       </c>
-      <c r="F350" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="351" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F350" s="19">
+        <f t="shared" si="18"/>
+        <v>9384.5324444444268</v>
+      </c>
+      <c r="G350">
+        <v>14760.273999999999</v>
+      </c>
+      <c r="H350">
+        <v>7656.4846666666599</v>
+      </c>
+      <c r="I350">
+        <v>10459.785777777701</v>
+      </c>
+      <c r="J350">
+        <v>7152.2606666666597</v>
+      </c>
+      <c r="K350">
+        <v>6893.8571111111096</v>
+      </c>
+      <c r="S350" s="47"/>
+      <c r="T350">
+        <f t="shared" si="15"/>
+        <v>15.827735221144346</v>
+      </c>
+    </row>
+    <row r="351" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="32" t="s">
         <v>41</v>
       </c>
@@ -14773,18 +15322,34 @@
       <c r="C351" s="11">
         <v>15800</v>
       </c>
-      <c r="D351" s="11">
+      <c r="D351" s="50">
         <v>104000</v>
       </c>
-      <c r="E351" s="18">
+      <c r="E351" s="49">
         <v>100</v>
       </c>
-      <c r="F351" s="19" t="e">
+      <c r="F351" s="19">
         <f xml:space="preserve"> AVERAGE(G351:P351)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="352" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2661.466499999995</v>
+      </c>
+      <c r="G351">
+        <v>3442.5415555555501</v>
+      </c>
+      <c r="H351">
+        <v>3676.5588888888801</v>
+      </c>
+      <c r="I351">
+        <v>84.286000000000001</v>
+      </c>
+      <c r="J351">
+        <v>3442.4795555555502</v>
+      </c>
+      <c r="T351">
+        <f t="shared" si="15"/>
+        <v>23.420959667253527</v>
+      </c>
+    </row>
+    <row r="352" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="32" t="s">
         <v>42</v>
       </c>
@@ -14794,18 +15359,49 @@
       <c r="C352" s="11">
         <v>23200</v>
       </c>
-      <c r="D352" s="11">
+      <c r="D352" s="50">
         <v>113000</v>
       </c>
-      <c r="E352" s="18">
+      <c r="E352" s="49">
         <v>900</v>
       </c>
-      <c r="F352" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="353" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F352" s="19">
+        <f t="shared" si="18"/>
+        <v>16790.943283950553</v>
+      </c>
+      <c r="G352">
+        <v>17306.832888888799</v>
+      </c>
+      <c r="H352">
+        <v>17885.744444444401</v>
+      </c>
+      <c r="I352">
+        <v>15875.531555555501</v>
+      </c>
+      <c r="J352">
+        <v>17620.1997777777</v>
+      </c>
+      <c r="K352">
+        <v>16536.782222222198</v>
+      </c>
+      <c r="L352">
+        <v>16322.1657777777</v>
+      </c>
+      <c r="M352">
+        <v>18322.851777777701</v>
+      </c>
+      <c r="N352">
+        <v>17788.512444444401</v>
+      </c>
+      <c r="O352">
+        <v>13459.8686666666</v>
+      </c>
+      <c r="T352">
+        <f t="shared" si="15"/>
+        <v>4.0517526631396947</v>
+      </c>
+    </row>
+    <row r="353" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="32" t="s">
         <v>43</v>
       </c>
@@ -14815,16 +15411,47 @@
       <c r="C353" s="11">
         <v>5140</v>
       </c>
-      <c r="D353" s="11">
+      <c r="D353" s="50">
         <v>95700</v>
       </c>
-      <c r="E353" s="11"/>
-      <c r="F353" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="354" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E353" s="50"/>
+      <c r="F353" s="19">
+        <f t="shared" si="18"/>
+        <v>11610.224172839464</v>
+      </c>
+      <c r="G353">
+        <v>11663.6895555555</v>
+      </c>
+      <c r="H353">
+        <v>12028.768222222199</v>
+      </c>
+      <c r="I353">
+        <v>11728.8342222222</v>
+      </c>
+      <c r="J353">
+        <v>12127.0682222222</v>
+      </c>
+      <c r="K353">
+        <v>11894.920888888801</v>
+      </c>
+      <c r="L353">
+        <v>11860.8155555555</v>
+      </c>
+      <c r="M353">
+        <v>8658.6317777777695</v>
+      </c>
+      <c r="N353">
+        <v>12161.541555555499</v>
+      </c>
+      <c r="O353">
+        <v>12367.747555555499</v>
+      </c>
+      <c r="T353">
+        <f t="shared" si="15"/>
+        <v>-3.6627158289237833</v>
+      </c>
+    </row>
+    <row r="354" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="32" t="s">
         <v>44</v>
       </c>
@@ -14834,17 +15461,47 @@
       <c r="C354" s="11">
         <v>30100</v>
       </c>
-      <c r="D354" s="11">
+      <c r="D354" s="50">
         <v>94200</v>
       </c>
-      <c r="E354" s="11"/>
-      <c r="F354" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I354" s="42"/>
-    </row>
-    <row r="355" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E354" s="50"/>
+      <c r="F354" s="19">
+        <f t="shared" si="18"/>
+        <v>14929.591925925888</v>
+      </c>
+      <c r="G354">
+        <v>10659.7813333333</v>
+      </c>
+      <c r="H354">
+        <v>17769.632222222201</v>
+      </c>
+      <c r="I354">
+        <v>14391.168666666599</v>
+      </c>
+      <c r="J354">
+        <v>18009.291111111099</v>
+      </c>
+      <c r="K354">
+        <v>17642.462444444402</v>
+      </c>
+      <c r="L354">
+        <v>12677.7297777777</v>
+      </c>
+      <c r="M354">
+        <v>10518.585999999999</v>
+      </c>
+      <c r="N354">
+        <v>18208.633111111099</v>
+      </c>
+      <c r="P354">
+        <v>14489.042666666601</v>
+      </c>
+      <c r="T354">
+        <f t="shared" si="15"/>
+        <v>9.5064842265873359</v>
+      </c>
+    </row>
+    <row r="355" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="32" t="s">
         <v>45</v>
       </c>
@@ -14854,16 +15511,50 @@
       <c r="C355" s="11">
         <v>22300</v>
       </c>
-      <c r="D355" s="11">
+      <c r="D355" s="50">
         <v>85200</v>
       </c>
-      <c r="E355" s="11"/>
-      <c r="F355" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="356" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E355" s="50"/>
+      <c r="F355" s="19">
+        <f t="shared" si="18"/>
+        <v>20397.098155555508</v>
+      </c>
+      <c r="G355">
+        <v>21316.276222222201</v>
+      </c>
+      <c r="H355">
+        <v>20913.134222222201</v>
+      </c>
+      <c r="I355">
+        <v>19314.250222222199</v>
+      </c>
+      <c r="J355">
+        <v>20347.8035555555</v>
+      </c>
+      <c r="K355">
+        <v>20078.940888888799</v>
+      </c>
+      <c r="L355">
+        <v>21013.5762222222</v>
+      </c>
+      <c r="M355">
+        <v>19878.608888888801</v>
+      </c>
+      <c r="N355">
+        <v>20649.173555555499</v>
+      </c>
+      <c r="O355">
+        <v>20346.905555555499</v>
+      </c>
+      <c r="P355">
+        <v>20112.312222222201</v>
+      </c>
+      <c r="T355">
+        <f t="shared" si="15"/>
+        <v>-0.59932781110065325</v>
+      </c>
+    </row>
+    <row r="356" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="32" t="s">
         <v>46</v>
       </c>
@@ -14873,16 +15564,50 @@
       <c r="C356" s="11">
         <v>24300</v>
       </c>
-      <c r="D356" s="11">
+      <c r="D356" s="50">
         <v>117000</v>
       </c>
-      <c r="E356" s="11"/>
-      <c r="F356" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="357" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E356" s="50"/>
+      <c r="F356" s="19">
+        <f t="shared" si="18"/>
+        <v>11284.419377777747</v>
+      </c>
+      <c r="G356">
+        <v>10809.4564444444</v>
+      </c>
+      <c r="H356">
+        <v>12377.8611111111</v>
+      </c>
+      <c r="I356">
+        <v>10336.3544444444</v>
+      </c>
+      <c r="J356">
+        <v>10403.9211111111</v>
+      </c>
+      <c r="K356">
+        <v>11277.855111111099</v>
+      </c>
+      <c r="L356">
+        <v>10035.7944444444</v>
+      </c>
+      <c r="M356">
+        <v>12978.0711111111</v>
+      </c>
+      <c r="N356">
+        <v>12110.040444444399</v>
+      </c>
+      <c r="O356">
+        <v>9770.1997777777706</v>
+      </c>
+      <c r="P356">
+        <v>12744.6397777777</v>
+      </c>
+      <c r="T356">
+        <f t="shared" si="15"/>
+        <v>16.068299147510999</v>
+      </c>
+    </row>
+    <row r="357" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="32" t="s">
         <v>47</v>
       </c>
@@ -14892,16 +15617,50 @@
       <c r="C357" s="11">
         <v>124000</v>
       </c>
-      <c r="D357" s="11">
+      <c r="D357" s="50">
         <v>549000</v>
       </c>
-      <c r="E357" s="11"/>
-      <c r="F357" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="358" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E357" s="50"/>
+      <c r="F357" s="19">
+        <f xml:space="preserve"> AVERAGE(G357:P357)</f>
+        <v>27701.970922222194</v>
+      </c>
+      <c r="G357">
+        <v>26780.771000000001</v>
+      </c>
+      <c r="H357">
+        <v>23664.81</v>
+      </c>
+      <c r="I357">
+        <v>32090.294888888799</v>
+      </c>
+      <c r="J357">
+        <v>30720.84</v>
+      </c>
+      <c r="K357">
+        <v>24679.715333333301</v>
+      </c>
+      <c r="L357">
+        <v>37662.388888888803</v>
+      </c>
+      <c r="M357">
+        <v>27775.013777777702</v>
+      </c>
+      <c r="N357">
+        <v>26030.331333333299</v>
+      </c>
+      <c r="O357">
+        <v>15666.51</v>
+      </c>
+      <c r="P357">
+        <v>31949.034</v>
+      </c>
+      <c r="T357">
+        <f t="shared" si="15"/>
+        <v>23.324885425872203</v>
+      </c>
+    </row>
+    <row r="358" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="32" t="s">
         <v>48</v>
       </c>
@@ -14911,16 +15670,41 @@
       <c r="C358" s="11">
         <v>164000</v>
       </c>
-      <c r="D358" s="11">
+      <c r="D358" s="50">
         <v>601000</v>
       </c>
-      <c r="E358" s="11"/>
-      <c r="F358" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="359" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E358" s="50"/>
+      <c r="F358" s="19">
+        <f t="shared" si="18"/>
+        <v>61828.87023809518</v>
+      </c>
+      <c r="G358">
+        <v>84592.184999999998</v>
+      </c>
+      <c r="H358">
+        <v>38534.606666666601</v>
+      </c>
+      <c r="I358">
+        <v>111057.24711111101</v>
+      </c>
+      <c r="J358">
+        <v>43415.330666666603</v>
+      </c>
+      <c r="K358">
+        <v>62520.374000000003</v>
+      </c>
+      <c r="M358">
+        <v>30857.894666666602</v>
+      </c>
+      <c r="O358">
+        <v>61824.453555555498</v>
+      </c>
+      <c r="T358">
+        <f t="shared" si="15"/>
+        <v>-16.878771716626048</v>
+      </c>
+    </row>
+    <row r="359" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="32" t="s">
         <v>49</v>
       </c>
@@ -14934,12 +15718,43 @@
         <v>551000</v>
       </c>
       <c r="E359" s="11"/>
-      <c r="F359" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="360" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F359" s="19">
+        <f t="shared" si="18"/>
+        <v>54085.943086419706</v>
+      </c>
+      <c r="G359">
+        <v>49345.990444444396</v>
+      </c>
+      <c r="H359">
+        <v>62544.972888888798</v>
+      </c>
+      <c r="I359">
+        <v>64906.4517777777</v>
+      </c>
+      <c r="J359">
+        <v>56334.583333333299</v>
+      </c>
+      <c r="K359">
+        <v>26420.588444444398</v>
+      </c>
+      <c r="L359">
+        <v>57456.157777777698</v>
+      </c>
+      <c r="M359">
+        <v>71501.408444444402</v>
+      </c>
+      <c r="O359">
+        <v>32938.880444444403</v>
+      </c>
+      <c r="P359">
+        <v>65324.454222222201</v>
+      </c>
+      <c r="T359">
+        <f t="shared" si="15"/>
+        <v>22.512975520888673</v>
+      </c>
+    </row>
+    <row r="360" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="32" t="s">
         <v>50</v>
       </c>
@@ -14953,12 +15768,46 @@
         <v>715000</v>
       </c>
       <c r="E360" s="11"/>
-      <c r="F360" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="361" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F360" s="19">
+        <f t="shared" si="18"/>
+        <v>72577.047933333291</v>
+      </c>
+      <c r="G360">
+        <v>88536.158888888895</v>
+      </c>
+      <c r="H360">
+        <v>96707.565555555499</v>
+      </c>
+      <c r="I360">
+        <v>96983.330888888799</v>
+      </c>
+      <c r="J360">
+        <v>93989.021111111098</v>
+      </c>
+      <c r="K360">
+        <v>46009.075111111102</v>
+      </c>
+      <c r="L360">
+        <v>70643.472666666596</v>
+      </c>
+      <c r="M360">
+        <v>57083.015111111097</v>
+      </c>
+      <c r="N360">
+        <v>50637.868888888799</v>
+      </c>
+      <c r="O360">
+        <v>76021.928</v>
+      </c>
+      <c r="P360">
+        <v>49159.043111111103</v>
+      </c>
+      <c r="T360">
+        <f t="shared" si="15"/>
+        <v>6.7133059982862582</v>
+      </c>
+    </row>
+    <row r="361" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="32" t="s">
         <v>51</v>
       </c>
@@ -14972,12 +15821,46 @@
         <v>616000</v>
       </c>
       <c r="E361" s="11"/>
-      <c r="F361" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="362" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F361" s="19">
+        <f t="shared" si="18"/>
+        <v>51128.447777777736</v>
+      </c>
+      <c r="G361">
+        <v>52126.895777777703</v>
+      </c>
+      <c r="H361">
+        <v>63505.829555555501</v>
+      </c>
+      <c r="I361">
+        <v>67471.556222222207</v>
+      </c>
+      <c r="J361">
+        <v>82594.246222222195</v>
+      </c>
+      <c r="K361">
+        <v>23595.475555555498</v>
+      </c>
+      <c r="L361">
+        <v>33666.490444444396</v>
+      </c>
+      <c r="M361">
+        <v>38751.469777777696</v>
+      </c>
+      <c r="N361">
+        <v>85527.080222222197</v>
+      </c>
+      <c r="O361">
+        <v>36561.4591111111</v>
+      </c>
+      <c r="P361">
+        <v>27483.974888888799</v>
+      </c>
+      <c r="T361">
+        <f t="shared" si="15"/>
+        <v>-7.9626451061980674</v>
+      </c>
+    </row>
+    <row r="362" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="32" t="s">
         <v>52</v>
       </c>
@@ -14991,12 +15874,46 @@
         <v>798000</v>
       </c>
       <c r="E362" s="11"/>
-      <c r="F362" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="363" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F362" s="19">
+        <f t="shared" si="18"/>
+        <v>29182.619511111065</v>
+      </c>
+      <c r="G362">
+        <v>40450.271999999997</v>
+      </c>
+      <c r="H362">
+        <v>33670.282888888803</v>
+      </c>
+      <c r="I362">
+        <v>48986.7515555555</v>
+      </c>
+      <c r="J362">
+        <v>12349.585555555501</v>
+      </c>
+      <c r="K362">
+        <v>14380.446</v>
+      </c>
+      <c r="L362">
+        <v>35630.823777777703</v>
+      </c>
+      <c r="M362">
+        <v>26975.835777777698</v>
+      </c>
+      <c r="N362">
+        <v>34032.753777777703</v>
+      </c>
+      <c r="O362">
+        <v>15526.5057777777</v>
+      </c>
+      <c r="P362">
+        <v>29822.937999999998</v>
+      </c>
+      <c r="T362">
+        <f t="shared" si="15"/>
+        <v>5.557865659834742</v>
+      </c>
+    </row>
+    <row r="363" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="32" t="s">
         <v>53</v>
       </c>
@@ -15010,12 +15927,37 @@
         <v>603000</v>
       </c>
       <c r="E363" s="11"/>
-      <c r="F363" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="364" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F363" s="19">
+        <f t="shared" si="18"/>
+        <v>23777.886031745998</v>
+      </c>
+      <c r="G363">
+        <v>20717.8797777777</v>
+      </c>
+      <c r="J363">
+        <v>26456.947111111102</v>
+      </c>
+      <c r="K363">
+        <v>23771.323777777699</v>
+      </c>
+      <c r="L363">
+        <v>24803.899111111099</v>
+      </c>
+      <c r="M363">
+        <v>21561.708444444401</v>
+      </c>
+      <c r="N363">
+        <v>25168.428</v>
+      </c>
+      <c r="O363">
+        <v>23965.016</v>
+      </c>
+      <c r="T363">
+        <f t="shared" si="15"/>
+        <v>11.276544657664186</v>
+      </c>
+    </row>
+    <row r="364" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="32" t="s">
         <v>54</v>
       </c>
@@ -15029,12 +15971,46 @@
         <v>549000</v>
       </c>
       <c r="E364" s="11"/>
-      <c r="F364" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="365" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F364" s="19">
+        <f t="shared" si="18"/>
+        <v>14741.358844444379</v>
+      </c>
+      <c r="G364">
+        <v>14789.1302222222</v>
+      </c>
+      <c r="H364">
+        <v>12223.298000000001</v>
+      </c>
+      <c r="I364">
+        <v>16368.502888888799</v>
+      </c>
+      <c r="J364">
+        <v>15564.984888888799</v>
+      </c>
+      <c r="K364">
+        <v>16269.564888888801</v>
+      </c>
+      <c r="L364">
+        <v>14686.4608888888</v>
+      </c>
+      <c r="M364">
+        <v>15567.932888888799</v>
+      </c>
+      <c r="N364">
+        <v>15645.6884444444</v>
+      </c>
+      <c r="O364">
+        <v>13137.128444444401</v>
+      </c>
+      <c r="P364">
+        <v>13160.896888888799</v>
+      </c>
+      <c r="T364">
+        <f t="shared" si="15"/>
+        <v>18.796702585161622</v>
+      </c>
+    </row>
+    <row r="365" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="32" t="s">
         <v>55</v>
       </c>
@@ -15048,12 +16024,35 @@
         <v>1590000</v>
       </c>
       <c r="E365" s="11"/>
-      <c r="F365" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="366" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F365" s="19">
+        <f t="shared" si="18"/>
+        <v>1647786.628022216</v>
+      </c>
+      <c r="G365">
+        <v>1607178.6651111101</v>
+      </c>
+      <c r="H365">
+        <v>1626496.75533333</v>
+      </c>
+      <c r="I365">
+        <v>1688804.2238888801</v>
+      </c>
+      <c r="M365">
+        <v>1618773.7398888799</v>
+      </c>
+      <c r="O365">
+        <v>1697679.75588888</v>
+      </c>
+      <c r="T365">
+        <f t="shared" si="15"/>
+        <v>-4.290292912798483</v>
+      </c>
+      <c r="U365">
+        <f>AVERAGE(T317:T365)</f>
+        <v>23.88677161094401</v>
+      </c>
+    </row>
+    <row r="366" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="32" t="s">
         <v>56</v>
       </c>
@@ -15067,17 +16066,48 @@
         <v>2510000</v>
       </c>
       <c r="E366" s="11"/>
-      <c r="F366" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="367" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F366" s="19">
+        <f t="shared" si="18"/>
+        <v>1645376.0278024632</v>
+      </c>
+      <c r="G366">
+        <v>1393942.1089999999</v>
+      </c>
+      <c r="H366">
+        <v>1508128.8288888801</v>
+      </c>
+      <c r="I366">
+        <v>1848780.1458888799</v>
+      </c>
+      <c r="J366">
+        <v>1826298.55511111</v>
+      </c>
+      <c r="K366">
+        <v>2337392.0737777702</v>
+      </c>
+      <c r="L366">
+        <v>1228936.14144444</v>
+      </c>
+      <c r="M366">
+        <v>1691812.3724444399</v>
+      </c>
+      <c r="N366">
+        <v>1619604.6058888801</v>
+      </c>
+      <c r="O366">
+        <v>1353489.41777777</v>
+      </c>
+      <c r="T366">
+        <f t="shared" si="15"/>
+        <v>-76.732118990597542</v>
+      </c>
+    </row>
+    <row r="367" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="32" t="s">
         <v>57</v>
       </c>
       <c r="B367" s="11">
-        <v>192540.7703</v>
+        <v>284264.25206666643</v>
       </c>
       <c r="C367" s="11">
         <v>515000</v>
@@ -15086,12 +16116,37 @@
         <v>1340000</v>
       </c>
       <c r="E367" s="11"/>
-      <c r="F367" s="19" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="368" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F367" s="19">
+        <f t="shared" si="18"/>
+        <v>282275.33488888864</v>
+      </c>
+      <c r="G367">
+        <v>160304.02577777699</v>
+      </c>
+      <c r="H367">
+        <v>315012.35800000001</v>
+      </c>
+      <c r="I367">
+        <v>97645.541444444403</v>
+      </c>
+      <c r="L367">
+        <v>347449.79800000001</v>
+      </c>
+      <c r="M367">
+        <v>487954.13400000002</v>
+      </c>
+      <c r="N367">
+        <v>343149.85244444403</v>
+      </c>
+      <c r="P367">
+        <v>224411.63455555501</v>
+      </c>
+      <c r="T367">
+        <f t="shared" si="15"/>
+        <v>0.69967192966330116</v>
+      </c>
+    </row>
+    <row r="368" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="32" t="s">
         <v>58</v>
       </c>
@@ -15105,14 +16160,42 @@
         <v>2030000</v>
       </c>
       <c r="E368" s="11"/>
-      <c r="F368" s="11"/>
-    </row>
-    <row r="369" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F368" s="19">
+        <f t="shared" si="18"/>
+        <v>1678848.8214126925</v>
+      </c>
+      <c r="H368">
+        <v>1439888.0758888801</v>
+      </c>
+      <c r="J368">
+        <v>1933759.1393333301</v>
+      </c>
+      <c r="K368">
+        <v>1553328.91777777</v>
+      </c>
+      <c r="M368">
+        <v>1741676.5737777699</v>
+      </c>
+      <c r="N368">
+        <v>1827879.4757777699</v>
+      </c>
+      <c r="O368">
+        <v>1803957.10633333</v>
+      </c>
+      <c r="P368">
+        <v>1451452.4609999999</v>
+      </c>
+      <c r="T368">
+        <f t="shared" si="15"/>
+        <v>-120.61088323425658</v>
+      </c>
+    </row>
+    <row r="369" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="32" t="s">
         <v>59</v>
       </c>
       <c r="B369" s="11">
-        <v>84700</v>
+        <v>133651.83300000001</v>
       </c>
       <c r="C369" s="11">
         <v>317000</v>
@@ -15121,9 +16204,31 @@
         <v>1930000</v>
       </c>
       <c r="E369" s="11"/>
-      <c r="F369" s="11"/>
-    </row>
-    <row r="370" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F369" s="19">
+        <f t="shared" si="18"/>
+        <v>322498.83302222163</v>
+      </c>
+      <c r="G369">
+        <v>255841.872888888</v>
+      </c>
+      <c r="J369">
+        <v>298939.383111111</v>
+      </c>
+      <c r="K369">
+        <v>122770.03644444401</v>
+      </c>
+      <c r="L369">
+        <v>469802.46077777701</v>
+      </c>
+      <c r="N369">
+        <v>465140.41188888799</v>
+      </c>
+      <c r="T369">
+        <f t="shared" si="15"/>
+        <v>-141.29772542829369</v>
+      </c>
+    </row>
+    <row r="370" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="32" t="s">
         <v>60</v>
       </c>
@@ -15137,9 +16242,34 @@
         <v>2000000</v>
       </c>
       <c r="E370" s="11"/>
-      <c r="F370" s="11"/>
-    </row>
-    <row r="371" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F370" s="19">
+        <f t="shared" si="18"/>
+        <v>1804622.6088148097</v>
+      </c>
+      <c r="G370">
+        <v>1815099.4246666599</v>
+      </c>
+      <c r="H370">
+        <v>1946421.86022222</v>
+      </c>
+      <c r="I370">
+        <v>1385581.56055555</v>
+      </c>
+      <c r="L370">
+        <v>2133996.6528888801</v>
+      </c>
+      <c r="N370">
+        <v>1847140.4761111101</v>
+      </c>
+      <c r="O370">
+        <v>1699495.67844444</v>
+      </c>
+      <c r="T370">
+        <f t="shared" si="15"/>
+        <v>12.820163825371511</v>
+      </c>
+    </row>
+    <row r="371" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="32" t="s">
         <v>61</v>
       </c>
@@ -15153,9 +16283,34 @@
         <v>1980000</v>
       </c>
       <c r="E371" s="11"/>
-      <c r="F371" s="11"/>
-    </row>
-    <row r="372" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F371" s="19">
+        <f t="shared" si="18"/>
+        <v>682032.61668518442</v>
+      </c>
+      <c r="H371">
+        <v>552598.32977777696</v>
+      </c>
+      <c r="I371">
+        <v>849716.89066666598</v>
+      </c>
+      <c r="J371">
+        <v>521680.27255555498</v>
+      </c>
+      <c r="K371">
+        <v>428657.62588888803</v>
+      </c>
+      <c r="N371">
+        <v>785691.62544444401</v>
+      </c>
+      <c r="O371">
+        <v>953850.95577777701</v>
+      </c>
+      <c r="T371">
+        <f t="shared" si="15"/>
+        <v>-31.411904433988219</v>
+      </c>
+    </row>
+    <row r="372" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="32" t="s">
         <v>62</v>
       </c>
@@ -15169,9 +16324,38 @@
         <v>2160000</v>
       </c>
       <c r="E372" s="11"/>
-      <c r="F372" s="11"/>
-    </row>
-    <row r="373" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F372" s="19">
+        <f t="shared" si="18"/>
+        <v>1849190.1731296249</v>
+      </c>
+      <c r="H372">
+        <v>1833272.3154444401</v>
+      </c>
+      <c r="K372">
+        <v>1741502.64544444</v>
+      </c>
+      <c r="L372">
+        <v>1703443.51411111</v>
+      </c>
+      <c r="M372">
+        <v>1936455.7325555501</v>
+      </c>
+      <c r="O372">
+        <v>1817372.9428888799</v>
+      </c>
+      <c r="P372">
+        <v>2063093.8883333299</v>
+      </c>
+      <c r="T372">
+        <f t="shared" si="15"/>
+        <v>11.096626291844956</v>
+      </c>
+      <c r="U372">
+        <f>AVERAGE(T324:T372)</f>
+        <v>16.192671041526324</v>
+      </c>
+    </row>
+    <row r="373" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="32" t="s">
         <v>63</v>
       </c>
@@ -15185,9 +16369,12 @@
         <v>16500000</v>
       </c>
       <c r="E373" s="11"/>
-      <c r="F373" s="11"/>
-    </row>
-    <row r="374" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F373" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="374" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="32" t="s">
         <v>64</v>
       </c>
@@ -15201,9 +16388,30 @@
         <v>11200000</v>
       </c>
       <c r="E374" s="11"/>
-      <c r="F374" s="11"/>
-    </row>
-    <row r="375" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F374" s="19">
+        <f t="shared" si="18"/>
+        <v>14642732.681777751</v>
+      </c>
+      <c r="G374">
+        <v>15591238.7764444</v>
+      </c>
+      <c r="H374">
+        <v>14424184.670111099</v>
+      </c>
+      <c r="I374">
+        <v>15591238.7764444</v>
+      </c>
+      <c r="J374">
+        <v>14138709.3093333</v>
+      </c>
+      <c r="K374">
+        <v>14375327.9471111</v>
+      </c>
+      <c r="L374">
+        <v>13735696.6112222</v>
+      </c>
+    </row>
+    <row r="375" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="32" t="s">
         <v>65</v>
       </c>
@@ -15217,9 +16425,24 @@
         <v>9540000</v>
       </c>
       <c r="E375" s="11"/>
-      <c r="F375" s="11"/>
-    </row>
-    <row r="376" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F375" s="19">
+        <f t="shared" si="18"/>
+        <v>13575862.100416625</v>
+      </c>
+      <c r="G375">
+        <v>13860455.2073333</v>
+      </c>
+      <c r="H375">
+        <v>11725526.4075555</v>
+      </c>
+      <c r="I375">
+        <v>13837810.975666599</v>
+      </c>
+      <c r="J375">
+        <v>14879655.8111111</v>
+      </c>
+    </row>
+    <row r="376" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="32" t="s">
         <v>66</v>
       </c>
@@ -15233,9 +16456,12 @@
         <v>13200000</v>
       </c>
       <c r="E376" s="11"/>
-      <c r="F376" s="11"/>
-    </row>
-    <row r="377" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F376" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="377" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="32" t="s">
         <v>67</v>
       </c>
@@ -15249,14 +16475,17 @@
         <v>7210000</v>
       </c>
       <c r="E377" s="11"/>
-      <c r="F377" s="11"/>
-    </row>
-    <row r="378" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F377" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="378" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="32" t="s">
         <v>68</v>
       </c>
       <c r="B378" s="11">
-        <v>8800000</v>
+        <v>11276982.050000001</v>
       </c>
       <c r="C378" s="11">
         <v>14500000</v>
@@ -15265,14 +16494,17 @@
         <v>10900000</v>
       </c>
       <c r="E378" s="11"/>
-      <c r="F378" s="11"/>
-    </row>
-    <row r="379" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F378" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="379" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="32" t="s">
         <v>69</v>
       </c>
       <c r="B379" s="11">
-        <v>13300000</v>
+        <v>17760068.359999999</v>
       </c>
       <c r="C379" s="11">
         <v>30900000</v>
@@ -15281,14 +16513,17 @@
         <v>25000000</v>
       </c>
       <c r="E379" s="11"/>
-      <c r="F379" s="11"/>
-    </row>
-    <row r="380" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F379" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="380" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B380" s="11">
-        <v>15700000</v>
+      <c r="B380">
+        <v>16764545.721333301</v>
       </c>
       <c r="C380" s="11">
         <v>25400000</v>
@@ -15297,12 +16532,15 @@
         <v>27400000</v>
       </c>
       <c r="E380" s="11"/>
-      <c r="F380" s="11"/>
-    </row>
-    <row r="381" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F380" s="19" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="381" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="385" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="27" t="s">
         <v>71</v>
@@ -15399,7 +16637,7 @@
         <v>95.6</v>
       </c>
       <c r="F387" s="19">
-        <f t="shared" ref="F387:F391" si="18" xml:space="preserve"> AVERAGE(G387:P387)</f>
+        <f t="shared" ref="F387:F391" si="19" xml:space="preserve"> AVERAGE(G387:P387)</f>
         <v>90.121999999999986</v>
       </c>
       <c r="G387">
@@ -15433,12 +16671,12 @@
         <v>89.2</v>
       </c>
       <c r="R387" s="11">
-        <f t="shared" ref="R387:R442" si="19" xml:space="preserve"> (F387 - B387)/B387</f>
-        <v>-5.8679757677042088E-2</v>
+        <f t="shared" ref="R387:R436" si="20" xml:space="preserve"> -(F387 - B387)/B387</f>
+        <v>5.8679757677042088E-2</v>
       </c>
       <c r="S387" s="19">
-        <f t="shared" ref="S387:S437" si="20" xml:space="preserve"> R387 * 100  * -1</f>
-        <v>5.867975767704209</v>
+        <f t="shared" ref="S387:S437" si="21" xml:space="preserve"> R387 * 100  * -1</f>
+        <v>-5.867975767704209</v>
       </c>
     </row>
     <row r="388" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15458,7 +16696,7 @@
         <v>96.8</v>
       </c>
       <c r="F388" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>102.14599999999989</v>
       </c>
       <c r="G388">
@@ -15492,12 +16730,12 @@
         <v>102.42</v>
       </c>
       <c r="R388" s="11">
-        <f t="shared" si="19"/>
-        <v>4.8296387520524314E-2</v>
+        <f t="shared" si="20"/>
+        <v>-4.8296387520524314E-2</v>
       </c>
       <c r="S388" s="19">
-        <f t="shared" si="20"/>
-        <v>-4.8296387520524311</v>
+        <f t="shared" si="21"/>
+        <v>4.8296387520524311</v>
       </c>
     </row>
     <row r="389" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15517,7 +16755,7 @@
         <v>94.6</v>
       </c>
       <c r="F389" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>92.835999999999984</v>
       </c>
       <c r="G389">
@@ -15551,12 +16789,12 @@
         <v>92.14</v>
       </c>
       <c r="R389" s="11">
-        <f t="shared" si="19"/>
-        <v>-9.6348416038094048E-2</v>
+        <f t="shared" si="20"/>
+        <v>9.6348416038094048E-2</v>
       </c>
       <c r="S389" s="19">
-        <f t="shared" si="20"/>
-        <v>9.634841603809404</v>
+        <f t="shared" si="21"/>
+        <v>-9.634841603809404</v>
       </c>
     </row>
     <row r="390" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15576,7 +16814,7 @@
         <v>8000</v>
       </c>
       <c r="F390" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5445.5180000000018</v>
       </c>
       <c r="G390">
@@ -15610,12 +16848,12 @@
         <v>5445.26</v>
       </c>
       <c r="R390" s="11">
-        <f t="shared" si="19"/>
-        <v>0.3380848471314884</v>
+        <f t="shared" si="20"/>
+        <v>-0.3380848471314884</v>
       </c>
       <c r="S390" s="19">
-        <f t="shared" si="20"/>
-        <v>-33.808484713148843</v>
+        <f t="shared" si="21"/>
+        <v>33.808484713148843</v>
       </c>
     </row>
     <row r="391" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15635,7 +16873,7 @@
         <v>120</v>
       </c>
       <c r="F391" s="19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>115.36600000000001</v>
       </c>
       <c r="G391">
@@ -15669,12 +16907,12 @@
         <v>115.46</v>
       </c>
       <c r="R391" s="11">
-        <f t="shared" si="19"/>
-        <v>9.8723809523809658E-2</v>
+        <f t="shared" si="20"/>
+        <v>-9.8723809523809658E-2</v>
       </c>
       <c r="S391" s="19">
-        <f t="shared" si="20"/>
-        <v>-9.8723809523809649</v>
+        <f t="shared" si="21"/>
+        <v>9.8723809523809649</v>
       </c>
     </row>
     <row r="392" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15728,12 +16966,12 @@
         <v>3750.5266666666598</v>
       </c>
       <c r="R392" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.61874982220711361</v>
+        <f t="shared" si="20"/>
+        <v>0.61874982220711361</v>
       </c>
       <c r="S392" s="19">
-        <f t="shared" si="20"/>
-        <v>61.87498222071136</v>
+        <f t="shared" si="21"/>
+        <v>-61.87498222071136</v>
       </c>
     </row>
     <row r="393" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15753,7 +16991,7 @@
         <v>95</v>
       </c>
       <c r="F393" s="19">
-        <f t="shared" ref="F393:F397" si="21" xml:space="preserve"> AVERAGE(G393:P393)</f>
+        <f t="shared" ref="F393:F397" si="22" xml:space="preserve"> AVERAGE(G393:P393)</f>
         <v>65.895999999999958</v>
       </c>
       <c r="G393">
@@ -15787,12 +17025,12 @@
         <v>68.739999999999995</v>
       </c>
       <c r="R393" s="11">
-        <f t="shared" si="19"/>
-        <v>-4.2209302325581961E-2</v>
+        <f t="shared" si="20"/>
+        <v>4.2209302325581961E-2</v>
       </c>
       <c r="S393" s="19">
-        <f t="shared" si="20"/>
-        <v>4.2209302325581959</v>
+        <f t="shared" si="21"/>
+        <v>-4.2209302325581959</v>
       </c>
     </row>
     <row r="394" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15812,7 +17050,7 @@
         <v>5000</v>
       </c>
       <c r="F394" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>161.41399999999993</v>
       </c>
       <c r="G394">
@@ -15846,12 +17084,12 @@
         <v>160.47999999999999</v>
       </c>
       <c r="R394" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.95119229435092423</v>
+        <f t="shared" si="20"/>
+        <v>0.95119229435092423</v>
       </c>
       <c r="S394" s="19">
-        <f t="shared" si="20"/>
-        <v>95.119229435092421</v>
+        <f t="shared" si="21"/>
+        <v>-95.119229435092421</v>
       </c>
     </row>
     <row r="395" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15871,7 +17109,7 @@
         <v>183000</v>
       </c>
       <c r="F395" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>142430.18866666619</v>
       </c>
       <c r="G395">
@@ -15905,12 +17143,12 @@
         <v>133916.80444444399</v>
       </c>
       <c r="R395" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.26582376975945265</v>
+        <f t="shared" si="20"/>
+        <v>0.26582376975945265</v>
       </c>
       <c r="S395" s="19">
-        <f t="shared" si="20"/>
-        <v>26.582376975945266</v>
+        <f t="shared" si="21"/>
+        <v>-26.582376975945266</v>
       </c>
     </row>
     <row r="396" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15930,7 +17168,7 @@
         <v>500</v>
       </c>
       <c r="F396" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>166.702</v>
       </c>
       <c r="G396">
@@ -15964,12 +17202,12 @@
         <v>164.14</v>
       </c>
       <c r="R396" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.81695948748575686</v>
+        <f t="shared" si="20"/>
+        <v>0.81695948748575686</v>
       </c>
       <c r="S396" s="19">
-        <f t="shared" si="20"/>
-        <v>81.695948748575688</v>
+        <f t="shared" si="21"/>
+        <v>-81.695948748575688</v>
       </c>
     </row>
     <row r="397" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15989,7 +17227,7 @@
         <v>79000</v>
       </c>
       <c r="F397" s="19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>23826.100444444404</v>
       </c>
       <c r="G397">
@@ -16023,12 +17261,12 @@
         <v>6693.4022222222202</v>
       </c>
       <c r="R397" s="11">
-        <f t="shared" si="19"/>
-        <v>0.591096238706046</v>
+        <f t="shared" si="20"/>
+        <v>-0.591096238706046</v>
       </c>
       <c r="S397" s="19">
-        <f t="shared" si="20"/>
-        <v>-59.109623870604601</v>
+        <f t="shared" si="21"/>
+        <v>59.109623870604601</v>
       </c>
     </row>
     <row r="398" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16082,12 +17320,12 @@
         <v>174.18</v>
       </c>
       <c r="R398" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.7805387036998408</v>
+        <f t="shared" si="20"/>
+        <v>0.7805387036998408</v>
       </c>
       <c r="S398" s="19">
-        <f t="shared" si="20"/>
-        <v>78.053870369984082</v>
+        <f t="shared" si="21"/>
+        <v>-78.053870369984082</v>
       </c>
     </row>
     <row r="399" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16107,7 +17345,7 @@
         <v>6500</v>
       </c>
       <c r="F399" s="19">
-        <f t="shared" ref="F399:F414" si="22" xml:space="preserve"> AVERAGE(G399:P399)</f>
+        <f t="shared" ref="F399:F414" si="23" xml:space="preserve"> AVERAGE(G399:P399)</f>
         <v>655.91456790123334</v>
       </c>
       <c r="G399">
@@ -16138,12 +17376,12 @@
         <v>164.88</v>
       </c>
       <c r="R399" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.96388784496784974</v>
+        <f t="shared" si="20"/>
+        <v>0.96388784496784974</v>
       </c>
       <c r="S399" s="19">
-        <f t="shared" si="20"/>
-        <v>96.388784496784979</v>
+        <f t="shared" si="21"/>
+        <v>-96.388784496784979</v>
       </c>
     </row>
     <row r="400" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16163,7 +17401,7 @@
         <v>47000</v>
       </c>
       <c r="F400" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>28053.94599999996</v>
       </c>
       <c r="G400">
@@ -16197,12 +17435,12 @@
         <v>22814.426666666601</v>
       </c>
       <c r="R400" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.13149269820599929</v>
+        <f t="shared" si="20"/>
+        <v>0.13149269820599929</v>
       </c>
       <c r="S400" s="19">
-        <f t="shared" si="20"/>
-        <v>13.14926982059993</v>
+        <f t="shared" si="21"/>
+        <v>-13.14926982059993</v>
       </c>
     </row>
     <row r="401" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16222,7 +17460,7 @@
         <v>49000</v>
       </c>
       <c r="F401" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>19360.027111111056</v>
       </c>
       <c r="G401">
@@ -16256,12 +17494,12 @@
         <v>17476.3644444444</v>
       </c>
       <c r="R401" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.62270993798864638</v>
+        <f t="shared" si="20"/>
+        <v>0.62270993798864638</v>
       </c>
       <c r="S401" s="19">
-        <f t="shared" si="20"/>
-        <v>62.270993798864637</v>
+        <f t="shared" si="21"/>
+        <v>-62.270993798864637</v>
       </c>
     </row>
     <row r="402" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16281,7 +17519,7 @@
         <v>92</v>
       </c>
       <c r="F402" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>80.656499999999994</v>
       </c>
       <c r="G402">
@@ -16315,12 +17553,12 @@
         <v>81.995000000000005</v>
       </c>
       <c r="R402" s="11">
-        <f t="shared" si="19"/>
-        <v>-4.737354947293837E-2</v>
+        <f t="shared" si="20"/>
+        <v>4.737354947293837E-2</v>
       </c>
       <c r="S402" s="19">
-        <f t="shared" si="20"/>
-        <v>4.737354947293837</v>
+        <f t="shared" si="21"/>
+        <v>-4.737354947293837</v>
       </c>
     </row>
     <row r="403" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16340,7 +17578,7 @@
         <v>96.42</v>
       </c>
       <c r="F403" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>85.755999999999986</v>
       </c>
       <c r="G403">
@@ -16374,12 +17612,12 @@
         <v>86.49</v>
       </c>
       <c r="R403" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.94732262557607039</v>
+        <f t="shared" si="20"/>
+        <v>0.94732262557607039</v>
       </c>
       <c r="S403" s="19">
-        <f t="shared" si="20"/>
-        <v>94.732262557607044</v>
+        <f t="shared" si="21"/>
+        <v>-94.732262557607044</v>
       </c>
     </row>
     <row r="404" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16399,7 +17637,7 @@
         <v>120</v>
       </c>
       <c r="F404" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>108.50283333333309</v>
       </c>
       <c r="G404">
@@ -16433,12 +17671,12 @@
         <v>109.675</v>
       </c>
       <c r="R404" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.91388892208686301</v>
+        <f t="shared" si="20"/>
+        <v>0.91388892208686301</v>
       </c>
       <c r="S404" s="19">
-        <f t="shared" si="20"/>
-        <v>91.3888922086863</v>
+        <f t="shared" si="21"/>
+        <v>-91.3888922086863</v>
       </c>
     </row>
     <row r="405" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16458,7 +17696,7 @@
         <v>100</v>
       </c>
       <c r="F405" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3385.2657777777722</v>
       </c>
       <c r="G405">
@@ -16492,12 +17730,12 @@
         <v>3297.2877777777699</v>
       </c>
       <c r="R405" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.52022239275085136</v>
+        <f t="shared" si="20"/>
+        <v>0.52022239275085136</v>
       </c>
       <c r="S405" s="19">
-        <f t="shared" si="20"/>
-        <v>52.022239275085134</v>
+        <f t="shared" si="21"/>
+        <v>-52.022239275085134</v>
       </c>
     </row>
     <row r="406" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16517,7 +17755,7 @@
         <v>110</v>
       </c>
       <c r="F406" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>104.54357142857144</v>
       </c>
       <c r="G406">
@@ -16542,12 +17780,12 @@
         <v>103.47</v>
       </c>
       <c r="R406" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.95637653477118501</v>
+        <f t="shared" si="20"/>
+        <v>0.95637653477118501</v>
       </c>
       <c r="S406" s="19">
-        <f t="shared" si="20"/>
-        <v>95.637653477118505</v>
+        <f t="shared" si="21"/>
+        <v>-95.637653477118505</v>
       </c>
     </row>
     <row r="407" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16567,7 +17805,7 @@
         <v>96</v>
       </c>
       <c r="F407" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1641.851111111109</v>
       </c>
       <c r="G407">
@@ -16598,12 +17836,12 @@
         <v>1640.6172222222201</v>
       </c>
       <c r="R407" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.50589384859672759</v>
+        <f t="shared" si="20"/>
+        <v>0.50589384859672759</v>
       </c>
       <c r="S407" s="19">
-        <f t="shared" si="20"/>
-        <v>50.589384859672762</v>
+        <f t="shared" si="21"/>
+        <v>-50.589384859672762</v>
       </c>
     </row>
     <row r="408" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16623,7 +17861,7 @@
         <v>105</v>
       </c>
       <c r="F408" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>104.70777777777744</v>
       </c>
       <c r="G408">
@@ -16654,12 +17892,12 @@
         <v>104.509999999999</v>
       </c>
       <c r="R408" s="11">
-        <f t="shared" si="19"/>
-        <v>-1.6227953419669892E-2</v>
+        <f t="shared" si="20"/>
+        <v>1.6227953419669892E-2</v>
       </c>
       <c r="S408" s="19">
-        <f t="shared" si="20"/>
-        <v>1.6227953419669892</v>
+        <f t="shared" si="21"/>
+        <v>-1.6227953419669892</v>
       </c>
     </row>
     <row r="409" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16679,7 +17917,7 @@
         <v>94.4</v>
       </c>
       <c r="F409" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>89.923999999999978</v>
       </c>
       <c r="G409">
@@ -16713,12 +17951,12 @@
         <v>88.864999999999995</v>
       </c>
       <c r="R409" s="11">
-        <f t="shared" si="19"/>
-        <v>-2.6332885789770197E-2</v>
+        <f t="shared" si="20"/>
+        <v>2.6332885789770197E-2</v>
       </c>
       <c r="S409" s="19">
-        <f t="shared" si="20"/>
-        <v>2.63328857897702</v>
+        <f t="shared" si="21"/>
+        <v>-2.63328857897702</v>
       </c>
     </row>
     <row r="410" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16738,7 +17976,7 @@
         <v>6428</v>
       </c>
       <c r="F410" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>8691.0338333333257</v>
       </c>
       <c r="G410">
@@ -16772,12 +18010,12 @@
         <v>7451.8594444444398</v>
       </c>
       <c r="R410" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.15621030744336645</v>
+        <f t="shared" si="20"/>
+        <v>0.15621030744336645</v>
       </c>
       <c r="S410" s="19">
-        <f t="shared" si="20"/>
-        <v>15.621030744336645</v>
+        <f t="shared" si="21"/>
+        <v>-15.621030744336645</v>
       </c>
     </row>
     <row r="411" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16797,7 +18035,7 @@
         <v>9285</v>
       </c>
       <c r="F411" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7385.2874074074025</v>
       </c>
       <c r="G411">
@@ -16828,12 +18066,12 @@
         <v>3980.29</v>
       </c>
       <c r="R411" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.30715611505002033</v>
+        <f t="shared" si="20"/>
+        <v>0.30715611505002033</v>
       </c>
       <c r="S411" s="19">
-        <f t="shared" si="20"/>
-        <v>30.715611505002034</v>
+        <f t="shared" si="21"/>
+        <v>-30.715611505002034</v>
       </c>
     </row>
     <row r="412" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16853,7 +18091,7 @@
         <v>130</v>
       </c>
       <c r="F412" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>127.37444444444444</v>
       </c>
       <c r="G412">
@@ -16884,12 +18122,12 @@
         <v>126.82</v>
       </c>
       <c r="R412" s="11">
-        <f t="shared" si="19"/>
-        <v>-4.9444444444444513E-2</v>
+        <f t="shared" si="20"/>
+        <v>4.9444444444444513E-2</v>
       </c>
       <c r="S412" s="19">
-        <f t="shared" si="20"/>
-        <v>4.9444444444444517</v>
+        <f t="shared" si="21"/>
+        <v>-4.9444444444444517</v>
       </c>
     </row>
     <row r="413" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16909,7 +18147,7 @@
         <v>302</v>
       </c>
       <c r="F413" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>7119.334388888883</v>
       </c>
       <c r="G413">
@@ -16943,12 +18181,12 @@
         <v>7138.5372222222204</v>
       </c>
       <c r="R413" s="11">
-        <f t="shared" si="19"/>
-        <v>-2.5732839261837608E-3</v>
+        <f t="shared" si="20"/>
+        <v>2.5732839261837608E-3</v>
       </c>
       <c r="S413" s="19">
-        <f t="shared" si="20"/>
-        <v>0.25732839261837609</v>
+        <f t="shared" si="21"/>
+        <v>-0.25732839261837609</v>
       </c>
     </row>
     <row r="414" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -16968,7 +18206,7 @@
         <v>925</v>
       </c>
       <c r="F414" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>6311.7867901234513</v>
       </c>
       <c r="G414">
@@ -16999,12 +18237,12 @@
         <v>6098.7288888888797</v>
       </c>
       <c r="R414" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.30216492062386413</v>
+        <f t="shared" si="20"/>
+        <v>0.30216492062386413</v>
       </c>
       <c r="S414" s="19">
-        <f t="shared" si="20"/>
-        <v>30.216492062386415</v>
+        <f t="shared" si="21"/>
+        <v>-30.216492062386415</v>
       </c>
     </row>
     <row r="415" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17058,12 +18296,12 @@
         <v>124.36499999999999</v>
       </c>
       <c r="R415" s="11">
-        <f t="shared" si="19"/>
-        <v>2.9794584500463957E-2</v>
+        <f t="shared" si="20"/>
+        <v>-2.9794584500463957E-2</v>
       </c>
       <c r="S415" s="19">
-        <f t="shared" si="20"/>
-        <v>-2.9794584500463959</v>
+        <f t="shared" si="21"/>
+        <v>2.9794584500463959</v>
       </c>
     </row>
     <row r="416" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17083,7 +18321,7 @@
         <v>22000</v>
       </c>
       <c r="F416" s="19">
-        <f t="shared" ref="F416:F436" si="23" xml:space="preserve"> AVERAGE(G416:P416)</f>
+        <f t="shared" ref="F416:F449" si="24" xml:space="preserve"> AVERAGE(G416:P416)</f>
         <v>16303.368541666627</v>
       </c>
       <c r="G416">
@@ -17111,12 +18349,12 @@
         <v>15879.9783333333</v>
       </c>
       <c r="R416" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.27861201143068026</v>
+        <f t="shared" si="20"/>
+        <v>0.27861201143068026</v>
       </c>
       <c r="S416" s="19">
-        <f t="shared" si="20"/>
-        <v>27.861201143068026</v>
+        <f t="shared" si="21"/>
+        <v>-27.861201143068026</v>
       </c>
     </row>
     <row r="417" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17136,7 +18374,7 @@
         <v>200</v>
       </c>
       <c r="F417" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>7489.0393888888839</v>
       </c>
       <c r="G417">
@@ -17170,12 +18408,12 @@
         <v>7531.5038888888803</v>
       </c>
       <c r="R417" s="11">
-        <f t="shared" si="19"/>
-        <v>-2.3593300014487107E-2</v>
+        <f t="shared" si="20"/>
+        <v>2.3593300014487107E-2</v>
       </c>
       <c r="S417" s="19">
-        <f t="shared" si="20"/>
-        <v>2.3593300014487109</v>
+        <f t="shared" si="21"/>
+        <v>-2.3593300014487109</v>
       </c>
     </row>
     <row r="418" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17195,7 +18433,7 @@
         <v>1300</v>
       </c>
       <c r="F418" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>77.451499999999967</v>
       </c>
       <c r="H418">
@@ -17223,12 +18461,12 @@
         <v>77.305999999999997</v>
       </c>
       <c r="R418" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.97887938351599568</v>
+        <f t="shared" si="20"/>
+        <v>0.97887938351599568</v>
       </c>
       <c r="S418" s="19">
-        <f t="shared" si="20"/>
-        <v>97.887938351599573</v>
+        <f t="shared" si="21"/>
+        <v>-97.887938351599573</v>
       </c>
     </row>
     <row r="419" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17248,7 +18486,7 @@
         <v>100</v>
       </c>
       <c r="F419" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>9384.5324444444268</v>
       </c>
       <c r="G419">
@@ -17267,12 +18505,12 @@
         <v>6893.8571111111096</v>
       </c>
       <c r="R419" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.15827735221144346</v>
+        <f t="shared" si="20"/>
+        <v>0.15827735221144346</v>
       </c>
       <c r="S419" s="19">
-        <f t="shared" si="20"/>
-        <v>15.827735221144346</v>
+        <f t="shared" si="21"/>
+        <v>-15.827735221144346</v>
       </c>
     </row>
     <row r="420" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17292,7 +18530,7 @@
         <v>100</v>
       </c>
       <c r="F420" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2661.466499999995</v>
       </c>
       <c r="G420">
@@ -17308,12 +18546,12 @@
         <v>3442.4795555555502</v>
       </c>
       <c r="R420" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.23420959667253527</v>
+        <f t="shared" si="20"/>
+        <v>0.23420959667253527</v>
       </c>
       <c r="S420" s="19">
-        <f t="shared" si="20"/>
-        <v>23.420959667253527</v>
+        <f t="shared" si="21"/>
+        <v>-23.420959667253527</v>
       </c>
     </row>
     <row r="421" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17333,7 +18571,7 @@
         <v>900</v>
       </c>
       <c r="F421" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>16790.943283950553</v>
       </c>
       <c r="G421">
@@ -17364,12 +18602,12 @@
         <v>13459.8686666666</v>
       </c>
       <c r="R421" s="11">
-        <f t="shared" si="19"/>
-        <v>-4.0517526631396947E-2</v>
+        <f t="shared" si="20"/>
+        <v>4.0517526631396947E-2</v>
       </c>
       <c r="S421" s="19">
-        <f t="shared" si="20"/>
-        <v>4.0517526631396947</v>
+        <f t="shared" si="21"/>
+        <v>-4.0517526631396947</v>
       </c>
     </row>
     <row r="422" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17387,7 +18625,7 @@
       </c>
       <c r="E422" s="45"/>
       <c r="F422" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>11610.224172839464</v>
       </c>
       <c r="G422">
@@ -17418,12 +18656,12 @@
         <v>12367.747555555499</v>
       </c>
       <c r="R422" s="11">
-        <f t="shared" si="19"/>
-        <v>3.6627158289237835E-2</v>
+        <f t="shared" si="20"/>
+        <v>-3.6627158289237835E-2</v>
       </c>
       <c r="S422" s="19">
-        <f t="shared" si="20"/>
-        <v>-3.6627158289237833</v>
+        <f t="shared" si="21"/>
+        <v>3.6627158289237833</v>
       </c>
     </row>
     <row r="423" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17441,7 +18679,7 @@
       </c>
       <c r="E423" s="45"/>
       <c r="F423" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>14929.591925925888</v>
       </c>
       <c r="G423">
@@ -17472,12 +18710,12 @@
         <v>14489.042666666601</v>
       </c>
       <c r="R423" s="11">
-        <f t="shared" si="19"/>
-        <v>-9.5064842265873362E-2</v>
+        <f t="shared" si="20"/>
+        <v>9.5064842265873362E-2</v>
       </c>
       <c r="S423" s="19">
-        <f t="shared" si="20"/>
-        <v>9.5064842265873359</v>
+        <f t="shared" si="21"/>
+        <v>-9.5064842265873359</v>
       </c>
     </row>
     <row r="424" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17495,7 +18733,7 @@
       </c>
       <c r="E424" s="45"/>
       <c r="F424" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>20397.098155555508</v>
       </c>
       <c r="G424">
@@ -17529,12 +18767,12 @@
         <v>20112.312222222201</v>
       </c>
       <c r="R424" s="11">
-        <f t="shared" si="19"/>
-        <v>5.9932781110065324E-3</v>
+        <f t="shared" si="20"/>
+        <v>-5.9932781110065324E-3</v>
       </c>
       <c r="S424" s="19">
-        <f t="shared" si="20"/>
-        <v>-0.59932781110065325</v>
+        <f t="shared" si="21"/>
+        <v>0.59932781110065325</v>
       </c>
     </row>
     <row r="425" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17552,7 +18790,7 @@
       </c>
       <c r="E425" s="45"/>
       <c r="F425" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>11284.419377777747</v>
       </c>
       <c r="G425">
@@ -17586,12 +18824,12 @@
         <v>12744.6397777777</v>
       </c>
       <c r="R425" s="11">
-        <f t="shared" si="19"/>
-        <v>-0.16068299147510998</v>
+        <f t="shared" si="20"/>
+        <v>0.16068299147510998</v>
       </c>
       <c r="S425" s="19">
-        <f t="shared" si="20"/>
-        <v>16.068299147510999</v>
+        <f t="shared" si="21"/>
+        <v>-16.068299147510999</v>
       </c>
     </row>
     <row r="426" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17609,7 +18847,7 @@
       </c>
       <c r="E426" s="45"/>
       <c r="F426" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>207022.75875555529</v>
       </c>
       <c r="G426">
@@ -17643,12 +18881,12 @@
         <v>158237.77155555499</v>
       </c>
       <c r="R426" s="11">
-        <f t="shared" si="19"/>
-        <v>4.7300954475772299</v>
+        <f t="shared" si="20"/>
+        <v>-4.7300954475772299</v>
       </c>
       <c r="S426" s="19">
-        <f t="shared" si="20"/>
-        <v>-473.00954475772301</v>
+        <f t="shared" si="21"/>
+        <v>473.00954475772301</v>
       </c>
     </row>
     <row r="427" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17666,7 +18904,7 @@
       </c>
       <c r="E427" s="45"/>
       <c r="F427" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>143218.90014444414</v>
       </c>
       <c r="G427">
@@ -17700,12 +18938,12 @@
         <v>181278.84977777701</v>
       </c>
       <c r="R427" s="11">
-        <f t="shared" si="19"/>
-        <v>1.7073516095358061</v>
+        <f t="shared" si="20"/>
+        <v>-1.7073516095358061</v>
       </c>
       <c r="S427" s="19">
-        <f t="shared" si="20"/>
-        <v>-170.73516095358062</v>
+        <f t="shared" si="21"/>
+        <v>170.73516095358062</v>
       </c>
     </row>
     <row r="428" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17723,7 +18961,7 @@
       </c>
       <c r="E428" s="45"/>
       <c r="F428" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>267055.65427777747</v>
       </c>
       <c r="G428">
@@ -17751,12 +18989,12 @@
         <v>356312.95799999998</v>
       </c>
       <c r="R428" s="11">
-        <f t="shared" si="19"/>
-        <v>2.8260122389366402</v>
+        <f t="shared" si="20"/>
+        <v>-2.8260122389366402</v>
       </c>
       <c r="S428" s="19">
-        <f t="shared" si="20"/>
-        <v>-282.60122389366404</v>
+        <f t="shared" si="21"/>
+        <v>282.60122389366404</v>
       </c>
     </row>
     <row r="429" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17774,7 +19012,7 @@
       </c>
       <c r="E429" s="45"/>
       <c r="F429" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>276897.77470000007</v>
       </c>
       <c r="G429">
@@ -17808,12 +19046,12 @@
         <v>95822.423999999999</v>
       </c>
       <c r="R429" s="11">
-        <f t="shared" si="19"/>
-        <v>2.5590973611825203</v>
+        <f t="shared" si="20"/>
+        <v>-2.5590973611825203</v>
       </c>
       <c r="S429" s="19">
-        <f t="shared" si="20"/>
-        <v>-255.90973611825203</v>
+        <f t="shared" si="21"/>
+        <v>255.90973611825203</v>
       </c>
     </row>
     <row r="430" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17831,7 +19069,7 @@
       </c>
       <c r="E430" s="45"/>
       <c r="F430" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>339636.52133333334</v>
       </c>
       <c r="G430">
@@ -17853,12 +19091,12 @@
         <v>812900.54799999995</v>
       </c>
       <c r="R430" s="11">
-        <f t="shared" si="19"/>
-        <v>6.1717524805733674</v>
+        <f t="shared" si="20"/>
+        <v>-6.1717524805733674</v>
       </c>
       <c r="S430" s="19">
-        <f t="shared" si="20"/>
-        <v>-617.17524805733672</v>
+        <f t="shared" si="21"/>
+        <v>617.17524805733672</v>
       </c>
     </row>
     <row r="431" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17876,7 +19114,7 @@
       </c>
       <c r="E431" s="45"/>
       <c r="F431" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>127134.93691358007</v>
       </c>
       <c r="G431">
@@ -17907,12 +19145,12 @@
         <v>96094.542222222197</v>
       </c>
       <c r="R431" s="11">
-        <f t="shared" si="19"/>
-        <v>3.1143992528666686</v>
+        <f t="shared" si="20"/>
+        <v>-3.1143992528666686</v>
       </c>
       <c r="S431" s="19">
-        <f t="shared" si="20"/>
-        <v>-311.43992528666683</v>
+        <f t="shared" si="21"/>
+        <v>311.43992528666683</v>
       </c>
     </row>
     <row r="432" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17930,7 +19168,7 @@
       </c>
       <c r="E432" s="45"/>
       <c r="F432" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>83958.0199333333</v>
       </c>
       <c r="G432">
@@ -17964,12 +19202,12 @@
         <v>47698.352444444397</v>
       </c>
       <c r="R432" s="11">
-        <f t="shared" si="19"/>
-        <v>2.1327619378109439</v>
+        <f t="shared" si="20"/>
+        <v>-2.1327619378109439</v>
       </c>
       <c r="S432" s="19">
-        <f t="shared" si="20"/>
-        <v>-213.27619378109438</v>
+        <f t="shared" si="21"/>
+        <v>213.27619378109438</v>
       </c>
     </row>
     <row r="433" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17987,7 +19225,7 @@
       </c>
       <c r="E433" s="45"/>
       <c r="F433" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>24510.86032222219</v>
       </c>
       <c r="G433">
@@ -18021,12 +19259,12 @@
         <v>24978.141111111101</v>
       </c>
       <c r="R433" s="11">
-        <f t="shared" si="19"/>
-        <v>0.35018942394790403</v>
+        <f t="shared" si="20"/>
+        <v>-0.35018942394790403</v>
       </c>
       <c r="S433" s="19">
-        <f t="shared" si="20"/>
-        <v>-35.0189423947904</v>
+        <f t="shared" si="21"/>
+        <v>35.0189423947904</v>
       </c>
     </row>
     <row r="434" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18044,15 +19282,15 @@
       </c>
       <c r="E434" s="45"/>
       <c r="F434" s="19" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R434" s="11" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S434" s="19" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -18071,15 +19309,15 @@
       </c>
       <c r="E435" s="45"/>
       <c r="F435" s="19" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R435" s="11" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S435" s="19" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -18088,7 +19326,7 @@
         <v>57</v>
       </c>
       <c r="B436" s="11">
-        <v>192540.7703</v>
+        <v>284264.25206666643</v>
       </c>
       <c r="C436" s="45">
         <v>515000</v>
@@ -18098,15 +19336,15 @@
       </c>
       <c r="E436" s="45"/>
       <c r="F436" s="19" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R436" s="11" t="e">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S436" s="19" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -18124,14 +19362,44 @@
         <v>2030000</v>
       </c>
       <c r="E437" s="45"/>
-      <c r="F437" s="45"/>
+      <c r="F437" s="19">
+        <f t="shared" si="24"/>
+        <v>1811440.7584938232</v>
+      </c>
+      <c r="G437">
+        <v>1867336.28633333</v>
+      </c>
+      <c r="H437">
+        <v>2055900.5162222199</v>
+      </c>
+      <c r="I437">
+        <v>1436658.6395555499</v>
+      </c>
+      <c r="J437">
+        <v>2046035.29811111</v>
+      </c>
+      <c r="K437">
+        <v>2059527.2837777699</v>
+      </c>
+      <c r="L437">
+        <v>1731211.46311111</v>
+      </c>
+      <c r="M437">
+        <v>1727443.9286666601</v>
+      </c>
+      <c r="N437">
+        <v>1822427.145</v>
+      </c>
+      <c r="O437">
+        <v>1556426.2656666599</v>
+      </c>
       <c r="R437" s="11">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+        <f xml:space="preserve"> -(F437 - B437)/B437</f>
+        <v>-1.3803426524228952</v>
       </c>
       <c r="S437" s="19">
-        <f t="shared" si="20"/>
-        <v>100</v>
+        <f t="shared" si="21"/>
+        <v>138.03426524228954</v>
       </c>
     </row>
     <row r="438" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18139,7 +19407,7 @@
         <v>59</v>
       </c>
       <c r="B438" s="11">
-        <v>84700</v>
+        <v>133651.83300000001</v>
       </c>
       <c r="C438" s="45">
         <v>317000</v>
@@ -18148,10 +19416,43 @@
         <v>1930000</v>
       </c>
       <c r="E438" s="45"/>
-      <c r="F438" s="45"/>
+      <c r="F438" s="19">
+        <f xml:space="preserve"> AVERAGE(G438:P438)</f>
+        <v>492591.50106666621</v>
+      </c>
+      <c r="G438">
+        <v>644148.34722222202</v>
+      </c>
+      <c r="H438">
+        <v>711755.85077777703</v>
+      </c>
+      <c r="I438">
+        <v>432994.44566666603</v>
+      </c>
+      <c r="J438">
+        <v>346191.74366666598</v>
+      </c>
+      <c r="K438">
+        <v>293213.13288888801</v>
+      </c>
+      <c r="L438">
+        <v>514783.272</v>
+      </c>
+      <c r="M438">
+        <v>787725.22122222197</v>
+      </c>
+      <c r="N438">
+        <v>532723.72944444395</v>
+      </c>
+      <c r="O438">
+        <v>382755.04655555502</v>
+      </c>
+      <c r="P438">
+        <v>279624.22122222203</v>
+      </c>
       <c r="R438" s="11">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+        <f xml:space="preserve"> -(F438 - B438)/B438</f>
+        <v>-2.6856322132646411</v>
       </c>
       <c r="S438" s="45"/>
     </row>
@@ -18169,10 +19470,31 @@
         <v>2000000</v>
       </c>
       <c r="E439" s="11"/>
-      <c r="F439" s="11"/>
+      <c r="F439" s="19">
+        <f t="shared" si="24"/>
+        <v>1912805.2779259218</v>
+      </c>
+      <c r="G439">
+        <v>2152576.8816666598</v>
+      </c>
+      <c r="H439">
+        <v>1413713.76888888</v>
+      </c>
+      <c r="I439">
+        <v>1932231.0179999999</v>
+      </c>
+      <c r="J439">
+        <v>1268785.4711111099</v>
+      </c>
+      <c r="K439">
+        <v>2210423.0536666601</v>
+      </c>
+      <c r="L439">
+        <v>2499101.47422222</v>
+      </c>
       <c r="R439" s="11">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+        <f t="shared" ref="R439" si="25" xml:space="preserve"> -(F439 - B439)/B439</f>
+        <v>7.5939479262839699E-2</v>
       </c>
       <c r="S439" s="11"/>
     </row>
@@ -18190,10 +19512,13 @@
         <v>1980000</v>
       </c>
       <c r="E440" s="11"/>
-      <c r="F440" s="11"/>
-      <c r="R440" s="11">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+      <c r="F440" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R440" s="11" t="e">
+        <f t="shared" ref="R440:R442" si="26" xml:space="preserve"> (F440 - B440)/B440</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="S440" s="11"/>
     </row>
@@ -18211,10 +19536,13 @@
         <v>2160000</v>
       </c>
       <c r="E441" s="11"/>
-      <c r="F441" s="11"/>
-      <c r="R441" s="11">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+      <c r="F441" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R441" s="11" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="S441" s="11"/>
     </row>
@@ -18232,10 +19560,13 @@
         <v>16500000</v>
       </c>
       <c r="E442" s="11"/>
-      <c r="F442" s="11"/>
-      <c r="R442" s="11">
-        <f t="shared" si="19"/>
-        <v>-1</v>
+      <c r="F442" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R442" s="11" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="443" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18252,7 +19583,10 @@
         <v>11200000</v>
       </c>
       <c r="E443" s="11"/>
-      <c r="F443" s="11"/>
+      <c r="F443" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="R443" s="11"/>
     </row>
     <row r="444" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18269,7 +19603,10 @@
         <v>9540000</v>
       </c>
       <c r="E444" s="11"/>
-      <c r="F444" s="11"/>
+      <c r="F444" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="R444" s="11"/>
     </row>
     <row r="445" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18286,7 +19623,10 @@
         <v>13200000</v>
       </c>
       <c r="E445" s="11"/>
-      <c r="F445" s="11"/>
+      <c r="F445" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="446" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="32" t="s">
@@ -18302,10 +19642,13 @@
         <v>7210000</v>
       </c>
       <c r="E446" s="11"/>
-      <c r="F446" s="11"/>
+      <c r="F446" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="S446" s="47">
         <f xml:space="preserve"> AVERAGE(S386:S425)</f>
-        <v>27.37018786489719</v>
+        <v>-27.234814730568825</v>
       </c>
     </row>
     <row r="447" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18313,7 +19656,7 @@
         <v>68</v>
       </c>
       <c r="B447" s="11">
-        <v>8800000</v>
+        <v>11276982.050000001</v>
       </c>
       <c r="C447" s="11">
         <v>14500000</v>
@@ -18322,14 +19665,17 @@
         <v>10900000</v>
       </c>
       <c r="E447" s="11"/>
-      <c r="F447" s="11"/>
+      <c r="F447" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="448" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A448" s="32" t="s">
         <v>69</v>
       </c>
       <c r="B448" s="11">
-        <v>13300000</v>
+        <v>17760068.359999999</v>
       </c>
       <c r="C448" s="11">
         <v>30900000</v>
@@ -18338,14 +19684,17 @@
         <v>25000000</v>
       </c>
       <c r="E448" s="11"/>
-      <c r="F448" s="11"/>
+      <c r="F448" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="449" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B449" s="11">
-        <v>15700000</v>
+      <c r="B449">
+        <v>16764545.721333301</v>
       </c>
       <c r="C449" s="11">
         <v>25400000</v>
@@ -18354,7 +19703,10 @@
         <v>27400000</v>
       </c>
       <c r="E449" s="11"/>
-      <c r="F449" s="11"/>
+      <c r="F449" s="19" t="e">
+        <f t="shared" si="24"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="450" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="451" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18888,8 +20240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911A5E9-8C1D-4937-B2E8-4FEF8E2ACD16}">
   <dimension ref="A1:AA148"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22019,10 +23371,8 @@
         <v>1340000</v>
       </c>
       <c r="E52" s="11">
-        <v>192540.7703</v>
-      </c>
-      <c r="F52">
-        <v>87989.332888888894</v>
+        <f>AVERAGE(F52:O52)</f>
+        <v>284264.25206666643</v>
       </c>
       <c r="G52">
         <v>429572.52122222201</v>
@@ -22038,18 +23388,6 @@
       </c>
       <c r="K52">
         <v>57604.905333333299</v>
-      </c>
-      <c r="L52">
-        <v>172884.67811111099</v>
-      </c>
-      <c r="M52">
-        <v>68721.888999999996</v>
-      </c>
-      <c r="N52">
-        <v>103490.877666666</v>
-      </c>
-      <c r="O52">
-        <v>70999.664777777696</v>
       </c>
       <c r="Q52" s="15" t="s">
         <v>57</v>
@@ -22102,9 +23440,6 @@
       <c r="K53">
         <v>631545.147</v>
       </c>
-      <c r="L53">
-        <v>395637.75866666599</v>
-      </c>
       <c r="Q53" s="15" t="s">
         <v>58</v>
       </c>
@@ -22136,19 +23471,19 @@
         <v>1930000</v>
       </c>
       <c r="E54" s="11">
-        <v>84700</v>
+        <v>133651.83300000001</v>
       </c>
       <c r="F54">
-        <v>25097.7303333333</v>
+        <v>126422.70477777701</v>
       </c>
       <c r="G54">
         <v>93008.541666666599</v>
       </c>
       <c r="H54">
-        <v>28183.440444444401</v>
+        <v>150763.67644444399</v>
       </c>
       <c r="I54">
-        <v>84033.493666666604</v>
+        <v>108866.961</v>
       </c>
       <c r="J54">
         <v>107524.908555555</v>
@@ -22157,7 +23492,7 @@
         <v>58437.360444444399</v>
       </c>
       <c r="L54">
-        <v>70514.322444444406</v>
+        <v>359275.792555555</v>
       </c>
       <c r="M54">
         <v>167258.269888888</v>
@@ -22685,7 +24020,7 @@
         <v>10900000</v>
       </c>
       <c r="E63" s="11">
-        <v>8800000</v>
+        <v>11276982.050000001</v>
       </c>
       <c r="F63">
         <v>12201472.7873333</v>
@@ -22748,7 +24083,22 @@
         <v>25000000</v>
       </c>
       <c r="E64" s="11">
-        <v>13300000</v>
+        <v>17760068.359999999</v>
+      </c>
+      <c r="F64">
+        <v>17568492.154777698</v>
+      </c>
+      <c r="G64">
+        <v>17870685.9532222</v>
+      </c>
+      <c r="H64">
+        <v>16909475.487111099</v>
+      </c>
+      <c r="I64">
+        <v>19346525.833888799</v>
+      </c>
+      <c r="J64">
+        <v>17105162.3722222</v>
       </c>
       <c r="Q64" s="15" t="s">
         <v>69</v>
@@ -22780,8 +24130,14 @@
       <c r="D65" s="11">
         <v>27400000</v>
       </c>
-      <c r="E65" s="11">
-        <v>15700000</v>
+      <c r="E65">
+        <v>16764545.721333301</v>
+      </c>
+      <c r="F65">
+        <v>13024442.7263333</v>
+      </c>
+      <c r="G65">
+        <v>16764545.721333301</v>
       </c>
       <c r="Q65" s="15" t="s">
         <v>70</v>

</xml_diff>